<commit_message>
Breaking BFPerry Transcribed letters into smaller files by year. Creating NER script and .txt for results.
</commit_message>
<xml_diff>
--- a/Elizabeth_Perry_Letters_Dataset.xlsx
+++ b/Elizabeth_Perry_Letters_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crboatwright/PerryLetters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F6BD71-0C47-734E-A5D1-CCE6D73CFAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE1C33B-791F-7342-969C-07CCD3147A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="760" windowWidth="27260" windowHeight="17440" xr2:uid="{C5676EFD-15AF-AA40-AEBC-1ABB6CC12875}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="824">
   <si>
     <t>LetterID</t>
   </si>
@@ -2094,6 +2094,420 @@
   </si>
   <si>
     <t> I have received no letter from you today.  Nothing has come from the Post office today.  So I will write you only a few lines.  I am disappointed at not hearing, but hope you were too busy to write, that you are quite well.  Mr. Hoke today is to buy the Hogs.  There is a fine drove in the village, &amp; he says not many more fine ones will come.  You must write now whether the carri[a]ge must be sent for you, or whether you will come in the Stage.  If it were not for bad roads, the carri]a]ge would be the pleasantest, but you will know best.  I hope to hear tomorrow.  I am very busy working.  All are well except Charles who in bad weather has Asthma.  The weather is still bad, cloudy &amp; drizzly.  I have no news to tell you.  I write so often I have not missed a single Mail. I wrote to Anna yesterday, &amp; will again tomorrow.  We get along quite well, &amp; am glad you are at a pleasant Hotel. The Legislature adjourns too soon to get through with the business.  You ought to postpone it, so as to pass all your important bills.  A few days longer, so much could be done.  Those who are in such a hurry should stay at home. I hope we will have good weather so as to clean the house before you return.  I must now conclude.  I think of you constantly. </t>
+  </si>
+  <si>
+    <t>EMP248_11_12_1852</t>
+  </si>
+  <si>
+    <t> I received a letter about an hour ago from you.  A Servant brought it to the door &amp; said, “Mr. Jones sends his respects, &amp; sends you this letter.”  I took it &amp; said nothing.  I knew he had not brought it from you that someone else had brought it, &amp; begged him perhaps to send it to me.  In your letter you say Dr. Pasley will bring it.  I did not hear from you yesterday, nor today.  I mean this morning, no Mail it was said came from beyond Newberry, so I was glad to get the letter this evening.  I wish you had enclosed Anna’s to me.  She writes such short letters.  I would like to see all she writes to you.  Not being accustomed to writing, she finds it difficult to express herself &amp; tell all I wish to hear, but what she does write, she writes well.  Aunt Eliza’s letter was very satisfactory, &amp; she is fastidious &amp; particular. &amp; expects a good deal even from children.  So approbation from her is worth something.  This has been a fine day.  It is getting cold, &amp; by Monday I hope will be good weather to kill hogs.  Mr. Hoke yesterday bought 10 for you weighing 2306 pounds, some of them about 200 weight, &amp; some a good deal more, but on an average 230 pounds.  All say it is the cheapest way of getting meat, &amp; everybody seems to have bought.  Mr. Lasly came today to offer to help kill.  He &amp; his sons, &amp; offered his daughter to help clean &amp; attend to stuffing Sausages, so we will get assistance from him.  He says he will be here Monday at daylight.  We are out of lard so I am very glad to have some soon.  Lard is selling 15 cts a pd. Charles has been suffering with Asthma, but is getting better &amp; expects to be well Monday.  I told Becky to attend to him.  She said, “it was her duty to attend to Charles, for he was a good old man.”  So this shows her to be better disposed than some of our other servants.  The servants all seem happy now, &amp; they respect Becky. &amp; do not quarrel &amp; abuse each other as they did.  Even Lindy’s child is beginning to thrive.  There is no complaint of not having enough to eat.  I dare say in consequence, that the eating will cost a great deal more than heretofore, but I know you will not object.  Susan this week spent several days &amp; nights with me.  It was quite unexpected.  She came in to pass the day, &amp; I felt so sorry for her, &amp; knew it would be a relief to Ann to have her away, that I told her to stay for the night.  She, Annie, &amp; Susy, so she staid three or four nights, &amp; went back to Mamma’s this morning to see Vardry &amp; Alex.  Mamma &amp; Ann have dined with me three days so I have not been lonely this week.  I feel so sorry for Susan.  She has had a hard fate.  She is sensitive &amp; ill fitted to endure the trials she had.  If she had been differently constituted perhaps she might, but as it is, I know of no one more to be pitied.  She said she enjoyed being with me, that I had everything to make me happy, that if it were not sinful, one might almost be envious of me.  When I think that it was just something in my person &amp; manners that struck an old Bachelors fancy, I realize how accidental our fates in life are. Susan has helped me a great deal in my work.  I have been trying to make the house look more comfortable, particularly the two rooms where we sit for the winter.  I have had them whitewashed &amp; new curtains put up.  The Sofa Mr. Wardell has finished looks very comfortable.  It will suit you exactly to lounge on these winter evenings.  The new Carpet on the Staircase &amp; Entry looks very pretty.  These improvements were so unexpected.  My money has not held out, but as Minerva’s wages this year I have spent for you.  I know you will not begrudge returning as much of that money as I need.  Another year Minerva’s wages will appropriate expressly for my clothes &amp; to buy things for the house I wish, &amp; you do not care for.  This year I have spent it for every purpose but myself.  In Jan[uar]y you will receive Bank Interest which will help you to pay your debts.  Mr. Arthur came to see me yesterday.  He inquired after you.  He says he went down on the R[ail] Road with Col. Dawkins last summer I think, &amp; he was drunk the whole time.  His bold, vain aspiring Northern Wife I dare say has made him miserable.  She does not love him for himself, &amp; therefore she wishes to gratify his vanity, that he should have honors &amp; distinctions.  She has met with more than her deserts in marrying him &amp; therefore she ought to be satisfied.  She ought to think that she was once a Music Teacher working for her bread, &amp; now she has an independent fortune.  The bench must have been little in demand, so few Candidates, &amp; such inferior ones.  I believe truly you would have been elected.  The State is beginning to appreciate you; if it does not, I hope the President will.  Genl Thompson today sent for your office key to look at a…this afternoon.  I went to the office to shut it, &amp; I saw Rices Digest open at a page relating to property given to children.  Mrs. Thompson is not confined yet.  I hope she will not be disappointed.  Perhaps the Legislature will not adjourn the 15th.  I almost wish you were coming in the Stage.  I am afraid the roads are so bad you will find the travelling in the carri[a]ge tedious, &amp; the horses will get injured.  Mr. Elford would have gone down in his carri[a]ge but for the roads.  I do not wish you to follow my advice, contrary to your judgement, but I wish you to inquire on the subject, &amp; find out whether the Stage with the night traveling, or the carri[a]ge &amp; horses with the risk of injuring horses is best, or whether the road from Cokesbury or from Laurens is best.  Mr. Arthur says the road from Cokesbury generally travelled is very bad, that there is a more private one that is better.  The Mails are so irregular.  I hope the letter in which you tell me, how you have determined to come, will come directly to hand without any delay.  If it does not, it will be bad.  Only twice however the Mails have failed, though several times I have received no letter, but I suppose you did not write.  Except to hear you speak, I would not care to be in Columbia during the Session.  The weather is so unpleasant, &amp; the house so filled with ladies all seeking pleasure, but I think I will go next winter to hear you speak.  This Spring I would like to go to Charleston, when you go to Columbia, &amp; if we are out of debt &amp; have plenty of money, this summer we can go to the North.  You must send me a copy of your speech, “the Speech of the Session.”  I will read it with more interest now in your absence than when you are with me.  I hope you will soon have it published in the Patriot. I thought Anna would have to send for more money.  She will not have to buy anything again for a long time.  Going away from home, the softer sex require so many things to make them neat &amp; comfortable, that they can at home do without, that it makes it quite expensive, but she is well fitted up &amp; will need nothing more for some time.  I thought she would send for more than 10 dollars. Fanny says she longs for you to come back, but after you come back she will be sorry.  I asked her why.  She said because she would have to go out of my room, &amp; sleep in the big room.  She already says Anna when she comes back must go up to bed with her after supper. Hext is well, &amp; when I ask where Papa is, holds up his hand as if to say gone.  Willie &amp; frank are well.  I have rode out three times, &amp; been to church each Sunday, the rest of the time busy at home. I hope to hear tomorrow, if so I will write more.  You ought to have told me what you thought of the Grocery bill.  At this moment I hear the singing in Becky’s room.  Mr. Arthur says he does not approve of it.  I am sure I do, &amp; hope it will bring religion near to the servants, make them feel its importance, &amp; lead them in the way they should go.</t>
+  </si>
+  <si>
+    <t>EMP249_11_12_1852</t>
+  </si>
+  <si>
+    <t>Sunday morning, 11 oclock</t>
+  </si>
+  <si>
+    <t>My dear husband.</t>
+  </si>
+  <si>
+    <t>The Mail this morning came very late, owing I suppose to the bad roads, to my great disappointment no letter has come from you.  One from Anna, &amp; one from Aunt Mary McCall I received.  I think you must have written, but the Post master in Columbia has neglected sending it.  Tomorrow no Stage comes, so I cannot hear until Tuesday, &amp; if you then write for the carri[a]ge, it may be too late for it to meet you.  Mr. Hoke says he thinks  the roads are too bad for a carri[a]ge to get along at all.  I wish you to come the way you prefer, but I hope you will come in the Stage.  It seems to me that will be the best way on account of the roads both for you &amp; the horses, but if you write for the carri[a]ge I will send it, if the letter comes in time.  I am going after church to dine at Mamma’s so have to write to you now.  I am so sorry I did not hear from you.  I am afraid you were spending your evening so pleasantly with some of those bold ladies, it made you forget your Wife; perhaps Becky Sharpe you got introduced to. I have written to Mr. Elford to buy us a set of common knives for every day use.  Our old knives are lost &amp; worn out, &amp; the new set is too handsome for every day, &amp; would soon get ruined, a common Butter knife I also begged him to get.  You  must bring us nothing at all.  Anna will bring us something.  Charleston is a cheaper place than Columbia.  The little things you get for the childrenare expensive &amp; useless, so bring back nothing but yourself.  I must write to Anna now.  She says she enjoys herself more than she expected, &amp; that she will come up with Mr. &amp; Mrs. Elford, &amp; that I must write &amp; tell you so that I can make you understand better than she can, that she is not to go to Columbia &amp; meet you, &amp; come up with you, but she will come all the way up with Mr. &amp; Mrs. Elford. I hope you will be careful on the R Road &amp; take a safe scarf &amp; wrap yourself up warm. I will now conclude.  I remain Your affectionate Wife, E.F. Perry I am glad you now like my letters.  I like you cannot bear to be scolded, especially by a husband.  The next time you begin, I will call in one of the servants &amp; let you finish on one who deserves it.  But you think you are so certain of my heart, you can impose on it, but you must not venture too far. If I had heard from you this morning I could have written you another sheet.  Now I have nothing more to write about, except to add I love you.  E.F.P. Anna’s letter today was a long one, a whole sheet.</t>
+  </si>
+  <si>
+    <t>EMP250_11_12_1852</t>
+  </si>
+  <si>
+    <t>I had written a long letter &amp; sent it to the Post office &amp; wrote I had not heard from you, when Mr. Beattie sent me two letters.  I can now only acknowledge them, for I expect Susan every moment to come from church &amp; carry me to Mamma’s…I now hear the carri[a]ge. I know the sugar was more than we use, but it is economy to get a large quantity at one time.  The barrels &amp; commissions cost as much if they are small, as if they are large.  I thought &amp; knew the Sugar would not last more than a year.  We have 14 servants.  We use more than a pound of Brown Sugar every day for them, more than a pound of white for ourTea &amp; Coffee each day.  The loaf Sugar was for company, the Clarified for cake, the powdered for icing.  This was the reason there was such a variety. Susan has come &amp; gone, &amp; I must now get ready, for when the carri[a]ge comes back.  I will write again tomorrow. Mr. Brown was not the Soul of Honour as I had thought.  I am glad you are coming up with Mr. Duncan, but think you would find it pleasanter on account of the bad roads to come in the Stage.</t>
+  </si>
+  <si>
+    <t>EMP251_12_12_1852</t>
+  </si>
+  <si>
+    <t>I have just written a long letter to Eliza Hayne, &amp; am tired writing, but will go on &amp; write my daily letter to you.  Tomorrow I will write again, &amp; then I will have a long rest, which I will be glad of, for writing takes up so much of my time I can do very little else now. I wrote in a great hurry yesterday after receiving the two letters by Mr. Beattie. Aunt Mary McCall has a box in town for us waiting to send.  I am so sorry I did not tell her to send it to Columbia, &amp; you would have sent it on by someone.  It contains my winter clothes, but it will be so late before I get it, they will be my next winter clothes, instead of this.  Mr. McKay was to have brought it up, &amp; after all he has never gone.  Mr. Elford now will take charge of it, or it will come by Express.  I hoped to have saved money enough out of what you left me to help pay for them, but I have not been able to, so you must be so good as to lend me the money out of the Bank Interest you will receive in January, &amp; I will give you Minerva’s wages as they are paid me, until I return you all.  I am sorry I did not keep Minerva’s wages this past summer to clothe myself with, but you were pressed for money, &amp; so I spent it for you, which you must remember.  But I would rather feel independent in this respect, &amp; in  future I will not place myself in the situation I am now have to ask you for money for myself.  It makes me feel mean &amp; sometimes the bills are higher than I expect, as it is in the present case, &amp; then I am afraid you will scold me, but you must not.  If you do, I will come down upon you about Governor &amp; Judge &amp; President of the United States, &amp; perfectly overwhelm you.  But in future I intend to buy my clothes, &amp; pay for them without your knowing anything about it.  Last winter I bought nothing, so this winter I had to buy something, so sent to town,  but they will only come in time to be ready for me next winter when I go to Columbia with you. The hogs are being killed today.  The whole household is at the river except El…, Lindy’s baby &amp; myself.  We still have some Stake &amp; some corn beef, but we are all tired of it.  I hope to have a plenty for you to eat on your return of Sausages, Spare ribs &amp;c. Willie says Mr. Memminger &amp; his family were at church yesterday, I suppose on their way down.  Eliza Hayne said Mr. Memminger had a daughter sick like Ann, cannot sleep at night &amp;c. You must find Janney’s far pleasanter than Maybins.  I am glad the Society is so pleasant there.  I will take for granted all the sentiment &amp; love you would like to express in your letters, &amp; which I know is in your heart.  You are in Columbia to attend to business, &amp; if you let me occupy you instead, it would be to the detriment of the State, of which you are the chief guardian.  If your watchful eye is moved for one instant, the State suffers; so I do not wish to interfere. I thought you were going to run Mr. Elford for Clerk of the House.  Mr. Dean perhaps being a Member could more readily be elected.  It requires a person either to be, or have been a Member of the Legislature to be elected to office.  It is a great advantage.  Several wives have been gratified unexpectedly this Session.  Mrs. Dean, Mrs. Glover, &amp; a future Mrs. Evans, one other Wife I would name, who would like to be gratified in the same way, all she begs of her husband is when opportunities offer to advance himself, not to decline it.  The husbands may be indifferent to these things, but the Wives never are. I am sorry yourself, Col. Brockman &amp; Mr. Elford have so misunderstood my Grocery bill.  I knew the Sugar was more than enough for one year, but I thought it would be more economical to send for a large quantity.  It saves commissions, barrels, drayage &amp;c. , &amp; we would not have to send for Groceries for a long time again. I am sorry it should have lead to a worse opinion of our servants characters than they deserve.  Reuben stole a ham, &amp; I dare say, he steals your Corn, &amp; steals our wood &amp; sells for himself, &amp; Mary has stolen my clothes, but the other servants I have no reason to suspect, &amp; hardly think Mary will do the same again.  I am sorry Mr. Elford should think me so careless a housekeeper, &amp; such a fool as not to lock up the Sugar that the simplest child would know ought to be done.  If my storehouse had groceries in it, I would never let anyone go in but myself, but it never had lard, only House Salt &amp; such things, that it was not necessary for me to go always to take out.  So tell Mr. Elford I think as he does if Sugar was not locked up, it would go twice as fast, &amp; if Corn was locked up, it would last twice as long.  I know of nothing new &amp; Hext has come now to be nursed, so I must stop, &amp; close my letter without reading it over.  The weather is cloudy &amp; cold.  I hope you will have a pleasant journey home the roads not impassable. I hope to hear from you tomorrow, &amp; every day till you return. Willie &amp; Frank are busy with the hogs.  Make Mr. Gladden &amp; Mr. Hill pay you, &amp; tell Mr. Watts to remind Mr. Williams of his promise. I will now close.</t>
+  </si>
+  <si>
+    <t>EMP252_14_12_1852</t>
+  </si>
+  <si>
+    <t> I received a letter from you this morning, &amp; am very glad to hear from you.  I have written to you very often.  I would have written oftener, but every day I write one letter to your Papa &amp; sometimes two.  The Mail sometimes brings no letter.  I write &amp; tell so, &amp; afterwards, some gentleman sends me a letter they have brought, &amp; then I have to write again to say I have heard.  I have sent your letter to your Grandmama to read.  This is a gloomy, cold day, &amp; I think it will cheer them up, to hear a little news from Charleston.  Vardry &amp; Alex are over there.  Alex has the Measles.  Vardry will be glad to hear about his knife &amp; Sugar dogs that you have not forgotten him, but I think a knife a dangerous present for so little a boy.  You had better bring him something else.  If you can think of something better, a Story book he would like.  He is fond of hearing stories read, buy some suitable play thing he would like, a little wagon or something of that kind.  Annie will be glad of the Doll.  You had better bring both hers &amp; Fanny’s ready dressed, buy a large head for the large doll, the largest you can find I expect will not be too large.  The present head is broke, &amp; a head for the other body that once had a China head also get.  That one will be small &amp; not cost much &amp; will do for Fanny to play with every day.  The doll ready dressed Fanny will use only on particular occasions.  The large doll is to teach you how to work, &amp; as the body costs so much, it is a pity for it to be without a head, which is the reason I wish you to bring a head for it.  If your money gives out, get Aunt Eliza to lend you, &amp; I will return it when I send money to pay for what I yesterday wrote Eliza to buy for me, or after your Papa can be done without, that it still takes a great deal more money than one at first supposes.  Now in town, it is such a good opportunity to buy what cannot be got here, &amp; there is so much to tempt, that I am willing to gratify you now, knowing you will be willing to deny yourself hereafter.  The new bonnet you have bought will last a long time this winter, next summer &amp; next winter you can wear it.  I am sorry your Cloak has not been made before.  You ought to have had it soon after your arrival, for the weather has been such as to make you need it.  I hope it is now made; it must be very pretty material, &amp; your bonnet must be  very pretty also.  Tell your cousin Eliza she must get me a pretty one.  I wish you to get a new dress, &amp; am sorry you did not get it immediately after your arrival.  You ought to have had it to wear visiting among your friends, &amp; you must get it now &amp; have it made up soon, so it may be of use to you before you leave.  I wish it for your dress frock all winter.  A bonnet for Fanny like yours will be pretty, &amp; if you can find a Worsted Cloak large enough for her, get it.  I intended buying one for Annie, but Susan has had a Cloak altered for her, which will answer for the winter, &amp; she says she prefers my giving her something else. What was the price of your Silver Comb?  I hope Eliza will write to me soon.  I have been expecting a letter from Aunt Eliza.  Ask her why she does not write.  I am glad you are enjoying yourself so much, &amp; meet the approbation of your Aunts.  Tell Aunt Anna Hayne I am gratified at her good opinion of you.  Icey Frank as soon as he was aware he had curls begged me to cut them off, as they were too girlish for him, that he is not the pretty curly headed boy as she may see from his likeness, but a fine looking handsome manly boy, &amp; his appearance even if he does not deserve it makes him a favorite with everyone.  Tell her the likenesses did justice to none of the children but you.  That Willie is a smart sensible boy, useful &amp; manly, drives us, &amp; hauls wood, &amp; cuts wood, &amp; then comes in the house &amp; reads, but still has that mischievous temper that will indulge itself in teasing &amp; playing.  He means no harm by it.  He is alive to the ridiculous, &amp; has a satirical vein, which your Grandmama thinks he inherits from her family, and he cannot help amusing himself with his brothers &amp; sisters but as he grows older he gets better, &amp; your Papa says he is a good boy, &amp; he is no flatterer.  Fanny is warm hearted &amp; affectionate, lively, &amp; your Papa says the prettiest &amp; smartest of all.  She yesterday said, “if I die first, I give all my play things to Anna.”  She says she longs for you to return.  She came out of the kitchen this morning very much offended Becky had turned her out.  The Lard is drying in the kitchen &amp; it is crowded &amp; confused, &amp; it is no place for her, so Becky was right, but she came in crying, &amp; asked me if Papa had given the children to Becky. &amp; if Dr. Irvine had built that kitchen for even Priscilla had told her to go out.  Hext is today 18 months old, a baby yet, for he is not weaned, &amp; nurses at night more than ever.  His eye is almost well.  At least his eyebrow there will be a little mark always on his eyebrow, but it will not be observed.  He is quite well.  Priscilla was here doing nothing, &amp; in the way, so yesterday you Grandmama was here, &amp; I told her she had better ask Mrs. Irvine to let her stay with her, so she did, &amp; Mrs. Irvine said she might &amp; this morning she went over.  She can bring in wood &amp; wait on your Aunt Annie &amp; come in on messages, &amp; I hope will be useful.  Catherine is of no use at all except to mind her Mothers child, &amp; yet your Grandmama pays 1 dollar a month for her &amp; is obliged to, while she keeps B….  Mary minds Isaac.  If Mama parts with … &amp; can get no one better, I am going to let her have Lindy.  As Becky is here, we have more servants than we can afford, so will hire out Lindy to your Grandmother for less than to anyone else, so I hope she will do well, for it will be well for her to have a family servant there, &amp; one who cares for her, &amp; make up to us the expense of buying Becky, which was very unexpected.  Lindy still has Rheumatism in her feet, but is able to work, &amp; by Spring I hope will be able to go to your Grandmama’s.  I received two letters from your Papa today.  He says the Legislature may not adjourn until Friday.  He says he is anxious to return home to see his Wife &amp; children who he loves better than fame, honors, distinction, property or anything besides, that though he has been passing his time very pleasantly, after two weeks…he always gets homesick.  He mentions having heard from you.  Your visit to the City must not make you discontented with the country, but on your return you must contribute your share towards the happiness of the home circle.  Your Papa had received a large box from town.  Your have seen Mrs. Elford I expect…your clothes.  </t>
+  </si>
+  <si>
+    <t>EMP253_14_12_1852</t>
+  </si>
+  <si>
+    <t>Tuesday, 12 oclock</t>
+  </si>
+  <si>
+    <t>I have just written a long letter to Anna &amp; am tired, but will now write to you.  I was very glad to receive two letters from you today, &amp; one from Anna.  I read Anna’s to you.  She writes well, &amp; Aunt Anna Hayne tel[l]ing her to write me word; that she did credit to her parents, is worth something, for Aunt Anna is very particular about the behaviour of children, expects more from them, than anyone I know of.  Anna asks after Hexts eye.  She ought to say his eyebrow.  Frank one day in the yard accidentally struck him on his eyebrow, &amp; it bled, but only for a little while, &amp; is now quite well.  I explain, for you might wonder what Anna alluded to.  I am glad she enjoys herself so much.  I was afraid she would be homesick.  Her visit will be attended with expense, but I dare say it will be of permanent benefit to her, &amp; she will be improved &amp; so many relations I have in town ought to see the children to feel an interest in them.  What Anna has bought will last her next winter.  I have written to her that there is so much to tempt her wishes, if they are gratified now, she must be willing to deny herself hereafter.  I think she will need more money.  If you would send her some just before you leave Columbia, I would be pleased, &amp; it would please her to be so thoughtfully remembered by her Father.  She will not for a long time again cause us so much expense.  I am glad you have received a box.  I hope it is the one from Aunt Mary McCall.  I would wish you to send it in the quickest way, for I ought to have had it weeks ago.  I have not made a single winter article of clothing yet.  Can it not come immediately by the Stage.  Write on the box that it must be sent by the Stage.  If you have not sent it yet, or do not until you come, be sure to bring it. If it cannot come in Mr. Duncan’s carri[a]ge, send it by someone coming in the Stage.  am very much pleased at the good opinion the Members have of you.  It is only for you to be known to be appreciated at a distance your character is not understood, but those who know you best, respect you most.  It requires but very little exertion on your part to be rewarded with the honors others get, for I think the prejudice against you is passing away.  I hope your friends will still as they proposed show their estimate of your character by voting for you for Governor.  I do not expect you to be elected.  It will please me though for you to receive votes.  It will make them think of you another time. Yesterday the hogs were killed.   Today Mr. Lasly &amp; his daughter are helping cutting the meat, drying the Lard &amp;c.  The daughter did not come in yesterday.  I thought she was at the river when I wrote to you.  The servants are all busy.  Mr. Lasly seems very obliging.   I have been several times to the L… house since I have been writing to you.  He says we ought to have 10 Cans of Lard, but I do not think so.   Charles says we ought to have had Becky 10 years ago, that he likes her, so do all the servants.  I have not yet seen any cause to regret buying her.  Lindy did not answer, even when she tried her best.  The servants did not respect her, so it was one constant state of confusion &amp; Minerva who we would have been obliged to take home, makes everybody unhappy about her.  Lindy in the Spring we must hire out.  We now have plenty of Milk.   We milk three Cows, the last one only commenced today.  This winter we can either churn, or have rich Milk, Syllabub, Custard &amp;c.  We will have plenty of Meat, Sausages, spareribs &amp;c.  The parsnips in the Garden Becky cooks delightfully, so when you return, we will live better than when you left, particularly after our Groceries come.  If Col. Brockman &amp; Mr. Elford let you get any Sugar, &amp; I lock it up, so the servants cannot steal it. Today is cold, rainy, &amp; gloomy.  The weather has not been suitable for cleaning the yard, scouring &amp;c.  I will be almost glad the Legislature should sit a little longer, to allow you more time to pass important bills for the reformation of the State, &amp; the Equality of the Upper county, &amp; allow me more time to clean the house for your reception.  It is cold.  I can hardly write.  Hext wants me, &amp; the children are making a noise.  I will be so glad not to have to write so much when you come back.  It takes up so much time &amp; fatigues me, so that I can hardly do anything after but rest, but for your comfort I write every day.   I hope you dined with your old friend Mr. Hearn.  In inviting the Greenville Delegation, I think Pinckney McBee ought always to be excepted, for he would be out of his place, &amp; would not even enjoy it, &amp; does not deserve it either, so I hope he is not included.  I have not heard yet of Mrs. Thompsons being confined.  I am glad you have dyed your Whiskers.  I expect your look five years younger.  You ought to have done it when you first went down. Anything that adds to your comfort, convenience, &amp; good looks, you must get. Be sure to bring the box with you or send it by the Stage.  I will be very glad to see you.  The weather is getting bad so cold cloudy &amp; rainy, but I hope it will clear before you set off.  Be careful &amp; not get hurt on the R[ail] Road. Hext if he has forgotten you, will soon remember you.  He calls Charlotte Oh Da, &amp; when he is in my lap, &amp; I say Oh Da come &amp; take Hext, he clings close to me. I thought you were going to buy a new W[h]ig, but perhaps the present one will do until you go the North &amp; get one there. I must now close.  I wish you could go &amp; see Col. &amp; Mrs. Preston before you leave.  If so give all of our love to you. I write in a great hurry &amp; will write until you set off to come home.</t>
+  </si>
+  <si>
+    <t>EMP254_15_12_1852</t>
+  </si>
+  <si>
+    <t>Wednesday, 1/2 past 9</t>
+  </si>
+  <si>
+    <t>I have just received a letter from you &amp; I cannot help saying, I feel very sorry when you are so respected by the Members, &amp; appreciated by them that you should not aspire to some of the honors in their gift.  Why do they elect such inferior persons to office as Mr. Glover &amp; Manning, &amp; not elect you who are superior to them.  I believe if you wished it they would elect you, &amp; you ought to have been elected Judge.  The 3000 a year would be a certain income which you rarely ever make.  This Session you seem to have been better treated than usual, &amp; you ought to have tried for something.  You seem to be more popular out of your District now, than in it, &amp; I wish it was known in Greenville, how well others think of you, for I wish everybody in Greenville where you live, to respect &amp; look up to you.  I will live on hope that you will not always be excepted in the distribution of honors, but it is your own fault, even Jones got what he tried for. This is another gloomy, rainy, cold day.  The roads will be dreadful.  It has given me no chance of cleaning the house &amp; yard, which need it much.  I wished everything to look nice for your return.  Even the washing cannot be done in this weather, which makes us very uncomfortable, having to do without handkerchiefs, towels &amp;c.  This is no weather to leave home, at least for ladies, so much as I would like to hear you speak in the Legislature, I do not expect to go down, unless it is to see you inaugurated.  I hope the Secessionists voted for you, &amp; another time that they will elect you.  It is strange there have not been more Candidates this time for Judge &amp; Governor. The servants say Mrs. Thompson was confined Sunday night &amp; has a Son.  I suppose it was in expectation of that, Genl Thompson was looking in Rice’s Digest at laws respecting property given to children. Mr. Rosemond yesterday sent some Lumber for the kitchen. Four Cans of Lard were dried yesterday, &amp; five or six more there will be.  That alone at the price Lard is selling 15 cts a pd, is more than 60 dollars.  The Kentucky Hogs are so fat.  In future I would prefer buying a few of them expressly for Lard, the rest…meat.  We will have a good many Sausages.  The servants are stuffing them today.  We got a machine from Mr. Rutledge which grinds the meat fine instead of chopping it.  We gave Mr. Lasly some of the Back bones, Spare ribs &amp;c.  He &amp; two sons were here the first day; he &amp; his daughter the second.  I would not have had him the second day, but Reuben said he himself would be obliged to haul wood, but it rained &amp; he did not.  Mr. Lasly has 10 children, the youngest 7 months old.  They are too large a family for our small Farm.  I think he has made a good bargain.  He ought to have paid for the house himself. I wish you had sent me all of Anna’s letters she wrote you.  I would like to read them.  Letters are my chief comfort when those I love are absent.  My disappointed hopes make me unhappy for a while, but I get over it &amp; hope on.  I now look to favors from the President for you.  I may not write again.  I suppose tomorrows letter will tell me when the Legislature adjourns.  If you do not hear from me again, you may know it is that I have not written, thinking you will leave Columbia before the letter reaches there. I do not suppose one wife besides myself has written to her husband every day as I have.  I assure you it interferes with my duties.  I am obliged often to send Hext away crying because he disturbs me, &amp; after writing I am fatigued &amp; unfit for cutting out work &amp; sewing so it makes me waste my time which is precious, for there is sewing still to do for servants &amp; children, &amp; Eliza being near confinement, often feels unwell &amp; has done nothing for me for weeks.  As for myself I have not done the first stick, &amp; what I most need is in the box that has been sent to you &amp; which I hope you will soon send up, or bring up with you.  I give up all to you, as my first wish is that you should be happy, &amp; if I do not write every day, I know you will be uneasy.  I wish your mind also kept calm &amp; quiet so you can attend to your Legislative duties.  Since Mr. Memminger is away, I expect you are the most important member in the house. This is dreadful weather, so cold &amp; cheerless, &amp; raining slowly which makes the roads &amp; yards so muddy.  I am glad you have heard from Mr. Livingston.  I was thinking the books had failed, &amp; no more numbers would be forthcoming.  Nothing comes from the Post office for you.  I suppose it is known you are away from home. Charles this morning was speaking of Becky in such a satisfied manner, that I told him if Baylis &amp; Peggy were out of the way, I believe he would try for Becky.  He laughed immoderately, &amp; said if he was young he did not know what he would do.  He told Willie Mr. Dean was going to move into the village where Mr. Bacon has been living, so Peggy would be nearer.  He will be saved his long walks.  I hope you will have a safe &amp; pleasant journey home &amp; pleasanter weather than we now have. I will now conclude.  My hands are cold &amp; go to the fire &amp; warm.  I hope to hear every day until you return.  Your affectionate Wife, E.F.P. P.S.  I wish Willie had gone with you.  He always improves when with you.  I wish there were better schools than in Greenville.  The Baptist College is a poor affair.</t>
+  </si>
+  <si>
+    <t>EMP255_16_12_1852</t>
+  </si>
+  <si>
+    <t>Wednesday, 11 oclock</t>
+  </si>
+  <si>
+    <t> I received a letter from you this morning, &amp; also one from Eliza.  I received one from your Papa.  He leaves Columbia tomorrow morning, so I am not to write to him again &amp; will be able now to write longer letters to you.  I am glad you are still enjoying yourself.  If you do not come home by Christmas, you will lose nothing, for you know at that time the servants having holiday, we live in less comfort than any other part of the year.  It reminds me of the way we are living at present.  This week Mr. Hoke bought some hogs for us, which have been killed, &amp; instead of living in abundance as one would think, we almost starve, &amp; have our meals irregular, all the servants being engaged drying Lard, cutting up Sausage meat, cleaning feet, stuffing sausages &amp;c, that they have no time to attend to us, so busy preparing for our future comfort.  Susan Hoke said she would write to Augustus to call &amp; see you, but as you have not mentioned him, I suppose you have not seen him.  She sends over to know if you mention him in your letters, for they were uneasy not having heard from him.  Fanny Hoke is quite sick with Measles &amp; Scarletina. Perhaps you heard that Mr. Sam Mauldin was carried down to Columbia &amp; put in the Lunatic Asylum.  He attempted several times to kill himself.  He took Laudanum in Greenville, going down he attempted to jump out of the Cars &amp; when left in the Asylum, tried to beat his brains out.  He eats Opium which is worse than drink.  How sad for his Wife &amp; family.  James Benson is married to a Lady in Abbeville. Mr. Wm Easely is married to Miss Sloan of Pendleton   Mr. Joab Mauldin is married to Miss McIver.  Mrs. Mims Sister Mrs. Genl Hampton has a Son.  This is all the Greenville news I know of to tell you. Frank commenced a letter to you, but I saw it would take so long to finish it, I told him he might stop.  Willie is generally busy reading, cutting &amp; hauling wood, &amp; as I write so often, he thinks he would have nothing to tell you.  Hext is quite well &amp; when I ask where Anna is, holds up his hand, as if to say gone.  Fanny speaks often of you &amp; calls you my sister.  She longs for Papa &amp; Sister to come back, &amp; then adds, I will be sorry too, &amp; when I ask why says because I will have to go out of Mamma’s room &amp; sleep with Anna.  Now I go upstairs &amp; sit with her at night.  Then she thinks that will be put a stop to, so she feels quite divided.  She wishes though she had gone to town with you, &amp; says I ought to have let her.  I did not think of it, but the weather has been so bad ever since you left, that I think this is the very worst time to leave home for enjoyment.  The Spring is much pleasanter &amp; is always the time I will choose. I am glad Uncle Arthur &amp; all of your friends are so affectionate &amp; enquire after us all so kindly.  They are kind to you not only for your sake &amp; mine, but for your Grandmama whom they all love.  You must go to see all of her old friends.  I often wish she would see them once more.  I know she must miss their friendship &amp; society.  You must buy a present for each servant.  I wish this Christmas to give each of the grown servants a Bible.  Reuben, Eliza &amp; Becky I think can read.   Charles, Lindy, Mary, Edward &amp; Clara can bring theirs to me or you at any time to read to them.  8 Bibles plain ones I will have to get.  If Eliza could get reasonable ones in Charleston, &amp; have them packed in the box she is to send, I would like it, but if she thinks it will take up too much room, I will get them here from Mr. Elfords book store.  A prayer book get for yourself &amp; one for Willie, a neat plain one for him, of a convenient size to put in his pocket. Becky’s comb you must not forget &amp; some little present for Ninny, Lucinda, John &amp; each of our servants, either a handkerchief, apron, or something pretty if you prefer it, not the value of the  present, will they regard but your remembering them, &amp; anything from Charleston will seem to them great.  A little present for Mary Mauldin also get.  Little China ornaments can be got for 15 cts.  Those little baskets, cups &amp; saucers &amp;c. that we have had, were of that price.  Get a little present for your Grandmama, Aunt Susy &amp; Aunt Annie, also for Vardry Alex Annie &amp; Susy, a doll for the two latter &amp; some toy or book for the former, a dress for Lindy’s baby of cheap calico, a knife for Willie &amp; Frank, the dolls &amp; sugar toys for Fanny, &amp; with the 2 dollars she gave you buy her a large box of Furniture.  I wish her to begin having a baby house, so as to keep all her things in order.  At some future time I wish you to get a dinner set of China for yourself so inquire now the price.  It will be useful when your young friends come to see you.  You can have a table set to yourselves.  I expect now you cannot afford it.  Some time hence you might get it.  If you need …rilla before you get back, you must buy some &amp; take.  Mrs. Elford went down first, &amp; I expect sent you the gingernuts.  Mr. Elford went down afterwards, I expect had the hair &amp; a letter for Eliza.  You must get Eliza to buy two bottles of “preparation of Castor oil,” one for Aunt Susy [&amp;] one for me.  I am glad you got a new bonnet.  I would like one for Fanny, if it is as pretty as any others worn by little girls of her age.  I have bought a Worsted bonnet here for Hext, &amp; given him Fanny’s cloak, so he can do without anything.  Buy a Cornelian ring for Annie &amp; Fanny, &amp; one for yourself.  I wish you to buy a dress, &amp; have any new fashioned apron; Sack or new bonnet, or anything else pretty you see made up for yourself.  All the pretty patterns you can get, bring.  I am sorry you will not see Aunt Harriet &amp; Sarah, &amp; that you have not seen either Aunt Emily or Aunt Susan, &amp; that sickness is the cause of not seeing the two later.  This visit is an event in your life which you will never forget, &amp; you are grateful I am sure to your friends for being so kind, &amp; will always do what you can in your power to return it.  I hope you will see Eloisa’s family before you leave.  The Legislature adjourns today.  Your Papa sets off tomorrow, &amp; will return in Mr. Duncan’s carri[a]ge, for one of the sons went down in it.  The roads must be very bad.  It is raining now, &amp; has been for several days.  Give my love to my friends.  Go &amp; see Mrs. Elford &amp; write when she will return; also go &amp; see Mary Crayton.</t>
+  </si>
+  <si>
+    <t>EMP256_17_12_1852</t>
+  </si>
+  <si>
+    <t>Friday morning 1/2 past 9</t>
+  </si>
+  <si>
+    <t>I wrote you a long letter yesterday &amp; did not expect to write to you today, but as tomorrow no Mail goes, I will write now.  I have just received a letter from your Papa.  He is to leave Columbia today, &amp; hopes to be at home tomorrow evening.  He comes up on the R[ail] Road &amp; from there in Mr. Duncans carri[a]ge.  As neither of us now have to write to him, we can write oftener to each other.  I would be glad if every morning you would write to me, &amp; tell me everything that interests you.  You will in this way tell me more than I will otherwise hear, for you will write of what may escape your mind when you get home.    As soon as you know from Mr. Elford what time he is to return, let me know. Four days in this week it has rained.  Today it seems as if the weather may clear.  I hope it will.  For your Papa’s sake who is coming home, for your sake, that you may be able to go about, &amp; for my sake that I may have the house cleaned.  It is very dirty, so much mud is brought into the house by the servants. The carpets I have had turned, &amp; whitewashed the two Dining rooms, &amp; bought some reasonable furniture Calico at Crittendens &amp; made new curtains for the dining room windows.  The Calico is beautiful &amp; was only 9 1/4 cts a yd &amp; everything looked neat, but the rainy weather has caused so much dirt to be brought into the house, that I now have to clean it all again.  The soil here is very bad, different from the City, &amp; there the yards &amp; streets are generally paved, which is so neat.  We are all well except Eliza.  She is sick in bed, &amp; has been unwell a long time.  Dr. Crooks had to come &amp; see her today.  Becky gets along well with all the servants.  They like her, &amp; respect her, so I hear no more abuse &amp; quarreling among them as I used to.  Baylies has Prayer meetings every evening in his room at…it is more of family prayers for the servants in the yard.  He thinks Lindy is feeling an interest in religion.  I hope so, &amp; that it will make her a good servant.  Next Wednesday the 22nd Rutters time is up, &amp; as your Grandmama does not like to hire Rutter with her two children, &amp; have to pay 1 dollar month for Catherine who does nothing for her, only minds Rutters child &amp; cannot even talk or go on a message, she intends to let Rutter &amp; her children go home, &amp; try Lindy instead.  If she does well, she will keep her.  If she does not, she will look for another servant.  Priscilla is there now, &amp; I expect will stay there for her food &amp; clothing.  She will help mind Lindy’s child.  Aunt Annie is very poorly.  Your Grandmama is not well today.  Alex &amp; Vardry have been there since Saturday, on account of Alex being sick with Measles.  He has worms also.  The weather has been so bad, that since you left I have been out very little, once to your Grandmama’s, three times to ride on business, &amp; twice to church.  Susan, Annie &amp; Susy staid with me awhile.  Becky sent in word last night to say, I must write you word not to forget her comb.  Your Aunt Susy says you must be sure &amp; bring 4 Sugar dogs for her children, &amp; if the 25 cts she gave you to buy them with is not enough, to get more money from Aunt Eliza, who has some of your Grandmama’s money.  She wishes pretty dogs, &amp; the children will be very much disappointed if you do not bring them, so you must not forget it.  Your Silver comb cost so much less than I expected, that I wish you to get one for Annie just like yours.  I suppose your size she can wear now, &amp; when she gets older too, she needs a comb always to keep back her hair.  The horn one she breaks, &amp; one of the plated kind her Mamma got her, but it hurts her head &amp; she cannot wear it, so as I intended to get her a cloak but now she does not need one.  I will instead get her a silver comb, which will be a lasting useful present for her.  You I expect will not have money enough to buy it, so if your cousin Eliza will add it to the list I have already sent her, I will pay for it, when I pay for the other things.  Willie &amp; Frank have bought have bought two pigs from me.  As soon as they can get at their Bank &amp; pay me, I will send you the money to invest in something for them, books perhaps.  The Candy &amp; Cocoa &amp; ground nut cakes you must not forget.  50 cts worth of Sugar ground nut cake, 50 cts worth of Cocoa nut cake, 50 cts worth of Candy of different kinds, &amp; 50 cts worth of Cakes of different kinds.  These things are instead of buying anything here for Christmas, &amp; if you are not here Christmas, we will put off the celebration till you return, &amp; it will be better, for at Christmas the servants have holiday, &amp; cannot do much for us. After their holiday is over, they can wait on us, &amp; Becky will make us something nice.  So do not regret if you are not here Christmas, we will wait for you.  I want you to buy a nice little bible for yourself, a larger size I wish for Willie &amp; Frank.  If you choose you can buy the three Bibles in town. Beg Eliza to have a Cloak made for Fanny &amp; buy a pretty bonnet &amp; all I have written for.  Fanny has no cloak to wear to church.  I wish it made up, for Eliza is sick, &amp; cannot work, &amp; I have no pattern to make it by.  Some little girl of Fanny’s age you will know of to fit by.  Be sure to bring the cloak made, &amp; try &amp; get patterns for yourself. Beg Aunt Anna Hayne to carry you to see her friend, &amp; our friend Elizabeth Jones.  I did not know until you mentioned it, that the Canaries were dead.  Gine my love to your Aunts &amp; cousins.</t>
+  </si>
+  <si>
+    <t>EMP257_18_12_1852</t>
+  </si>
+  <si>
+    <t> I have just received a letter from you, &amp; one from your Papa, the last one I will get from him for a long time, for he will reach home today.  Mr. Hoke has just sent me word, that he heard of his just having left the head of the R[ail] Road, which I was thankful to hear, as so many accidents now happen.  He comes home through Abbeville, passes Cokesbury where Mrs. Holmes lives, &amp; was to sleep at Col. Wares last night. I must begin &amp; tell you of the increases in the family which will surprise you.  Yesterday afternoon I rode over to Mamma’s, &amp; as soon as I got back, the children came running to me, crying out, “Eliza has a baby, it is to be Hext’s maid,” &amp; so it was.  Eliza has a girl, the baby is well, but Eliza last night was very ill.  She fainted, &amp; was out of her head.  I went up to see her.  This morning she is better. Before I was out of bed this morning, Frank came running up saying “the Sow has five pigs.”  So I told him I would give each of you a pig, which you must each attend to, &amp; when they grow up, you would sell them to your Papa. Since you left two Cows have had Calves, so you see what an increase there has been in the family.  Willie &amp; Frank will soon have to help your Papa support them.  We now have plenty of Milk &amp; Cream.  Willie &amp; Frank enjoy it, &amp; have given up Tea &amp; Coffee which I am glad of.  Your not coming back with your Papa will give us two pleasures.  We are now with pleasure expecting him, &amp; afterwards we will have the pleasure of looking forward to your return.  Your Papa writes, he has directed you to get money from Mr. Elford if you need it.  Mr. Elford has money of his.  You can also tell your Cousin Eliza, that she can get money from Mr. Elford to pay for the things she buys for me. I know I will like your Cloak, &amp; all you have bought.  I may before you leave write for a few more things.  I hope Eliza will have a pretty cloak made for Fanny.  I would like you to get the largest size box of Furniture  for Fanny.  I want her to have a baby house.  She gave you 2 dollars of hers.  If 150 the Furniture costs, with the 50 cts left, buy some other toy for the baby house.  I would like you to get a Bedstead for it, &amp;   several other peices of Furniture also bring her that will be suitable for the baby house.  She is so fond of arranging things it will delight her to fix the house, &amp; give her occupation, which we have to find for children to make them happy. I am glad you are making so pretty a quilt.  I wish you always to have one on hand.  Eliza said Worsted Quilts were pretty, &amp; they must be very warm for winter &amp; suit Greenville.  I wish you would get her to make one patch, buy several kinds of Worsted cloth, &amp; you bring it up with you &amp; make a quilt.  I am glad your Aunts think you behave well, &amp; feel young again.  In being with you, interest in the young is what prevents persons feeling their age as they grow older, &amp; it is wisely ordered.  So old age is not as sad as it otherwise would be.  We live over again in the young.  We are interested for them, as we once were for ourselves.  You must bring us any present you think proper.  I wish two pair of Mits to wear in the house &amp; a neck ribbon to wear to church.  You may bring me these as presents.  For your Aunt Eliza’s present, ask your cousin Eliza what to get for her mother, &amp; then ask Eliza what to get for Eliza &amp; Sue. Mrs. Barnwell Rhett’s is a sad death, &amp; she will be a great loss to her children.  Children require so the care of a Mother, that her loss is even greater than the Father. Tell your Aunts Willie is not quite so ungallant as he was.  As he grows older he feels the value of the Fair Sex &amp; pays them more respect. Tell Aunt Eliza, no change for the better takes place at your Grandmama, that Mammas situation is one of constant trial, &amp; I wonder her mind &amp; body have been able to bear it.  A living trouble like hers is worse than death.  She tries to be cheerful &amp; to bear up, but it is hard not to despond.  Aunt Eliza must write to her &amp; try &amp; comfort her.  Her letters are consoling.  She must also send messages to Susan to tell her to bear up. &amp; to Ann to acquiesce in what has happened.  You must bring your Grandmama &amp; Aunts whatever present you choose, either something useful or pretty.  Buy for yourself a few peices of Music, easy enough for you to learn. I wish you could learn to Crochet. Since I commenced writing Aunt Mary McCall’s box has arrived. It stopped in Columbia &amp; your Papa sent it on by the Stage.  Tell your cousin Eliza the bonnet is prettier &amp; fancier than I expected.  It is a dark Straw with a feather, so I will be able to wear it to church, but it is not suitable for common occasions, so the one I wrote her to get, I will still be glad of, as I need one to wear on occasions that the other I would not wear the feather would look unsuitable, &amp; it is very small.  Tell her the Cloak Aunt Mary has sent me is beautiful to look at, but not useful.  It is the lightest grey colour &amp; so small, it cannot meet across the chest. So instead of the bonnet, the Cloak I must try &amp; dispose of.  Ask her what a Cloak like the kind she is now making for herself would cost for me, the materials &amp; the making it.  I like a dark Cloak that will not soil easily, for even our carri[a]ges here are not always clean.  I will get her to have a cloak made for me.  I am as tall as Eloisa, but much stouter across the chest particularly &amp; back. </t>
+  </si>
+  <si>
+    <t>EMP258_21_12_1852</t>
+  </si>
+  <si>
+    <t>Tuesday evening</t>
+  </si>
+  <si>
+    <t>Your affectionate daughter,</t>
+  </si>
+  <si>
+    <t>We were all out this morning shopping, &amp; that is the reason why I did not write to you.  I will not have time to write but a few lines.  Aunt Emily has invited us to drink tea this evening with her.  It has been raining &amp; thundering today but this morning was beautiful.  Aunt Eliza says that she knows that Aunt Emily is going to send for us, if it pours down.  It  has stopped raining now.  Aunt Anna &amp; aunt Martha are going in the country,,,that is Thursday.  They are to take tea with aunt Eliza tomorrow evening.  All of my relations are kind to me &amp; they all send their love to you all.  Cousin Sarah Gibbes invited me to tea yesterday.  I went.  I spent a very pleasant evening.  She has three daughters &amp; four sons.  Two of her sons are grown &amp; one of her daughters.  The next daughter is fifteen &amp; her next just eleven.  She sends her love to you all &amp; says she is very sorry for Aunt Annie, &amp; aunt Susy.  Cousin Eliza says she will try to have a cloak made for Fanny.  I saw Miss Mary Drayton in the streets this morning &amp; she said that Mr. &amp; Mrs. Elford  were going next Tuesday or the end of next week.  I expect that I will go up with them.  I am enjoying myself exceedingly well.  I have bought six bibles for the servants. Cousin Eliza says she will get the other two for the servants if you wish her to do so and the two for Willie &amp; Frank.  I have just received a letter from you but have not time to answer it.  Give my love to all, especially to Papa.  Your affectionate daughter, Anna. P.S. Aunt Eliza, Cousin Eliza, &amp; cousin Susan send their best love to you all.</t>
+  </si>
+  <si>
+    <t>EMP259_21_12_1852</t>
+  </si>
+  <si>
+    <t>My dear Anna</t>
+  </si>
+  <si>
+    <t>Your Mama,</t>
+  </si>
+  <si>
+    <t> I have just received two letters from you, and one from Aunt Eliza.  I write to say as there is such a difficulty in having work done, I will give up having Fanny’s cloak made.  If the materials are bought &amp; a pattern sent, I will have the Cloak made here.  I will make it myself.  If a ready made Worsted Cloak would have been got, it would have saved the trouble of making one.  If cloak patterns cannot be got, perhaps a S… a large one will do.  If so get [page torn] materials for a S… &amp; a pattern. I wrote to Eliza to have a Cloak made for me; at least that I would wish one, but as there is such a delay, it will be best to inquire the prices of ready made Cloaks, black silk &amp; other dark kinds.  It will be better to give more, &amp; be saved the trouble of buying materials &amp; waiting to have the Cloak ma[de].  There is such a delay in fitting oneself with suitable winter clothes, so that this winter I am obliged to have some things.  Last Sunday I wore a hat with a feather, &amp; an old black Silk dress, &amp; felt very shabby indeed.  As Eliza wil[l] be confined to her room for a month I got Margaret [to] let Clara come &amp; make a dress for me, the first she has ever made alone.  She is now in the room with me making the dress. Tell Aunt Eliza Aunt Mary McCall sent me two beautiful dresses.  The blue one was got at Browning &amp; Semans 25 cts a yd.  The whole peice looks beautiful, much prettier than yours at the same price.  The Cashmere is 75 [page torn] &amp; is embroidered.  I send a pattern, but not of the part embroidered.  Mary said belts were not worn, the dresses were peaked, but I intend to have my dresses made my same favorite way &amp; so need a belt for each dress.  Ask Eliza to buy me a belt for each.  They can come up in [page torn] large envelope, if no opportunity occurs. There are a great many stores here, but the shopping is very limited.  If we get a dress, we cannot get trimmings for it.  You would not price a pr of Gaiter boots to fit, &amp; some simple things we cannot get, &amp; the Stores are so frequented by Greenville Loungers, it is disagreeable  to go in them &amp; the merchants are acquaintances , &amp; they talk &amp; press their goods on us, so it is very awkward to refuse.  The shopping [l]ine is more like disagreeable visiting in the City.  It is a business matter{&amp;} I am surprised Mr. Elford did not deliver my packages immediately.  He is more careless than I thought.  He is not as punctual &amp; exact in business as your Papa is.  Mr. Elford’s little daughter is not expected to live.  He has been written for &amp; may come back before he has time to let you know, before you can get ready to come.  If so I will let you know of the first opportunity I hear of.  It may be inconvenient for your Aunt to have you longer, &amp; I do not wish you to impose on her hospitality, so you must consult her wishes about lengthening your visit.  She has been very kind indeed to you, &amp; has afforded you a great pleasure by introducing you to your relations.  You cannot return her kindness [page torn] it deserves, but you must show your value of it, by making her some useful present.  You must get money from Mr. Elford &amp; pay for what I wrote for, &amp; also if you need any. [G]et at Klinckes a Jar of preserved Ginger &amp; give to your…in my name &amp; get a present for her Eloisa &amp; Susan.  If you buy the dress &amp; trimmings &amp; bring it home, Eliza can make it when she gets well.  A dress for 25 cts a yd as pretty as the blue Aunt Mary has got me at that price, &amp; which [pagetorn]  send a pattern of will do.  Beg Eliza to get me two belts to suit [page torn] patterns I send.  I will write to Aunt Eliza soon.  Tell her I [w]ould be gratified if she would write to your Papa about you.</t>
+  </si>
+  <si>
+    <t>EMP260_24_12_1852</t>
+  </si>
+  <si>
+    <t>Your affectionate mother</t>
+  </si>
+  <si>
+    <t>I have just written to your cousin Eliza &amp; will now write to you.  I expected you home this morning.  I heard Mr. Elford would be here.  Last night I heard a Stage as I thought stop at the gate.  The driver called out very loud, &amp; then blew his horn.  I thought you had come, &amp; woke your Papa &amp; he woke Charlotte.  By that time the horn sounded at a distance, &amp; I discovered it was the Augusta Stage that had passed.  This morning Mr. Hoke told your Papa, Mr. &amp; Mrs. Elford had arrived at 6 oclock.  Little Mary Elford died only a short time before.  She was at Mr. Perry Duncans.  Mr. Duncan sent in a servant to prepare Mr. &amp; Mrs. Elford for the sad event.  The servant passed them on the road, but they were afraid to inquire of him about the child, so rode on, &amp; knew not whether the child was alive or not until they got to Mr. Duncan’s &amp; found it dead.  It was something like Scarlet fever, for yesterday an irruption broke out.  Fanny Hoke has also been sick in the same way, but is getting better.  How many little children have died lately in Greenville.  It must be a warning to those who are left.  Mrs. Harvey has moved into the County.  Her two oldest children will stay in the village &amp; go to school.  Susan Hoke I see very often.  She sends her love.  She says she wrote to Augustus to go &amp; see you, but as you have not mentioned his visit, I suppose he has not been.  I am sorry Mr. Elford was hurried home so much sooner than he expected, &amp; that you did not come back with him.  Do inquire of Mary C…ton &amp; anyone else from Greenville who may be in town of some opportunity, &amp; let you know that you may return.  If you hear of none, in a little more than a week your Papa will go down for you.  He would set off at once, if it were not for some business that detains him at home.  I proposed that Willie should immediately go down for you, but your Papa said somebody would have to go to take care of Willie.  The  children are very much disappointed at not having their Christmas presents.  I have nothing to give them.  They will have to hang their Stockings after you come back.  I am sorry you are not here.  I put off making the Hogs feet into Jelly until you returned but now it is so warm I can wait no longer &amp; am making the Jelly today.  I am sorry also you have been obliged to stay so much longer than we intended you should, &amp; as your aunts house will soon be full, I feel uneasy at your putting her to inconvenience.  You must write to me every day until you return.  Do not forget the Candy &amp; Cocoa nut cake for the children.  I am getting nothing of the kind for their Christmas here.  I have sent Eliza 20 dollars, &amp; I have troubled her so much in shopping for me that except a…for Fanny, &amp; something for a S… or Cloak for her, &amp; a pair of Gaiter boots for me, &amp; a Prayer book for yourself, there is nothing more I wish at this time.  You know we pay our bills.  We have to contract during the year, at the Blacksmiths, Sadlers. Doctors &amp;c, buy meat Corn &amp;c, so I am more straightened than at any other time, or I would send for a great many things I need, &amp; I have also a large bill to pay Aunt Mary McCall 21 dollars for the Cloak, which is almost white, &amp; I never expect to wear, but I know she did the best for me, as she thought, &amp; therefore I do not wish to hurt her feelings, &amp; she has been kind to you, but it would have been better not to have got me my cloak.  The bonnet is too fashionable for Greenville, but I cannot dispose of it, so wear it.  If I had known there was so much difficulty in getting work done I would not have written to you to get a dress.  I am sorry I troubled your cousin so about work. Your friends have been kind to you, &amp; I am sure you will never forget it.  I hope to see you soon, &amp; to hear from you every day.  Frank says bring him some crackers, &amp; Willie &amp; himself a knife.  In haste.  Your affectionate mother  Mr. Hopkins &amp; his family have just passed on their way to Florida.  Fanny is regretting she did not see them, &amp; says she wishes Rosa had staid.  I think Fanny is almost crying.  She is now saying, “I want Anna.  I wish Anna would come.” The Silver Comb I want for Annie like yours.</t>
+  </si>
+  <si>
+    <t>EMP261_25_12_1852</t>
+  </si>
+  <si>
+    <t>Saturday afternoon</t>
+  </si>
+  <si>
+    <t>This is Christmas day, &amp; a very dull day it has been.  The weather continues very bad.  I never knew so long a spell of rainy warm weather in winter.  The streets &amp; yards are very muddy, &amp; the house looks as if it never could recover.  The Carpets I am afraid are ruined.  The roads must be dreadful.  Your Grandmama &amp; family were not able on account of the weather to come in &amp; spend the day with me.  I sent them some of our desert, as they could not come.  I let Becky have holiday, &amp; Lindy cooked.  Tomorrow Lindy will have holiday.  The pleasure seems to be all among the servants.  Last night some of them went to a party; today they have dined out, &amp; their having holiday seems to make them happy.  The children hung up their Stockings, so I was obliged to put something in.  I bought 5 cts worth of Candy apiece, a mug, a 5 cts doll, a cake, an apple, a switch &amp; 10 cts apiece.  So St Nicholas they think has not forgotten them.  Fanny regrets very much that you are not here.  I hope when you return we will have pleasant cheerful weather or you will think Greenville very dull.  Your Papa will go down for you.  He may not have time to go &amp; return before New Years day.  If he does not, he will go immediately after New Years Day &amp; that will be as soon as Mr. Springer thinks of coming.  So by New Years day have everything ready.  I dare say he will spend a few days in town though, so you will have time to get ready after he gets down.  I expect he will take Willie with him. Mary Elford was buried this morning.  I hope she has spent her Christmas in a happy world with Laura McKay, who was so afflicted, that I think it was a blessing she was taken, as her life would certainly have been one of suffering. Fanny Hoke is getting better.  Fanny sent her a doll &amp; she sent Fanny a box.  Susan Hoke told me she wrote to Augustus to go &amp; see you.  I suppose he feels awkward about visiting.  Butler Tompson told your Papa his Fathers wifes son, weighed 13 ½ pounds, &amp; his father was very proud of it. I am always writing you something to get, &amp; I expect as long as you remain in town it will be the case.  I wish you to get me a little key basket, &amp; 1 dozen black lacets for Gaiter boots.  The tines come off so soon, &amp; then ties cannot be laced.  Mr. Westfield puts such large tines on they will not go through the holes, &amp; then they cannot be laced, so buy one dozen black lacets for Gaiter boots. Some neat dark Calico about 12 ½  cts a yd such as will wash I also wish, &amp; will write for before you leave.  A good many yds I would like, but I will wait until I get Eliza’s next list.  Beg her to send me a list of the other things she has bought.  I know I will like the bonnet she has got, &amp; will wear it constantly.  I see in my list Calico is mentioned for A… the 1.37 ½ for the Calico if Eliza chooses &amp; the 1.12 ½ for Reedy House might be added to your money, &amp; pay for some of the things you have got. I am obliged to your Aunts for making you such acceptable presents as the Bible &amp; Prayer book, the very things you were going to buy.  Also to Aunt Eliza for the boxes &amp; Aunt Emily.  Your friends are very kind &amp; I am thankful for the good opinion they have of you.  I am greatly indebted to your cousin Eliza for all the trouble she has taken to shop for me.  I will never forget their kindness to you.  Aunt Mary McCall has been kind.  I hoped to have heard today from her about the Cloak but have not.  If the man will take it back, your Papa can carry it down, but I suppose he will not change it. Give my love to your Aunt &amp; cousins, Aunt Mary, Aunt Anna, Aunt Emily &amp; my other Aunts.  I wish you would see about Sarah Matthews &amp; Aunt Harriett but suppose you will not.  Give my love to cousin Sarah Gibbes, Mrs. Irvine Keith, Mrs. O’Driscoll, &amp; my other family.  Have you seen Elizabeth Jones? It is 10 oclock.  I can hardly see to write.  Hext is well &amp; fat &amp; lively &amp; good, better than he used to be.  Minerva is sick, over at the Mansion House, with cold &amp; headache.  The rest are well.  Lindy is still lame from Rheumatism, &amp; is not going at present to your Grandmama’s.  She has engaged Nancy Greens daughter.  While Lindy’s baby is young, I know she would not do well hired out.  She can hardly work but next summer, after her child can run about she will do better.  She is now only able to help the other servants.  I will stop now &amp; finish my letter after the candles are lit. Dear Anna, You had better buy the dolls not dressed &amp; dress them yourself.  I hope Aunt Harriett will come down from Mrs. Wilkes to see you if you are in town when she is there.  I am sorry you have not dined with your Aunts in Meeting St. but hope you will now.  We used to spend pleasant days with them when we were children.  I hope Alston will name his son after his father.  He lost one named Robert, but I think he ought to name another after his father, &amp; that it would please his Mother.  I am sorry Aunt Anna Turnbull &amp; Aunt Martha have gone in the country.  I hope you will see them again, &amp; that they will be in town when your Papa &amp; Willie go down.  Tuesday week I expect your Papa will go down for you.  Wednesday the day after he will stop at Newberry to attend a R[ail] Road meeting, Thursday he will go to Columbia, &amp; Friday reach Charleston.  He will remain there a few days.  It is very unexpected he is going down, but now he has determined to go, he is pleased with the trip, he is obliged to be back before the 15th Jany.  He would have gone down immediately, but all business men ought to be at home Sale Day, &amp; he could not return in time.  So you will soon see him, &amp; I expect Willie.  Write every day.</t>
+  </si>
+  <si>
+    <t>EMP262_28_12_1852</t>
+  </si>
+  <si>
+    <t>Tuesday morning, 10 oclock</t>
+  </si>
+  <si>
+    <t>I have just received a very pleasant letter from you.  Your friends are very kind to you, &amp; the enjoyment you now have, must last you a long time.  In looking back to it, you can experience it over again.  Uncle Arthur &amp; Aunt Elizabeth are kind.  The presents I will like to see.  You must get your cousin Eliza or Susan either to show you or how to finish the Mit, or to finish it for you.  As unfinished they will be useless, &amp; perhaps you can learn how to knit a purse with the ball of Silk.  I am glad you have seen H… Drayton.  You were right to speak to Miss Drayton, for she would have spoken to you if she had recognized you, &amp; if you had not spoken, you would have missed seeing H…, who is a fine girl, &amp; was kind to you in Greenville. &amp; I am sure would have been very sorry not to have seen you.  Did you tell her the fate of the China doll? She bought? &amp; dressed for you. Your dress I know is a pretty one, &amp; you will find it useful.  You have remained so much longer in town than you expected, that your other dresses perhaps look shabby, so this new one is made just at the right time.  I am sorry you did not take down your other Flannel petticoat.  I will send you by your Papa a new Sun bonnet I have just made for Fanny, but it is large enough for you &amp; send that blue silk apron I bought for myself at Cox &amp; Gowers but have not worn.  Perhaps it may be useful to you, the few days you remain after you receive it  If Aunt Mary McCall could have returned me the money for my Cloak, I would have written to Eliza to get me one, as I need a cloak very much, but situated as I now am, with Aunt Mary’s cloak on hand, &amp; not able to dispose of it. &amp; having bought so many other things &amp; a second bonnet I am not able to get another Cloak.  I hope Aunt Mary will be able to get the man to give me another Cloak this winter or next.  I am going to send it down to her.  When I first wrote to Eliza about another Cloak I thought I could dispose of the light one, but I have not been able to, so for the present I must hope Aunt Mary can do something with it. I know I will like the bonnet Eliza has got.  I am glad the box was about to be sent when you wrote.  There are a few things I wished Mr. Elford to get, which his leaving town so soon, may have prevented his attending to.  If so, when your Papa goes down I will send a list not a long one, a dozen large &amp; a dozen small knives without forks, for every day use, two peices of the cheapest Calico 4 or 5 cts a yd to make Comfortables,13 Stair case rods, are what Mr. Elford I expect has not got, &amp; a Fender,…dogs, Shovel &amp; Tongs, Broom &amp; Bellows for the Dining room.  These things if your Papa cannot get, I will be glad for Eliza to, &amp; I think she will be the best judge.  Send a list of all you have got since the last list sent.  My hair not being able to be made into chains, for a small one I wished made, for you to wear your Medallion with.  I think you need some kind of chain.  What kind would be suitable.  Ask Eliza, &amp; what is the price, write me, so I can tell your Papa, &amp; you can get one after he goes down.  I think the 12 ½ cts chain must look very unsuitable.  A pair of India rubber shoes you must get.  One thing I wish to know is the price of a nest of baskets, beginning from the largest Market basket to the key basket.  Ask Eliza to let me know the price, so if I can get a nest I will send by your Papa for it.  Mr. Elford was to have inquired for me. You can work on your quilt when you return.  I am glad you practice regularly on the Piano.  I hope you will play better than when you left.  I am also thankful you do not forget to perform your religious duties, &amp; that you have behaved so well as to gain the good opinion of your friends.  You must set a good example to the others when you return, &amp; try to be a comfort to us &amp; make us all happy by your good conduct. You are greatly indebted to Aunt Eliza as you may tell her, for it is through her kindness, you have been put in the way of receiving kindness from your other relations.  She so kindly invited you to visit her, which has given you so much enjoyment.  Willie is sorry now, he did not accept the invitation given him.  Now that he hears how pleasantly you have passed your time; he thought it would be like Columbia, where he has no acquaintances &amp; soon gets tired of, for there he is the whole time among grown persons, his Papa’s associates. &amp; such society improves him, so I am always well pleased to have him there.  Today Willie is not well, has a sore throat, which many are complaining of.  Mary has, &amp; Edward &amp; Mrs. Hoke.  Susan Hoke was here yesterday.  She said she is certain Augustus did not get her letter telling him to go &amp; see you, &amp; that he cannot know you are in town, or he certainly would go &amp; see you.  It has rained almost constantly since you have been away &amp; yesterday was the eighth day it rained without intermission, &amp; today it is not raining, but is still cloudy &amp; warm, &amp; not like clearing. If you do not know what to buy for the servants, I can tell you.  Becky’s comb &amp; a handkerchief apiece for the five women, two Bibles I am going to give to Reuben &amp; Charles two of those you have bought, a Bible to Eliza, for Eliza &amp; Lindy’s babies buy a little Worsted bonnet apiece for 25 cts, or 25 cts worth of Calico for the little servants any little thing, some Candy if you can think of nothing else.  One of the Bibles you have bought you can give to John Macbeth for the servants at Mamma’s, for Lucinda a handkerchief, for the little servants candy; Ninny a handkerchief or apron. Do not forget the Sugar dogs for Vardry &amp; the others.  When I know all you have bought, I can then see whether I can get some books or not.  I hope to be able to, but having to pay for Groceries &amp; Doctors &amp; other bills, I cannot ask for money at this time to buy many things I would like.  It is such a good opportunity, your being in town.  Give my kindest love to Aunt Eliza, &amp; your cousins &amp; thank them for taking such kind care of you.</t>
+  </si>
+  <si>
+    <t>EMP263_29_12_1852</t>
+  </si>
+  <si>
+    <t>I have been disappointed today at not hearing from you, but I suppose you have been so much engaged shopping or seeing your friends, you were not able to write by this Mail. Mr. Elford went to his office today for the first time since he returned.  He told your Papa he left orders with his brother to give you any money you wished, so I hope his brother has given you some.  If he has not, you can immediately send to him &amp; ask for whatever money Eliza needs to pay for the things she has bought for us.  I prefer her doing so to waiting until your Papa goes down, as I would like her to have the money at once.  I am glad to say that Mr. Elford bought all the things I requested him to, the Knives, Fender, Calico, &amp; even the nest of Baskets, so I will not have to trouble your cousin Eliza to get them for me.  She has shopped so much already for me, I am unwilling to occupy her time in that way, more than I can help. It is reported the Cholera is in Charleston, but I hope it is a mistake.  If it were so, you would have mentioned it, &amp; Augustus Hoke would have made it an excuse to come home. Willie took some pills last night, &amp; feels better today.  He has gone to the Farm to haul wood.  Franks only amusement is to cut wood.  Fanny is trying to make herself useful.  She has been pulling Sage, then asked what next she should do.  I told her to move Hexts carri[a]ge out of the front walk, then pick up towels lying about the yard.  Hext has gone to the Mansion House to ask for a bill of some Hams we got there this Fall. Yesterday after I wrote the wind blew, &amp; the Sun came out &amp; the weather became fine, &amp; continues so.  I hope it is the same with you, &amp; that you will have pleasant weather the remainder of your stay in town. This afternoon if I can, I will go &amp; see your Grandmama.  She is interested in all you write about, &amp; pleased her friends have been so kind to you &amp; that you are so affectionate in your remembrances of her, &amp; forget no one at home. This visit to town is an Era in your Life.  I am sure you will never forget it, or the kindness of your friends.  I suppose you were surprised at finding how many relations you had there.  I hope you have dined with your Aunts in Meeting st.  I can imagine you spending a quiet, pleasant, improving day, seated in Aunt Mary’s chamber, working on your Quilt.  Are Mom Phillis &amp; Minda still alive? Christmas has not been spent differently from any other time, except among the servants.  Mrs. Choices servants had dancing even in the day &amp; a party takes place every evening I believe somewhere.  Even Becky last night asked to go to a Fair all the way at Mr. Goodletts.  I objected on account of the distance, for fear she would get sick. Baylis then came in to say he had procured a Buggy &amp; intended to drive her there, &amp; would come back soon, so I let her go.  Johnny came in for a ticket for Clara to go, said two gentlemen had come to escort her.  The two gentlemen were Genl Thompsons servants,  Tonight Dr. Irvines servants give a party, &amp; Charlotte asked to go, &amp; Clara wishes to have a Fair in this yard. The Mauldins yesterday inquired of your Papa when you would return.  He met them in the streets. The Piano has not been opened (except by Mr. Wardell) since you left.  You must buy a few pretty peices of Music, simple enough for you to learn. Give my love to Aunt Eliza, Eliza &amp; Sue, &amp; beg them to write to me, &amp; Eliza to send a list of her further purchases, my bonnet, Fannys &amp;c.  I would like to see it, &amp; a list of the Confectionary &amp; toys.  I will open the box when it comes &amp; take out the bonnet &amp; such things, but the presents I will not take out or show the children until you return.  I hope the box will come soon.  The Rail Road being unfinished, our Groceries will come up by way of Hamburg.  The roads are so bad the freight by wagons is very high now, so we are sorry now we did not wait until Spring to get the Groceries, but often we cannot get even necessaries here, such as Rice &amp; Salt.  At present no Salt can be got in the village.  Many persons have to keep the Hogs they have bought &amp; feed them, until they can get Salt.  Genl Thompson is complaining of having to feed his hogs, on this account, says they are eating him out of everything.  It is near dinner time, so I must soon close.  I hope you spent a pleasant day with Miss Drayton.  In this fair weather it must be pleasant walking on the Battery. I hope to hear tomorrow from you.  Give my love to Aunt Mary, Aunt Anna, Aunt Emily, &amp; Aunt Elizabeth, &amp; my friends generally. I hope you will see Aunt Anna &amp; Aunt Martha again.  I suppose you will not see Aunt Sarah &amp; Aunt Harriet.  I am sorry you will not, &amp; also Aunt Susan.  Thank Aunt Eliza &amp; your cousins for their kindness to you, for which I feel very grateful, &amp; believe me , Your affectionate Mother, E.F.P. P.S. I hope your cousin Eliza received the letter containing 20 dollars I sent last week.</t>
+  </si>
+  <si>
+    <t>I have just written to Aunt Eliza to say, you may remain longer in town, that my only fear was, you would put her to inconvenience. &amp; be in the way, when the family became larger, but as she says this is not the case, &amp; you are passing your time so pleasantly, &amp; are anxious to remain longer, we have no objection at all to your remaining, &amp; coming up with Mary Crayton, if she does not stay longer in town, than you think you ought to stay.  Your Papa is better today, but will not be able at present to fix upon any time to go for you, &amp; if you come up with Mary Crayton, or any other lady coming, he will not go down, as the traveling is too unpleasant at this season to visit town for pleasure.  We leave it to you now &amp; your Aunt to return, at a suitable time.  Of course I would not object to your lengthening your visit, except that I thought you were trespassing on your Aunt’s hospitality, which she says is not the case.  I am very much pleased with the accounts Aunt Eliza &amp; your cousin Eliza give of you, they say you have pleased all your friends, behaved exceedingly well, &amp; have all the virtues that adorn the female character.  I hope you will improve as you grow older, &amp; not disappoint your friends, &amp; be a comfort to all those kind friends, who are interested in you, &amp; set a good example to Fanny.  The character of the oldest sister has great influence over the others, &amp; therefore a great responsibility rests on you.  I am glad you perform all of your duties so regularly &amp; do not forget the most important, the religious one, you must keep yourself very neat, clean your teeth regularly, wash your hands, face, ears clean your nails, &amp; be very nice in person, you know cleanliness is a virtue placed very high in the bible.  I see in the paper Charcoal recommended as the best tooth powder, buy a box &amp; use it every morning.  If I cannot get any here, I will get you to buy some for me.  I do not need the key basket now.  Mr. Elford has bought a nest, which I suppose includes the…for keys, so if you have not got it already, you need not. I much prefer Fanny’s cloak being made.  I countermanded the order thinking it could not be done conveniently, but Eliza has engaged the mantua maker, &amp; says it can be done.  I will be very glad to have it made, &amp; of a large size, as the winter is so far advanced it will be more useful next winter than this. Tell Eliza by Butler Thompson I will send down a Gaiter boot, so she can know exactly the kind I wish, &amp; I may write for a pr of India rubber shoes, &amp; she can put them over the Gaiter. Mamma asks Eliza with the money she has of hers to spend 2.25 or about that, for a Silver spoon for Sarah Taft’s child.  It is named after Mamma, Susan Hayne McCall Taft.  She wishes the four Initials marked on the spoon S.H.M.T.  Eliza will know what kind of spoon will be suitable. I am glad you spend Christmas so pleasantly, &amp; am sorry as you were, that you could not have been at Mr. Wm Ravenel’s where I suppose the tree was beautiful. But it was kind in Mrs. Drayton to ask you. I am pleased you remembered your Aunt &amp; cousins with a little present.  If I had not a large debt to pay to Aunt Mary McCall, I would send you money to make them handsome presents.  Minerva’s wages are due in two weeks &amp; the whole of it I have to send to Aunt Mary &amp; more besides, &amp; what is mortifying, the Cloak is useless, &amp; the bonnet almost so.  I have worn it once only, &amp; am sorry I wore it then, as Eliza has got me one I know I will like better, &amp; Aunt Mary’s, perhaps I might have disposed of it at a low price, or kept it for you to wear at a future time, taking out the feather.  But Aunt Mary meant to please me, but Ella being so much smaller than I am, if she had thought about it, she would have known the bonnet was too small for me.  She has been kind to you, &amp; I am grateful to her, &amp; will not let her know my disappointment. Ask Eliza the price of her cloak, materials &amp; mating.  I can better judge by the estimate she sent me, &amp; wish to know what just such a one as hers costs.  I will be sure to get one, perhaps just like hers next winter.  Mrs. Robinson, Mrs. Thompsons Aunt says she will take down mine, next week.  I will direct it to Aunt Eliza &amp; get her to send it to Aunt Mary.  Perhaps I may send you a sun bonnet, apron, and flannel petticoat.  You may have use for them as you are to stay longer &amp; I will send you my gold chain to wear with your medallion when you take tea out, as I think you have nothing suitable to wear with it.  I see Eliza bought you two Collars 12 ½ apiece.  If you need it, get some more, &amp; if Eliza thinks you need undersleeves, buy or make some.  Tell Eliza anything you really need, I wish her to get for you, if she can get it with convenience. I have written word you may get a wicker box.  If you can get one, you will find useful for every day use.  Generally they are only for show, &amp; the scissors, thimble &amp;c in them only for ornament.  Perhaps you can get one without thimble scissors &amp; buy for it all that is needed, but consult with Eliza, &amp; beg her to get you a useful one.  Another Christmas I will get you a Writing desk, as you must keep up a correspondence with the relations who have been so kind to you, &amp; will need a desk.  Inquire the price &amp; let me know of a neat writing desk. &amp; when you get the…box, tell me the price. You must continue to behave well as you have done, &amp; not make your Aunt regret having to ask you to stay longer.  She is very kind to you.  Give my love to all my Aunts.  I will let you know when the box comes.</t>
+  </si>
+  <si>
+    <t>EMP264_31_12_1852</t>
+  </si>
+  <si>
+    <t>EMP265_00_12_1852</t>
+  </si>
+  <si>
+    <t>I have just written two letters one to your Papa the other to Mr. Elford on business, &amp; will write to you now.  My pen is bent, so I cannot write well.  I suppose you have seen Mr. Elford before this.  If he stays longer in town than you wish, or ought to stay, you can come up by any other opportunity you hear of.  He told me he might be only 10 days in town, but perhaps 3 weeks, so I thought he &amp; his Wife would be the very best persons you could come up with, &amp; the Stage at the time he comes, will not be so crowded, as at the time the Legislature adjourns. I received a long letter from you today.  I was glad to hear from you.  I am sorry your Cloak had not been made, as you must have needed it, ever since you have been in town.  I am sorry you did not mention the price of the things you bought.  I your next letter you must.  As you have written to your Papa for money I do not like you to write a second time for me so unless you have money left, I may not send for the articles I wish until he returns home, &amp; then I will send the money.  I thought you would need more than 10 dollars.  He says you wrote for 10.  You write me if you have any money left, &amp; then I can tell you what to get, but first get all you need, a dress frock for Fanny &amp; a cloak for her, are what I would first get, after you have supplied yourself, a pr of gaiters for yourself, myself, Fanny &amp; Hext I wish, such as your cousin Eliza wears.  The price of a bonnet for Fanny, I would like to know.  The Candy if you do not write in time for, you can get as much as you think best.  Buy a pretty pair of Ear[r]ings, for yourself.  Eliza had best write the list of your purchases.  If you need more money send to your Papa.  He will send it to you, &amp; I dare say you will need it.  I do not care to send to him for money for myself, but I wish you to get for yourself all you need.  I can do without the things I intended sending for, for Aunt Maery McCall has got me what I most needed. I am glad you are enjoying yourself, &amp; that your friends are so kind to you.  Remember me to them all.  I send you a little book to read  that your Aunt Eliza gave you.  I read it this morning to Fanny, &amp; it contains just such advice as I would like to give you now, but I am obliged to stop, for since beginning this letter I have received by Mr. Beattie two letters from your Papa.  I had written to him &amp; told him I had not heard, &amp; now I must write again, which makes me shorten your letter.  I write so badly.  You must tell Aunt Eliza &amp; your Cousins what I say, &amp; can read aloud parts but do not show them the letters, for I am ashamed of them.  Beg Aunt Eliza to write to me. Willie Frank &amp; Fanny &amp; Hext will all be glad to see you again, also your Grandmama Aunts Papa &amp; myself.</t>
+  </si>
+  <si>
+    <t>EMP266_00_12_1852</t>
+  </si>
+  <si>
+    <t>I do not know that I can get a cloak this winter.  I hope Aunt Mary’s can be changed.  If not I expect I will have to do without, as I cannot afford another, unless one could be got reasonable, so tell Eliza merely to let me know the prices.  I will then let her know. If she has not got the second dress for Fanny, I expect one will be enough, for Aunt Mary’s bill is high.  Until I have paid for that, I find I must be economical.  Your dress I can have made here. &amp; materials for a S… for Fanny &amp; a pattern will be sufficient. You will be so well supplied with clothes you will need nothing next winter. If I had known Aunt Mary’s bonnet I could wear at all I would not have sent for another, but it is very small.  Next summer I will have a peice added between the crown &amp; front, &amp; cover it over with ribbon &amp; wear it as a summer bonnet, &amp; make up for my extravagance in get[t]ing two, but the one Eliza has got will be very useful. Thank Aunt Eliza for her letter.  I write now in great haste, &amp; when I have leisure I will write to her.  I am glad you pleased Mrs. O’Driscoll by your playing, &amp; that your friends are satisfied &amp; pleased with you.  I am sorry you have missed seeing so many.  The Spring is the pleasantest time for a visit. Tell Eliza I will not trouble her with shopping for a long time again, &amp; when the Rail Road is finished I hope once in a while we can go down &amp; shop for ourselves &amp; not trouble our friends so often. The most economical way is not to send at all, but go without what we cannot get here, for when I once begin a list, I do not know where to end it. The weather is again bad.  You have had nearly 3 days together clear.  I am thankful that you have a happy contented disposition, &amp; it is well , as you know in Greenville our happiness has to be found at home.  There is nothing beyond home to amuse &amp; divert.  Everyone complains of the want of society, &amp; the little sociability there is now, that there is less than there used to be. Give my love to all my friends, particularly those in the house with you Mr. Elford ought to have been to see you.  I suppose he was busy.</t>
+  </si>
+  <si>
+    <t>EMP267_1852</t>
+  </si>
+  <si>
+    <t>Today has been so unfavorable, that we did not go to church.  I have just done reading to the children, so will now write you a few lines.  One important matter I nearly forgot mentioning to you.  When you are away the servants have so much…to do, I thought this a good time to purchase their summer clothes, for them to make up, so the money you left, I first bought some necessaries, &amp; the remainder spent in Homespun for servants, but it was not enough to pay for all.  Would you be so good as to send me by Mr. Elford 10 dollars, to finish paying for the Homespun &amp; to carry me on in Housekeeping.  It will be more than is necessary but you had better send that sum.  I have to pay Mom Phillis 2 dollars for being with Lindy.  I hope Mr. Keith will settle with you &amp; pay you for all the cases you have been engaged in with him.  In writing your Editorial from Pickens, do not mention Mr. Easley’s name in connexion with the case you have against him, as his family are respectable, you must have some regard for their feelings.  If Miss Wynn were modest, she would now keep herself secluded &amp; not wish to bring herself into public notice, as she is by bringing suit.  She is sufficiently disgraced &amp; if a trial comes on, I am afraid other acts of indecency will be brought forward against her. So instead of vindicating her fair fame, she will establish its infamy.  Her father perhaps does not know how bad she is.  Like Mrs. Rabe Dr. Rabe before her trial did not know half of what was brought against her. Lindy &amp; her baby are doing well.  Write me a long letter by Mr. Elford. The Patriot in which you mentioned Scurry’s case you ought to send to Belton Williams friends,, mother, Uncles, , &amp; cousin.  I think it a shame Scurry should be acquitted.  It was almost deliberate murder.  Massey certainly then ought not to have been hung, &amp; I hope Mr. Wiliams will still pay you the additional fee.  I am afraid the…spirit will pass over.  Mrs. Earle across the river, told Mamma she heard Mr. Sharpe was losing his property fast.  When will you be paid for Mr. Barnes Rail Road Case.  You will have been longer from home now than sometimes when you go to Columbia, &amp; a Call was bad to have during Court week at Anderson.  Many are at Court, who would wish to attend. Good bye.  We all long to see you.</t>
+  </si>
+  <si>
+    <t>EMP268_1852</t>
+  </si>
+  <si>
+    <t>Write by Mr. Elford,</t>
+  </si>
+  <si>
+    <t>Tonight Reuben said that Kossuth ploughed well, &amp; that that good quality ought to be mentioned in the advertisement.  I do not know what kind of advertisement Mr. Elford has written, but perhaps you had better write such a one as you would wish, &amp; give it to Mr. Elford to put in next weeks paper, for someone then may buy him to use on their farm to plough.  He certainly is fit for nothing else, though perhaps some person who understands breaking a horse, may in time break him, but I very much doubt it, for he seems by nature to be a[n] obstinate bad horse, &amp; I cannot understood how Mr. Redwood can be a truthful man, &amp; at the same time say, Kossuth was a good Buggy horse.  I am truly thankful you are going to sell him.  I have not had a comfortable ride since you owned him.  Selim &amp; Hocky  will do to draw together, until you sell Selim &amp; get a fine pair.  Perhaps H…’s…you can buy &amp; use with him, but I would rather be without horses, than have such a one as Kossuth.  He is not worth his food.  Goodnight. </t>
+  </si>
+  <si>
+    <t>EMP269_1852</t>
+  </si>
+  <si>
+    <t>Tuesday, 1/2 past 9</t>
+  </si>
+  <si>
+    <t>Your sympathizing Wife,</t>
+  </si>
+  <si>
+    <t>I have just received your letter mentioning your sad accident.  Mr. Beattie a short time previous had come to show me a letter from Mr. McKay who merely mentioned you had broken your arm at 10 oclock Monday morning &amp; were doing comfortably well.  Mr. Beattie was afraid I might hear exaggerated accounts.  I was very much shocked &amp; grieved , but was thankful it was not fever you had.  But I am afraid this accident may bring on fever, that you ought to come home at once.  Mr. Elford has just been here, &amp; offered to send his carri[a]ge for you, &amp; I have accepted the offer, so hope to see you tomorrow.  I have almost a mind to go in the carri[a]ge but am afraid you may not like it.  I am thankful it is your left arm, but truly sorry, it has occurred at all.  Edward Dr. Crooks said this morning was better that he regarded him now out of danger.  The symptoms at present were all favorable.  I was just going to write you about the Election when Mr. Beattie came.   I am sorry as yet the news is not encouraging.  The voting has been so strange that almost any result may be looked for.  Pinckney McBee is ahead.  Mr. Carson has managed wonderfully.  Mr. Ware thinks you next, but the Disunionist thinks Smith &amp; Irvine ahead of you.  John Russell has been run by them in opposition to Col. Brockman.  Until the boxes are heard from today, there is no telling what the result will be.  I would send Willie out but Mr. Elford thinks it a risk for him to go, as his tongue you know is…, &amp; he had a little headache night before last.  I believe I would certainly go, but he says it would be unsafe also for me. Be sure &amp; come home tomorrow.  I will ride &amp; meet you if nothing prevents.  Laurens is sickly &amp; with your accident, you will be sure to get fever if you stay there, so I will expect you certainly tomorrow.  Reuben will go any time in the stage &amp; bring the horse &amp; Buggy I am sorry the horse was foundered; how careless in the Ostler. I long to see you &amp; help nurse your arm.  I think I will have to go on your next tour with you.  I can write for you.  I will leave Hext, be a good time to wean him.  Susan will take care of the house &amp; children.  I hope you are doing well, &amp; will be at home tomorrow evening.  Your sympathizing Wife, E.F.P. P.S. The carri[a]ge will soon be here to take this letter, so I must seal it.  How kind in Mr. Elford.  Mr. Hoke says his being beat this time will do him good, make him popular hereafter.  Tomorrow I hope to see you.  Last night I dreamt of you, but was awake almost the whole night.  I must have had a presentiment of some evil.  I was crying &amp; begging you not to go where you would get fever.</t>
+  </si>
+  <si>
+    <t>EMP270_1852</t>
+  </si>
+  <si>
+    <t> Mr. Elford called here little while ago, to say he was going to Anderson tomorrow &amp; would take a letter, so I will write a few lines. Yesterday I had a very bad headache, owing to the trouble &amp; fatigue I had had with the children who were here Saturday.  I am so unaccustomed to have my quiet disturbed, that having even one person stay in the house any time, fatigues me, so that I feel the effects for several days after, so in future I intend to trouble myself very little about company, only your friends to stay one night at a time I am willing to have. I am glad you have decided at last about Kossuth.  He is too bad a horse to be at the expense of feeding.  I sent word to Mr. Elford to advertise him, horse saddle &amp; all you bought.  The bridle which is broken, I will have mended.  I will be delighted to have the 145 dollars back in your pocket as soon as you sell Selim, &amp; the first fine pr of horses you come across buy. Mr. Ward came here today to see you to know if you had heard from Mr. Harrison about his Land case. A letter came from the office today from Mr. Gordon, begging you to cash his bond as you had proposed, that he had written to you at Columbia about it, but supposes the letter miscarried. If Mr. Elford can take your brush which by mistake I left out, I will send it to you. Write by Mr. Elford.  Your letters are always a comfort to me, &amp; break in upon my loneliness. Stop to see Mrs. Dub….  I hope Mr. Keith will settle with you, &amp; pay you some large fees.  It is time to have a settlement.  We are all well.  I have nothing new to write you, take care of yourself, particularly in the fever country you pass through &amp; believe me, Yours truly &amp; affectionately, E.F.P. P.S. I do not mean that I intend to give up all company for the children, but when they wish it, it will be one or two at a time to spend the day &amp; when they wish a larger number it must be in the evening. I love to have my house to myself.  It is a privilege to be alone.  A boarding house is the last thing I would keep.</t>
+  </si>
+  <si>
+    <t>EMP271_1852</t>
+  </si>
+  <si>
+    <t>I am sorry you have such bad weather in Columbia.  You will find it duller than at home.  I hope you are behaving well.  You must write what purchases you make.  I sent the Book marks to Mary Mauldin &amp; Mrs. Hopkins &amp; they each sent word, they were very much pleased with them.  Mrs. Hopkins said she must look for something for you.  The pincushion Mrs. Hoke gave you &amp; you intended giving to Aunt Harriet McCall, you had better not give to her, as it would be making a difference between her &amp; your other Aunts, which would not be right.  You can give it to someone else, Sally Martin perhaps.  I would rather you get a Cloak, a nice one to wear to church, in preference to anything else.  Get the Cloak first &amp; then what else you need afterwards.  Aunt Mary McCall wrote me word she had got a Cloak for herself in New York, where she was the past summer, &amp; I have written to her to get me a Cloak.  Mr. McKay is going down next week &amp; will bring it up. I hope you have given your Papa no trouble.  You must not interfere with his business.  Let him attend to that, even if you are left alone the whole day.  Tell Aunt Harriet when you see her, that I have not forgotten her Pincushion &amp; needle…&amp; as soon as I can get a pretty pattern will make them. Aunt Eliza wrote word that Mrs. Isaac Hayne &amp; Eloisa Martin being in Columbia would make their social circle much smaller than usual, but there were many who would take a kind interest in you &amp; she would carry you to see all of our friends. In a City you must remember persons are more particular than in the County, &amp; as your good behaviour will reflect credit on your Parents, you must keep that in mind &amp; acquit yourself well.  I do not wish you to be grave &amp; restrained.  Be lively &amp; happy, but be correct in all your words &amp; actions.  As soon as you get down, have your patches cut out, so you can have some employment.  Aunt Mary or Aunt Eliza or Eliza or Sue will cut them for you.  Practice every day on the Piano.  Read your Prayer book &amp; say your Prayers, begin your day well, &amp; it will be apt to end well. I will now close.  Hext is asleep in the cradle.  Fanny is busy fixing something in the Entry.  Willie I expect is in the Library, &amp; I do not know where Frank is.</t>
+  </si>
+  <si>
+    <t>EMP272_01_01_1853</t>
+  </si>
+  <si>
+    <t>I have just received a letter from you, &amp; am very glad to hear.  When nothing prevents it, you must write every day, but do not let writing to me interfere with any other engagement.  I write to you every day, because I hope my letters give you the same pleasure yours do me. I am glad to tell you your Papa feels much better today, &amp; has gone to his office, but he will not be well enough to go to Newberry to attend the R[ail] Road meeting Wednesday.  I wrote to Aunt Eliza &amp; yourself yesterday, to say I was perfectly willing you should remain longer in town, even if you wished it, as long as Mary Crayton staid, as she so decidedly said, your being with her was a pleasure, &amp; you did not incommode her at all, even if her family were larger, it was no inconvenience to her, to have you.  But if at any time you feel anxious to return before Mary Crayton does, write &amp; tell me so, &amp; your Papa I dare say, by that time will be well, &amp; he will go down for you.  Now that you are to stay longer, continue to be as good a girl as you have been, &amp; your friends will be more &amp; more attached to you.  Occupy yourself practicing &amp; working &amp; reading &amp; make yourself useful in every way you can to Aunt Eliza &amp; your cousins.  Perhaps you can learn some new peices of Music to surprise me when you return.  If it gives no trouble, get one of your friends to teach you to knit a purse, &amp; finish the Mit, &amp; when Aunt Ann &amp; Aunt Martha return, go &amp; see them frequently, &amp; Aunt … &amp; Aunt Anna go &amp; see, &amp; Aunt Harriet I hope you will see before you leave.  I know she would be sorry not to see you.  You are passing your time so pleasantly, &amp; seeing so much that is new to you. &amp; seemed anxious to remain, that I am sure you will be pleased that your Papa &amp; myself are willing you should. Soon I am to send 49 dollars to Aunt Mary McCall, 21 for the Cloak &amp; 7.50 for the bonnet, making $28.50 which is spent uselessly, &amp; I would gladly have sent to you,  The rest of the money is for two dresses &amp; trimmings, as pr velvet Cuffs, a peice of ribbon for the neck, a pr Gloves &amp; a blue veil.  This is all.  Next week I will send you more money.  Write word how much you wish.  As soon as you get your work box, write about it, &amp; tell me the price.  I think it will be a very suitable present to make Aunt Eliza.  So after I hear about yours, perhaps I may write to you to get her one, but do not say anything about it, until you buy it &amp; surprise her.  Inquire the prices of neat writing desks; either a writing desk or work box, whichever she most needs will be a good present for your Aunt.  I am glad you gave the Jar of Ginger &amp; the other presents. Day after tomorrow is Sale day, &amp; your Papa will receive money, &amp; I will be able to send you all you need.  This week he has been paying some of his debts.  Three Doctors bills Dr. Crooks 58 dollars, Dr. Earle 24, &amp; Dr. Dean 22,  Cox &amp; Gower 189 dollars for the carri[a]ge &amp; repairs on Buggy &amp;c, Mr. Westfield 44 dollars, &amp; Mr. Heldman 54.  For the Hogs Mr. Hoke bought 10 of them, he paid 140 dollars.  It is pleasant when one goes to town &amp; sees so many things they need &amp; cannot get here, to have plenty of money; your Papa paying his debts, &amp; I also having to pay a large debt, prevents my giving you as much as I would like, but when you make another visit to town, instead of having to send 49 dollars to pay for what is of no use to me, I can give it all to you, &amp; you can gratify your feelings, of generosity, &amp; buy presents for all who have been so kind to you.  I am well supplied with clothes for next summer, &amp; can save all of Minerva’s wages for the next visit any of us pay to town. You can buy for Mary Mauldin a little China cup or basket for 28 cts, also for Sally Hoke , a Sugar figure for Fanny Hoke she will be pleased with; more ground nut cake &amp; Candy I will send money for as presents to the children here.  I will not show them the presents in the box if possibly can help it. Mr. McKays school begins Monday. &amp; we expect Fanny will commence at once.  She says she does not wish to go, but I know she will be pleased.  She will be occupied, which will make her happy as it does everybody.  Sometimes she prefers going to Miss Hopkins, &amp; then again to Mr. McKay.  We prefer sending her to the latter, so as to be with you.  In the Male Academy, Mr. Thomas a young man who graduated the other day in Columbia &amp; took the third honor, is to teach.  We will send Frank to him.  Perhaps Mr. Hillhouse will also be engaged in the Male Academy.  Willie will go to the Baptist College, which does not commence until February.  Mamma let Reitta go home, &amp; engaged old Mrs. Greens servant Sarah to go to her today. &amp; Sarah has disappointed her &amp; says she cannot go yet, so I was obliged to let Lindy go.  The yard is so much pleasanter now, since Becky was here, that Lindy is very sorry to go.  I expect she feels she is not able to do as well for Mamma as she ought, for she went off wiping her eyes.  She had her child in her arms.  Priscilla who is to mind it, following with a basket &amp; escorted by Fanny, &amp; Charlotte &amp; Hext.  On account of the Measles being at Mamma’s, this is the first time Hext has been there since you left.  I told Lindy to do her best, for we were obliged to hire her out, as we had too many servants, &amp; they must make something for us.  Though I did not intend to hire her out until her child was older, only to accommodate Mamma &amp; let her go now, &amp; if she did well it would be a good place for her. Tonight the servants here give a party.  Becky I believe is the one, &amp; as she is a Methodist, it will be quiet, no dancing or noise.  There is to be a show here next week of animals &amp; a Circus which the children are expecting with great pleasure.  I am glad Eliza is having Fanny’s cloak made.  Beg her to send it up by the first opportunity, either Butler Thompson or anyone Mary Crayton knows is coming. Give my love to Aunt Eliza &amp; your cousins.  I am pleased at the high opinion they have of you, &amp; hope you will continue to merit it.  Write me everything that interests you.  I write so often, Willie thinks it no use for him to write.  Mrs. Robinson &amp; Butler Thompson go down next week, &amp; today I am going to pack my Cloak to be ready for her to carry, &amp; if she can take them, your bonnet, apron, &amp; flannel petticoat.  I must now close.</t>
+  </si>
+  <si>
+    <t>EMP273_03_01_1853</t>
+  </si>
+  <si>
+    <t>No mail comes today so I have not heard from you, but I cannot let the day pass without writing to you.  We again have bad weather.  Last week was tolerably good, &amp; yesterday we were able to go to church, but this morning after breakfast it commenced raining &amp; has now set in for a bad day. Willie &amp; Frank &amp; Fanny all set off for school today.  Fanny went to Mr. McKay, but the day being bad only the Brooks, two of them &amp; Rebecca Croft &amp; Harriet Crooks were there. So Mr. McKay said school would not commence until Wednesday, for tomorrow a snow is expected to be here. As the Baptist college does not commence until February we sent Willie to the Male Academy with Frank, but that school does not commence until Monday.  If we like it, Willie can continue there, but if he does not improve, we will send him to the college when it commences. Mr. Hillhouse keeps school in Dr. Irvines building back of the Baptist church.  Mr. Gailliard I believe is not going to keep school. Today I intended sending or carrying my box with my Cloak to Mrs. Robinson to take to town for me, &amp; I have enclosed in a letter to you, my gold chain, for you to wear with your Medallion, when you take tea out, &amp; a gold pencil case I bought once for myself, but it was too large for a lady, &amp; I have never used it.  I send it, that you may make it a present to your cousin William Edward from yourself, as a proof that you feel grateful for the kindness he has shown you, since you have been under his Mothers roof.  If he has no gold pencil case. Give it to him. but if he has one, this will be of no use to him, so I will think of something else for you to give.  I will write you about giving Aunt Eliza a present, &amp; also Eliza &amp; Susan.  I will send the letter enclosing the pencil case &amp; chain by Butler Thompson, who carries down Mrs. Robinson or by anyone I can hear of going before.  I hope I can send it soon.  I will tomorrow, if the weather permits go up to Mrs. Thompsons to carry the box &amp; letter, &amp; inquire when Mrs. Robinson goes. I hope you are satisfied &amp; not disappointed your Papa is not going down as he first intended.  His being sick, &amp; Aunt Eliza, Eliza, &amp; yourself all writing to ask you should stay, I have written &amp; suppose you have received the letters, saying you might.  I hope your longer stay will enable you to see those friends, who have been in the country, &amp; perhaps returned by this time.  What do your friends think of the Daguerreotype?  Do they think yours a good likeness?  None of the others did justice. I would be very glad if you would learn to embroider&amp; embroider clothes for yourself, &amp; Fanny, Hext &amp; your Aunt Susy’s children.  If not too hard you must learn.  I wish you could learn as you grow older every kind of work, like your cousins Eliza &amp; Susan.  It makes you so useful, &amp; happy, &amp; it is such a resource &amp; makes the time up pleasantly.  I hope in time you will knit, Crochet, embroider, &amp; do every kind of work, so if convenient, commence now, &amp; learn as much as you can while in town.  If it does not give your cousins trouble to teach you, you are so quick in everything I think you can learn easily. You will be perfect in playing your peices on the Piano, practicing them so much, perhaps you will learn a new peice. I am afraid the box will not come for a long time.  A box your Papa packed in Columbia when he was there, has not come yet.  The bad roads cause delays.  You will have to hang up a bag for Fanny, if you expect the box of furniture to surprise her.  A stocking would be too small. Your Papa is getting a great deal better.  Give my love to Aunt Eliza, Eliza &amp; Susan, &amp; thank them again for being so kind to you.    I am glad you were able to visit alone.  You will learn to be independent. Annie slept here night before last, but she would go home yesterday, or I would have kept her longer.  None of your Grandmama’s family were able to come in to church yesterday.  Your affectionate Mother, E.F.P. I sent you 8 stamps.</t>
+  </si>
+  <si>
+    <t>EMP275_05_01_1853</t>
+  </si>
+  <si>
+    <t>Wednesday morning, 11 oclock</t>
+  </si>
+  <si>
+    <t>I have been disappointed today in not hearing from you, but suppose you were prevented writing by some engagement, &amp; as I have said before, I never wish you to write to me when anything occurs to make it inconvenient.  I received two letters from you yesterday.  I wrote to Eliza &amp; Aunt Mary McCall, which left me no time to write to you.  I sent Aunt Mary 49 dollars to pay my bill, which I am very glad she will soon receive.  I disliked being in debt to her so long.  If your Papa comes in before I close this letter, I will get some money from him &amp; send it to you.  I would send to his office, but persons are generally there &amp; he dislikes being interrupted by messages.  If I do not send the money today, I will tomorrow. I am glad you are still enjoying yourself.  Miss Drayton has been very kind to you.  I suppose you know the Fords are cousins of yours.  You have so many relations, you might stay in town a long time, before you found them all over.  The patterns of your Cloak &amp; dress are beautiful.  The dress much prettier than the blue one Aunt Mary sent me. &amp; well worth 64 cts more a yard.  A Cloak as dark as yours would have just suited me.  I am very anxious to receive Fanny’s.  She has not been to church yet, for she has nothing to wear [&amp;] if the box does not come soon, I will have to buy her a dress here.  The Cloak I hope will come by some private opportunity.  My Cloak Aunt Mary will change for a black Cape, about one yard deep, which she says will be very comfortable.  I can wear it this winter for dress, &amp; next winter I hope get a handsome cloak.  As soon as the box arrives I will let you know.  The bad roads will delay it for a long time.  Our Groceries I dare say will not be here for weeks or months. Fanny went to school today.  Willie &amp; Frank will go Monday.  Mr. Rosemond has commenced building the new kitchen.  It is to be joined to the old one, &amp; have four rooms, two below for a kitchen &amp; ironing room, &amp; two above for chambers.  The kitchen we have been working in so long, will be a general sitting room for the servants, so our kitchen can be kept clean, &amp; the Cellar will be kept as a Lumber room. Lindy is still over at Mamma’s &amp; Sarah Green is not a good servant, so your Grandmama hears, &amp; I expect she will be obliged to keep Lindy.  Susy has the Measles.  I would be very sorry for Lindy’s baby to take it, but it must now take its chance; for I am obliged to let Lindy stay there, Mama having ho servant to cook.  R… is hired to Mrs. Charles Roberts.  There was a Circus here yesterday, &amp; an animal show.  The two shows connected together.  The children went &amp; were delighted.  More ladies must have been at it, than I have ever known before from what the children say, &amp; I hear Ministers even were there, Mr. Buist &amp; Mr. Mims.  The say it was an uncommonly good performance.  I saw nothing of it.  The band did not [page torn] down the street as they generally do. Your Aunt Annie is as poorly as ever, &amp; as much opposed to your Aunt Susy &amp; the children being there.  I do not know anyone more dreadfully situated than your Grandmama.  The walking being so bad, &amp; the horses all the time hauling wood.  I have been there very little, &amp; your Grandmama scarcely ever can have her horses, as they are all the time hauling wood, &amp; Aunt Annie does not like her to leave her for one moment.  I have not paid any visits since you left.  Writing has been my principal occupation, &amp; Eliza being still confined to her room, I am obliged to sew.  Clara made my blue dress, not as well as Eliza, &amp; the other one I am keeping for Eliza to make.  The baby is well, &amp; so is Eliza, but she will not be out of her room for two weeks yet.  Clara is now working for Mamma &amp; Ann &amp; Susan. Susan Hoke says she has repeatedly written to Augustus Hoke to go &amp; see you, &amp; she thinks he cannot have received the letters, &amp; so does not know you are in town, but it is no consequence  whether he goes or not, except it is rather ungrateful in him not to go &amp; see Aunt Eliza who was kind enough to invite him to tea; but I dare say he feels awkward, not being accustomed to visit among ladies. I am glad you are learning independence &amp; visiting alone.  A little girl may be modest, &amp; yet at the same time be easy &amp; independent, &amp; able to act for herself.  I am glad also you play for your friends on the Piano.  It is right to begin at once, &amp; be obliging, &amp; not refuse, which generally proceeds from affectation &amp; a too great desire to please.  They refuse, because they are afraid they will not excite admiration enough, though sometimes it is from awkwardness.  I am glad to hear that you are obliged &amp; able to entertain your friends.  I hope you will play well when you return.  It is no consequence whether you work much on your quilt now.  You will have plenty of time to finish it when you return. Mrs. Beattie &amp; Mrs. Henry Earle have been here since I commenced writing.  Mr. Mauldin I hear is much better.  He is still in Columbia.  Mrs. Joab Mauldin stays with Mrs. Mauldin. Sally &amp; L… Cleveand are going to school at the Limestone Springs, &amp; Mrs. Cleveland is going in the county.  Your Papa has not come home since I commenced writing, &amp; I sent Fanny to his office this moment, &amp; two gentlemen are there, so I cannot send the money today, but will soon.I hope you are behaving so well, as still to merit the good opinion of your friends.  I sent the box with the Cloak &amp; a letter containing the chain &amp; pencil case by Mr. John Jones last night.  I had sent the bonnet &amp; petticoat before I got your letter saying you did not need them.  Fanny says she likes school.  There are a great many scholars, Vardry &amp; Annie go.  Give my love to Aunt Eliza &amp; my cousins. </t>
+  </si>
+  <si>
+    <t>EMP276_06_01_1853</t>
+  </si>
+  <si>
+    <t>I have just received a letter from you, &amp; am very glad to hear.  Your Papa is getting a great deal better &amp; will soon I hope be quite well.  He has now rode to the Farm to fix upon a spot for Mr. Lasly to build the Log house.  When he comes back I will get some money from him to send in this letter. I am glad you still enjoy yourself.  The weather is now much pleasanter; today is very fine.  Monday afternoon we had a real Snowstorm, &amp; the snow continued on parts of the ground for several days, but has now all melted away. Yesterday afternoon I set off to walk to your Grandmama’s, but before I got halfway, I met Susan herself coming in, so I turned back, &amp; was very glad to, for the ground was very damp, &amp; I had on thin Gaiters. This afternoon Jenny Carson is to have company.  Susan told me Annie was to go. &amp; this morning, Miss Malinda, to my great surprise, sent to ask Willie &amp; Frank to go.  I thought she would not have asked any of my family, but I am glad she did, as I hope she feels kindly to them, so I sent word Willie &amp; Frank should go with pleasure.  They go at 4 oclock this afternoon. Mr. Leary was to leave Greenville today.  Mr. Irwin told your Papa, Mr. Leary said, Willie understood what was taught him, better than any boy he knew of, &amp; his chief regret in  going away, was leaving Willie &amp; George Wells.  Willie was to have gone to the Baptist College but it commences in February, so in the meantime he will go to the Academy, &amp; if he improves, I hope your Papa will continue him there.  Mr. Thomas &amp; Mr. Hillhouse are both to be in the Academy.  Mr. Thomas teach[es] the large, &amp; Mr. Hillhouse the small boys.  Frank is very sorry at this arrangement.  He wishes Mr. Thomas to teach him.  A Catalogue of the Students of the Furman Institution has been published &amp; “B. Franklin Perry,” is among them. Fanny has gone to school again today.  Johnny walks with her.  I think she likes it quite well.  She has bought a Copy book &amp; a lead pencil &amp; a Primer.  Annie came in after Fanny left with Permilla &amp; went to school.  Julia Sharp goes to school, &amp; the Brookes, &amp; Eliza Lynch &amp; a good many.  Miss Hopkins teaches in Mr. Crofts old house.  Miss Bessileau lives there now.  I have not heard how many students she has, or who they are. Tom Butler has sold his place to Mr. Campbell, &amp; bought that small place of Jimmy Gallows on the Anderson road beyond Abram Willimans. Mr. John Jones left last night, &amp; not the night before as I had expected.  He came in the village Tuesday evening too late for the Stage.  I hope my cloak is now on the road, &amp; will soon be safe in Mr. Reeds store.  In future I will have to write to your cousin Eliza to shop for us.  She understands what suits us, better than Aunt Mary.  She has shopped well for you.  She &amp; Susan are smart to be able to make bonnets for themselves.  You must learn to work for yourself in the same way. I mean as you grow older.  Velvet bonnets are very pretty &amp; lasting.  If you make yourself useful, you will always be happy. Mr. Smith who was in Browning &amp; Semans Store has returned on account of Cholera.  He must be a great coward.  He asked Willie if you had returned, said he saw you almost every day in Charleston.  He came so near death last summer with Typhoid fever, I suppose it alarmed him, &amp; he now wishes to be very careful.  Cholera not being infectious, is not advancing as other diseases, for if a person lives prudently, there is scarce any danger of taking it. Mrs. Henry Earle said her son William  told her if she would ask, when you were going to return, he would drive her.  I told her you were enjoying yourself so much you had no wish to return yet, &amp; I might have added unless her son, was a very fine young man, he need…no thought on you now or ever, for it is  much better for a lady to remain single, than to marry, unless the gentleman has every quality to make her happy, &amp; a happy single lady is far more to be envied than an unhappy married one.  Eliza &amp; Susan are as happy as anyone can be.   They are useful members of society. &amp; afford pleasure to so many friends, &amp; have so much resource, that I dare say they do not know an unhappy moment.  How much better is their situation than Mrs. Hume Simmons, your Aunt Suzy’s &amp; many others.  Mrs. Westfield’s mother Mrs. Stokes is dead, &amp; was buried Tuesday afternoon.  Col. Dunham’s health is very bad, &amp; he is not expected to live long. I will give your love to the Mauldins. They do not go to school yet. Your Papa has given me 40 dollars, 15 of it you must keep to pay your expenses home, which will leave 25 dollars for you to spend.  When Eliza sends another list, I will know whether this will be enough or not.  I do not think I will write for anything more.  Our Groceries set off at a time the Rail Road was out of order &amp; brought no freight, so they were sent to Hamburg to come up in wagons which has caused their delay, the roads being so bad wagons for the present are not travelling.  The box set off about that time, &amp; I suppose was sent also to Hamburg.  Now the R[ail] Road is in order except the bridge &amp; freight comes more quicky, so I am sorry over Groceries &amp; the box did not wait until now.  The freight also from Hamburg is so high, the groceries will cost a great deal.  In future we will always get in the Spring.  Give my kindest love to Aunt Eliza &amp; beg her to write &amp; to Eliza &amp; Susan &amp; beg Eliza to write. </t>
+  </si>
+  <si>
+    <t>EMP277_07_01_1853</t>
+  </si>
+  <si>
+    <t>I received a letter from you this morning, &amp; was very glad to hear, you are still enjoying yourself as much as ever.  The excursion to the island will be delightful, &amp; I hope you will have as pleasant weather, as we now have.  Today is delightful, just like Spring.  You will find it quite a novelty to be on the water.  I am glad you passed a pleasant evening at Mrs. Cunninghams.  Before you leave, you must go &amp; see her, &amp; give my love to her. &amp; ask when Pamela &amp; Mrs. Cunningham are going to return from the North.  I believe they are still there, &amp; tell Emma you have the cup &amp; saucer she sent you.  It is now in the Drawing room. I sent you yesterday 40 dollars.  I directed the letter to Eliza, but the letter was written to you.  I hope you will receive the money safe.  You ought to get it tomorrow evening, after you return from the island.  As soon as you receive it, write &amp; tell me, as I will be uneasy until I hear. If your Papa has the key to the Carpet bag, I will send it by Butler Thompson.  He goes Monday I believe.  Eliza mentioned your having bought a key for the bag, so If your Papa has not the key, I hope the one you have bought will answer. If you would buy some of the things I have written for, &amp; send by John Jones &amp; Butler Thompson, I will be very glad, for I need them, the Gaiter boots, Fanny’s cloak, the 12 ½ cts Calico for my dress, the Mits, the lacets for Gaiters, &amp; as much as they can bring.  My cloak &amp; Fanny’s cloak at any rate I hope they can bring.  Having sent for so many things, I have not bought anything here, &amp; am in want particularly of the Calico for the dress, but if inconvenient to get &amp; send before you come, I can wait.  Your trunk will be so full that I expect you will be glad to send beforehand as many things as possible.  Mr. Elford was to have got 13 stair case rods, but he did not.  If they could be put in your trunk. I would write for them &amp; send the measure, but I expect you would not have room. I would like you soon to get the work box for Aunt Eliza.  Get Eliza to choose it for you, &amp; also one for yourself, but they must be useful ones, such as will really be of use to hold thread, needles &amp; everything used in work.  Make it a present to Aunt Eliza in your name, &amp; tell her to always keep it to remember you by.  I think it a better present than a writing desk, but you can consult Eliza. I hope before this you have received the box with the Cloak, &amp; the letter with the chain &amp; pencil.  I am sorry I sent the petticoat &amp; bonnet, your visit being lengthened, I thought you would need them, &amp; sent then before you wrote word I must not. Willie &amp; Frank went to Mrs. McBee’s yesterday afternoon &amp; staid until late at night.  There were a great many children there.  The boys played in the yard, &amp; the girls in a room.  Fanny has gone to school.  Hext is quite well.  I send you a peice of poetry on the death of Mr. Elford’s children.  I do not know who wrote it.  Show it to Aunt Eliza.  Your Grandmama &amp; Aunt Suzy have just been here.  Your Aunt Suzy begs me to ask your cousin Eliza not to forget to buy her a bag she wrote for suitable to use at church &amp; two alpacca  Aprons, such as your cousin Susan mentioned were worn.  They all send their love. &amp; say they would write to you, but they have nothing to write about. I hope you will see Aunt Harriet before you leave, but I am afraid you will not, &amp; perhaps not see Aunt Anna or Aunt Martha either.  I am glad you have seen Aunt Susan, &amp; that Paul &amp; his wife you may see, as they have returned.  This season of the year almost all who can go in the country, &amp; many pass the whole winter there. I am glad Eloisa has returned, &amp; that you will become acquainted with her family.  Sarah also I hope you will see. Your cousins Cloaks I expect are very pretty, &amp; more useful than the light one Aunt Mary got me.  The black cape I dare say is comfortable.  That will be its recommendation, &amp; after this winter I will wear it in common, &amp; as I will not next winter have to get either bonnet or dress, I can afford to get a handsome cloak.  Mr. Smith the Jeweller sent me yesterday as a present a white velvet Emory.  I will give it to you, for your work box.  I mean to put in it &amp; sharpen your needles.  Your Grandmama says, Lindy is not able to get through her work, so she is going to hire Maria who she had once before from Mrs. Pearson.  Lindy’s baby she thinks has the Measles.  I was very sorry to let Lindy go there, feeling certain the baby would take the Measles, &amp; knowing Lindy would not suit, but situated as your Grandmama was, I felt compelled to oblige her, &amp; run the risk of Measles, &amp; now after all , Lindy as I supposed does not suit.  She will have to remain there until the child gets well, for if she returns Hext &amp; Eliza’s baby will take it, &amp; Dr. Crooks said I must not let Hext go near them.  Little Clarissa was just beginning to grow well &amp; improve, &amp; has been so delicate, the Measles will go hard with it.  Give my kindest love to Aunt Eliza, &amp; beg her to write to me, &amp; tell me all about you, &amp; give my love to Eliza &amp; Susan, &amp; beg them to write, &amp; my love to Aunt Mary &amp; Aunt Anna.  It must have been a release to Miss Elizabeth Lee to leave this world.  Mr. Mauldin is still in Columbia. Your Papa is a great deal better &amp; would write to you, but as I write every day, there seems no necessity for him to.  I generally have some business to write about.</t>
+  </si>
+  <si>
+    <t>EMP278_08_01_1853</t>
+  </si>
+  <si>
+    <t> I have been busy all day &amp; not able to write, but as no Mail leaves on Saturday, the Cars not running Sunday, it is no consequence my not having written today.  This letter will go tomorrow.  I send a letter every day except Saturday when no Mail goes.  This is the day you were to go to the island.  I hope you have had as pleasant weather as we have here.  It is like Spring but so warm, I am afraid it will rain soon.  You must give me an account of your experience.  I know you will enjoy it. I hope this evening you will have received my letter containing 40 dollars, 15 dollars of it is to pay your expenses home.  I will see from the next list Eliza sends me whether the remainder is enough to buy the things I have written for. There is no danger of the children seeing the toys before you return.  The roads are so bad, the box will not come for a long time.  It set off before the R[ail] Road was repaired, so had to come by way of Hamburg.  If it had set off now it would have come on the R[ail] Road to Laurens, &amp; we would have got it sooner.  If I had known there would be such a delay, I would not have sent for so many things for myself &amp; the children, &amp; instead sent you the money to spend.  They will come so late, we could have done without some of the things this winter.  However I will have less to buy next winter.  I received a letter from you today.  I am always glad to hear from you.  You seem to be enjoying yourself as much as ever.  I would like to see Professor Anderson.  I wish you would get him to come here. You must thank Aunt Mary &amp; Aunt Anna in my name for the books they have given you.  The Listener I think I read long ago.  I will be glad to read it again; the other book I will also like to read. I received today a letter from Aunt Mary McCall.  She says she has got me the black cape &amp; had to pay 2 dollars, because the man said it was a disadvantage to change the cloaks.  The light cloak was 21 dollars.  The 2 dollars added to change it, makes the Cape 23 dollars.  Your cousin Eliza’s, you say was about 15 dollars, 8 dollars less than my Cape, so you can tell me which you think the best bargain, but I am glad to get something useful on any terms.  Aunt Mary said, the day she wrote, she intended carrying the Cape to Aunt Eliza’s.  I hope you will send it to me by the first opportunity, &amp; Fanny’s Cloak also, by Mr. Jones or Butler Thompson, the first that returns.  I walked to your Grandmama’s this afternoon.  Willie went with me, &amp; Reuben came for me in the carri[a]ge.  Your Aunt Annie begged me to say to your cousin Eliza that she wished all the Music she had sent, &amp; in addition begged her to get “Nelly was a Lady,” set in a peice arranged in the prettiest way, so she writes all the Music charged to her 1 dollars worth she prefers taking it all.  It is well, for perhaps Mr. Bacon would prefer giving you peices of his own selection, but if you see any peices you would like to get, to learn after you return you can get them. All at your Grandmama’s were as well as usual, except Suzy.  She has had the Measles.  Alex &amp; Vardry were there.  Clara is working for Susan &amp; Ann.   … inquired particularly after you, &amp; sends her treble love; all send their love.  I told … you had sent her a handkerchief.  I told Flora Hoke this morning that one was coming in the box for her.  You must get a handkerchief for each of Aunt Eliza’s women, like those you have sent, &amp; you had better soon get the work box &amp; give to Aunt Eliza.  Mr. John Hodges is dead.  He died of typhoid fever.  Your Papa saw him in Columbia &amp; says he looked as well &amp; healthy as possible.  Mrs. Sam Town[e]s is very sick.  I believe her lungs are affected.  I have not heard that it is so, but I know they were once, so suppose it is the case now.  I have not visited her for a long time, but as she is so sick I have some thoughts of riding tomorrow to see her, calling for your Grandmama &amp; Aunt Suzy to go in the afternoon.  I hope Alston will name his son Robert after his father &amp; the next one after himself. Lindy came home today.  The child has a cold, but I hope not the Measles.  I will let her go very often &amp; help your Grandmama.  She can make ginger cake for her, &amp; bread, &amp; help in other ways.  Maria I hope will do well.  She has no child, which is an advantage.  I wish your Grandmama to have a good servant.  I did not think Lindy would do, for she is willing but not capable &amp; efficient, &amp; has rheumatism, so sometimes she can hardly walk, &amp; has also to attend to her child. Mr. Randolph has moved into Col. Town[e]s house next door, &amp; Col. Goodlett lives in Mr. Brooks house, where Mr. Randolph has moved from.  He is to keep a boarding house.  Col. Goodlett says Mr. Randolph left the house in such a condition, it required a hoe to scrape the dirt from the floor.  It is well Aunt Eliza did not board with him last summer.  If she had, she would have been disgusted with Greenville.  It was fortunate she found rooms at Mrs. ….  Cornelia Ioor has sent me some Pecan nuts, by your Papa.  They are coming in a box from Columbia, but I do not know when they will reach here.  I am glad the ginger has proved useful.  I sent for a Jar for your Grandmama, &amp; one for your Aunt Suzy, &amp; one for myself.  These are my Christmas presents.  It is cheaper to buy ginger preserves, than to make preserves.  Give my love to your Aunt &amp; cousins, &amp; thank them for their kindness to you.  My love to Aunt Mary &amp; Anna &amp; all my friends.</t>
+  </si>
+  <si>
+    <t>EMP279_10_01_1853</t>
+  </si>
+  <si>
+    <t>I received letters from your cousin Eliza &amp; yourself yesterday.  Thank Eliza for hers, &amp; as she says she will soon write again, beg her to, &amp; I will write to her.  You have really passed your time pleasantly.  Your friends have been very kind to you.  I feel indebted to all of them, but more especially to your Aunt Eliza &amp; her family.  Thanks Aunt Mary &amp; Aunt Anna for the presents you say they have sent to the children, &amp; thank Aunt Mary McCall for her presents.  She has been very kind.  I will send her the 2 dollars, she had to pay for changing the Cloak.  Your Aunt Suzy wishes to know the price of the black cape.  I do not know, as it cost me on account changing 23 dollars, so at Mr. Reed’s, inquire the price that I may tell Susan.  You say I had better send a list of the articles I wish purchased, so I will.  I have almost forgotten what I have written for, you can add what I have overlooked.  The work box for your Aunt &amp; yourself you must first get, then what I have put on the list, &amp; after that the Candy, cocoa nut cake &amp; little presents you intended getting.  The 40 dollars I hope you have received, the 15 taken out for your expenses back leaves 25 dollars.  Eliza wrote word yesterday I must send 25, so I am glad you have exactly that sum.  It may not be enough, as I have written for knives, so if it is not let me know.  Tooth powder I cannot get here.  Be sure &amp; bring 3 boxes of powdered Charcoal.  I used to get it 20 cts a box; not paste, but merely powdered Charcoal.  One of the boxes is for you.  If you have not got it yet, get it immediately &amp; use, the two others bring home.  Sally Hoke came here this morning, &amp; her teeth looked so black, it reminded me of telling you to attend to yours.  I suppose you have not needed any Sarsaparilla.  The Lacets for Gaiters though trifling is important,  for every morning now I am delayed trying to lace with a pin, &amp; then have to give up, &amp; wrap the lacet round the boot, the tins come off, &amp; the tinners here put on such large ones, they will not go trough the holes.  I send a button for you to get one dozen like 18 ¾ cts.  Ask Aunt Mary McCall where she got it.  She did not send enough.  The Calico you sent in the box for your Aunt Annie, If it comes soon, I may take, if you are willing to make myself a dress to wear at home.  I need it very much, &amp; your Aunt Annie has just had a worsted Gown made to wear at home. &amp; bought a Calico one, &amp; Clara is to make it for her.  I have made none to wear at home yet.  The two I have got, are what I sent patterns to you of.  The blue one is made &amp; I wear to church, but if you prefer my not taking the Calico, you must say so.  I have written to Eliza to get me Calico for a dress, but it will be long before I get it, through I am very much afraid the box also will not be here soon. After you have purchased my list, &amp; sent me an account, if you remain long enough, I may write for a few more things, two nice pocket handkerchiefs, about 37 ½  apeice or the peice Susan, but cost 43 ¾, &amp; your Papa wishes Linen for shirts which I may write for.  Send up as many things as you can by private opportunities, Mr. Jones &amp; Thompson.  I hope before this my cloak has arrived safely &amp; that I will soon get the other one.  When the ginger gives out, if you would like it, you can get your Aunt another Jar. I am glad you have fine weather now.  At least I suppose you have, as we have now delightful weather like Spring.  Yesterday was cloudy &amp; drizzly, so we did not go to church.  In the morning your Grandmama sent to ask how Mrs. Sam town[e]s was &amp; she is very ill, &amp; not able to see anyone.  Her lungs are affected, &amp; she can scarcely speak.  The roads to her house are almost impassable. So we did not go to see her, but if she gets better we will go. Beg Aunt Eliza to write to me.  Tell her you write about others, &amp; wish to hear from her about you. I hope the Cholera will not increase.  If it becomes alarming, I suppose Mary Crayton will immediately return, &amp; you would come with her.  Let me know when you think she will return, if she will soon or not, if she will return this month. Willie &amp; Frank commenced school today, both at the Academy.  Mr. Hillhouse teaches Frank, Mr. Thomas Willie.  Willie has come back already, &amp; says Mr. Thomas, as yet has only two scholars, George Wells &amp; himself.  He is to buy more books today, &amp; go back again this afternoon. I will go to see Mrs. Mauldin, &amp; ask when her daughters are going.   You say you saw pretty key baskets.  If you choose you can get one as a present to your Aunt Suzy or Annie or for yourself, or for me.  It will not come amiss.  If they are reasonable, but if you prefer it, get something else.  The…of baskets Mr. Elford has got me.  I may spare some of them to your Grandmama as presents.  I think he said he had got a nest, but I may be mistaken, for I thought he had got knives &amp; rods which he has not. You must excuse my shabby looking letter.  I am busy &amp; often write so hurriedly I am almost ashamed to send my letters.  You must take Aunt Eliza &amp; Eliza as your examples for neat writing, not me.  My gold pen is bent, &amp; writes badly, which is my excuse.  I will send the carpet bag key by Butler Thompson.  Mrs. Robinson sent word she was going Wednesday.  I suppose he will go with her.  I will write a few lines by him.  I will soon write to Eliza.  If you would like it, you can buy a pretty work basket apiece for your cousins Eliza &amp; Susan, &amp; not get any to bring home.  The nest of baskets will do for us. Give my kindest love to your Aunt &amp; cousins &amp; thank them for being so kind to you., &amp; giving you so much pleasure, enough to think of &amp; talk of a long time.  My love to my other friends.  Your affectionate Mother, E.F. Perry Buy some large sheets of letter paper &amp; write longer letters.  Burn up my letter.</t>
+  </si>
+  <si>
+    <t>EMP280_11_01_1853</t>
+  </si>
+  <si>
+    <t>I have just received two letters from you, &amp; must answer them immediately, for the Mail now closes at 12 oclock, &amp; the letters must be just in sooner than heretofore.  I hear very regularly from you, every day except Monday when no Mail comes, &amp; you ought to hear every day from me except Monday, so Monday you get no letter from me. Your friends have all been as kind as possible to you,  You must thank Aunt Brewton for the present you say she has sent Willie, &amp; tell her I hope her Godson will do credit to her.  If he is as good as he is smart, there will be no fear but what he will.  I do not say so from vanity, but from the opinion all his Teachers have expressed, &amp; not to me, but to others have they expressed it, so I know it is their real opinion.  Your Papa also has a high opinion of Willie’s mind, &amp; he has a good judgement, &amp; no vanity, either for himself or his children. Thank your cousin Eloisa for the cup &amp; saucer.  It is in a box of paper &amp;c. your Papa had packed in Columbia but it has not come yet.  The roads are in so dreadful a condition no waggons are transporting goods, either from the Laurens R[ail] Road, or the box would have come on from Hamburg, where our groceries are at present &amp; the box with them that Aunt Eliza had packed.   Today your Papa received a letter from Jeffers &amp; Cothran the factors who are to forward the boxes, &amp; they say since Christmas no waggons have come, that the streets present every day the appearance of the Sabbath, &amp; from the accounts they hear of the roads, it will continue so a long time, but by the first opportunity they will send on the boxes.  If I had imagined this delay, I would have done without several things I wrote for, &amp; sent you the money instead, or bought things for summer use.  F… &amp; my bonnets, we will have to put up for next winter.  You will be here at the opening of the box I have no doubt, &amp; witness the joy of the children.  A person in Mobile is writing sketches of distinguished men, &amp; mentions Uncle Robert.  In a Columbia paper there is an extract in which Aunt Brewton is mentioned.  It will be published in the Patriot.  I will cut it out &amp; send to you, &amp; you can give it to Aunt Brewton.  Perhaps she has seen it, [but] if not, it will gratify her, to see honorable mention made of one whose memory she reveres as she does Uncle Roberts. It was kind in Eloisa to say, she would like to have you stay with her.  I appreciate her kind intention.  You must go often to see her, &amp; Aunt Anna Turnbull &amp; Aunt Martha &amp; Aunt Mary &amp; Aunt Anna Hayne, &amp; any friend Aunt Eliza tells you to go &amp; see. I am sorry Aunt Emily is sick, &amp; Paul’s wife in delicate health.  Give my love to Aunt Emily when you next see her, &amp; Aunt Susan, Aunt Brewton, Aunt Elizabeth &amp; Uncle Arthur, Aunts in Logan st. &amp; Meeting st.  Your Papa is now quite well.  All at your Grandmama’s are the same as usual.  Clara works every day for them.  I help them in that way, as much as I can, &amp; work for myself.  Margaret at present can spare her.  Eliza has not worked for me since the birth of her baby, but will again next week.  Lindy is at home, at present with her child to attend to.  No one will hire her, but next summer we will get her a place. The new kitchen is building, &amp; when it is done, our servants will be comfortably accommodated, &amp; we will have a nice kitchen for our own use.  No one but the cook to stay in &amp; an ironing room, for no purpose but ironing.  The two new chambers, Eliza &amp; Lindy will have.  If Minerva wishes it, she can come over &amp; sleep in the room Eliza now has.  Charles will either sleep in the cellar or the old kitchen, &amp; the small house, you shall again have to keep as a play house.  Mr. Rosemond will repair it.  I will give Fanny the press in the little dining room as a baby house &amp; put in the play house, all the toys you have bought her, shall stay there.  If you had kept all the presents ever given you, how many you would have had.  Begin now &amp; keep them all carefully.  When you have bought the list I have sent you, I hope to send some more money.  Have you spent the 5 dollars you took out of your Bank.  Send as many things by Mr. Jones or Thompson as they can bring.  I expect you spent a delightful day at the island.  Your Aunt &amp; cousins have been so kind in trying to gratify you in every way.  You must tell them I thank them for their kindness to you.  Tell them not to give themselves any trouble on your account.  The visiting among your friends, &amp; seeing them, is an enjoyment to you &amp; Greenville is so quiet.  A walk up King st.  is such a contrast to a walk here that it affords you delight.  The shells we will be glad of, &amp; something new in Greenville.  You must keep them as a curiosity.  I am sorry you have not seen your cousin Sarah Taylor yet.  If you do, tell her the Scripture Biography she gave Willie, I find very useful in reading to the children &amp; servants on Sunday, &amp; tell Eloisa the basket she gave me in town, I use even now as a key basket. I saw in the Courier that your Papa had been alluded to by Mr. John Preston.  In Columbia last winter Professor Thornwell’s brother pointed to your Papa &amp; said “See that person, two years ago, he was avoided by Politicians as death, &amp; now he has more influence in the Legislature, than any other Member, &amp; more coveted by aspirants.”  Your Papa has always acted independently, &amp; in acting as he thought right, has gone against his own interests, which proves his sincerity.  Such conduct always in the end begets esteem, &amp; he has in his opinion the best reward, a good conscience &amp; his own self respect. Give my love to Aunt Eliza &amp; your cousins.  Their kindness I will never forget.  Ask Aunt Eliza to write to me.  I will write to Eliza tomorrow.  Go &amp; see Mary Crayton, &amp; let me know when she expects to return.</t>
+  </si>
+  <si>
+    <t>EMP281_11_01_1853</t>
+  </si>
+  <si>
+    <t>Tuesday afternoon</t>
+  </si>
+  <si>
+    <t>I wrote you a long letter this morning.  I now write only a few lines.  I will send them by Butler Thompson &amp; send the key you asked for.  I will send this letter to Mrs. Robinson &amp; she will give it to Butler Thompson, who I suppose is going with her.  His father a week or two ago said he was.  The weather is now clouding over &amp; we will soon have rain again.  Write word when Mary Crayton intends returning so I may know when to expect you.  I suppose this month she will return.  Your cousin Eliza said about the 20th of this month. Fanny goes to school, but she prefers staying at home.  She will like it better when you go with her.  I sent to ask Mrs. Mauldin when her daughters were going to school &amp; she sent word, they were not going at all.  I sent Aunt Mary today the 2 dollars she paid for changing the Cloak.  I hope you have received the 40 dollars I sent you safely.  I write so hurriedly, you must tear up my letters, tear up this one.  I write so much &amp; have other things to do, I write in haste.  Be a good girl.  I hope Mr. Jones or Thompson will bring the Cloak.  Mr. &amp; Mrs. Bacon came to see me this morning &amp; inquired about you.  I told then what Mrs. O’Driscoll said, &amp; that you practiced every day.  Mr. Bacon says he has only 3 scholars now that for a short time in summer he had 23, but he ought to have 30 scholars the whole year round to afford him a support, that if he did not get more scholars he could not live here, but this climate agreed with his health, so he hoped he could get enough to enable him to stay.  I hope he will find you improved.  He says he has no objection to your buying any pretty peices for yourself.  Your Grandmama &amp; Aunts send their affectionate love.  Your Grandmama says you write wonderfully well.  She is pleased at Aunt Brewton remembering Willie.  Give my love to your Aunts &amp; cousins, whose kindness to you has been very great, &amp; I know you feel grateful, &amp; will never forget it, &amp; when in your power return it.  Mrs. Sam Town[e]s is better &amp; Mr. Hodges through very low, is not dead.  The report was not a mistake. You must soon buy the work box for Aunt Eliza as a testimony of your love for her, &amp; a proof you feel gratified for her kindness.  Your affectionate mother, E.F. Perry P.S.  Get a Cornelian ring for yourself &amp; one for Fanny.  Her silver comb I will give to Annie, which is more valuable than a ring.  Buy 2 dolls for Fanny &amp; Annie.  You can dress them when you return &amp; a small doll to L…a knife with 2 blades for Willie &amp; Frank, not expensive ones.</t>
+  </si>
+  <si>
+    <t>EMP282_00_01_1853</t>
+  </si>
+  <si>
+    <t>…like to get for yourself you may.  The knives for Willie &amp; Frank need not be fine ones, as they will soon lose them.  Put on paper a list of what I have mentioned in this letter.  Your Aunt Annie wishes “Nelly was a Lady[.“]  The 75 cts for Music that was charged to you, your Grandmama wishes to add to her bit, so that 75 cts you will have to add to your money to buy something with.  I you need a thick pr of shoes for school, you had best get them now.  I hope to be able to get some more pocket handkerchiefs, as need more.  If I write for them, I will wish some at 16 cts, for you, &amp; marked with your name  &amp; some for 25 cts marked with mine.  Mrs. Sam Town[e]s is getting better, &amp; sent word she would be glad to see me.  At the time Mr. Town[e]s was abusing your papa in his paper, I would not take pleasure in visiting his family, so gave her up, but your Papa has forgiven him, &amp; Mr. Town[e]s looks to him to do more for him than anyone. A great change has taken place &amp; the very persons who during political excitement abuse your Papa the most, are now writing to him. to use his influence with Genl Pierce to give them Offices.  They say your Papa writes for them, would have an effect, more than anyone else.  He does for them, &amp; those who have injured him, what he would not do for himself. I will go to see Mrs. Town[e]s when the roads are good.  Now they are at most impassable.  I dare say it will not be before you return.  You can go with me.  I will call Julia Sharpe to keep the seat at her desk for you.  I am certain she will.  Except Miss Hopkins there is no other school for girls. I hope Clara will be a valuable servant for you by &amp; by; then her wages can even support you.  Margaret says she can do everything except make Pastry, &amp; that that she would soon learn.  Our servants are so expensive now, the supporting them &amp;c, that if it were not for the hope of future profit, we would be obliged to sell them.  Eliza’s baby is a month old Monday.  Then Sarah will go back to Margaret, who I hope will take her, through she sent word she did not care for her.  She is useless here, &amp; get[t]ing into bad habits.  Eliza’s influence &amp; example to her children is so bad, I would be thankful if we could get rid of her.  Johnny at present seems a good boy. Give my love to all my Aunts.  If Aunt Harriet is at Mr. W…, ask Aunt Eliza to write to her, &amp; beg her to come down for one day &amp; see you.  It is only a short ride, &amp; I am certain if she knew you were in town, she would come &amp; see you.  I will send you stamps in this letter.  When they give out, it would be well to buy some. Aunt Anna’s friend was a pious lady, &amp; so afflicted, that her death must have been a blessing, as they have every reason I hope to think she is happy now.  Mr. Elford has money of your Papa’s. but has had no settlement since he returned. So I do not know wat he bought for me.   Mr. Wm Watson I believe goes to town soon.  I had just written this sentence when your Papa came in &amp; brought Mr. Elford’s bills.  He has bought the nest of baskets, the Calico for Comforts, the Fender, Andirons, shovel &amp; tongs, broom &amp; bellows, the nest of baskets is 3.87.  Mama I expect will take some of them, the Calico 6 ¼ a yd, the other things $18.19 cts. I have just heard Mr. Hodges is dead, that he was resigned, he had no children, &amp; his Wife &amp; himself not very happy.  Mr. Henry Thompson &amp; your Papa got elected to Commissioner of…&amp; he came this morning to ask if he would appoint his son Henry as keeper of the gate, which Mr. Hodges used to keep; that Henry will stay at Mrs. Hodges, keep the gate, &amp; keep school at the same time, &amp; attend to his studies.  He will make several hundred dollars a year, &amp; is only 17.  You see when persons are poor &amp; thrown on their own resource, how they manage to support themselves, &amp; at the same time improve their Character &amp; acquire habits of industry, they make their own fortunes, whereas, if their parents had a few hundreds to give them, they think themselves above work. &amp; become idle &amp; dissipated &amp; ruined characters.  I am glad there is at last something cheering for Mrs. Thompson.  She has sent repeatedly to ask if there was bundle here for her, but I have heard of none that was coming for her, unless some of her friends intend sending one by you.  If Charlotte Smith hears of your being in town, I dare say she will send a bundle.</t>
+  </si>
+  <si>
+    <t>EMP283_1853</t>
+  </si>
+  <si>
+    <t>I have just received a letter from you &amp; will answer it tomorrow.  Thank Aunt Brewton in my name for yours &amp; Willie’s presents.  It was very kind, &amp; they will be very useful.You have so much to bring for yourself, I dare say you will not have room for Mrs. Herriot’s boxes.  If so, you must return them, &amp; tell her you are sorry you cannot bring them.  After awhile, persons will be going down from here who can bring them for her. </t>
+  </si>
+  <si>
+    <t>EMP284_13_01_1853</t>
+  </si>
+  <si>
+    <t>I have just received a long letter from you &amp; must answer it immediately as the Stage goes now at 12 oclock.  There is one thing that I wish to get &amp; that is a pattern for the side of an Ottoman.  Get it the length of the paper I send, &amp; of the shape.  I have cut the paper, &amp; one bunch of worsted like each colour in the pattern.  I have had broadcloth for you to work ottomans for your Grandmama, &amp; this winter I would like to continue them at least.  I will teach you how to do the worsted work, &amp; you must work a pincushion  for each friend who has shown you kindness, since you have been in town, tell them so.  I have plenty of Broadcloth &amp; Canvass &amp; some Worsted.  Also, buy one dozen worsted needles of different sizes, some of them very small, &amp; you can commence when you return, &amp; work them at your leisure.  You have made a pleasant visit.  I know you will need more money.  If I do not send what you need in time, if your Aunt advances it, I will immediately return it, as soon as I hear from you how much it is, but I much prefer your asking me for it, than getting it from anyone else.  So write &amp; let me know what you need.  I am sorry Wm Ed had a pencil case.  Perhaps Eliza might think of something else for him, &amp; be sure &amp; buy the work box for Aunt Eliza, &amp; a basket or something else for Eliza &amp; Sue, &amp; a handkerchief for each of the servants. I am glad you make yourself useful to your Aunt, &amp; helped her fix the curtains.  I wish you would see Sarah Taylor, but if you leave before she comes, perhaps in Columbia you may have time to see her.  I am glad Aunt Anna &amp; Aunt Martha you have seen again.  Tell them to write to me by you.  Bring as many letters as you can from our friends.  Let them know when you will leave, &amp; beg them to write.  I suppose you have not seen K…’s relations, Mary, Sarah &amp; Edward though they are not I believe estimable characters,  Still if you could see them &amp; tell K… you have, it would gratify her.  I am glad Mr. Jones will return soon, &amp; that he will bring some of the things.  I sent a letter enclosing the key yesterday to Mrs. Robinson &amp; she had gone.  It is no consequence, for since I have heard Butler Thompson was only going as far as Columbia with them, so I will send the key in this letter. We all will be very glad to see you.  Mr. McKay &amp; the oldest Miss Hayden teach the large girls; the youngest Miss Hayden teaches the small girls.  Fanny says they are not cross.  Mr. Thomas teaches Willie a great many more studies than Mr. Leary did.  He wishes Frank to learn Latin, but we prefer not.  He is too young.  You must take good care of the children at school.  Only two of the Brooks go to school.  Mrs. Sam Town[e]s is getting better, &amp; Mr. Hodges also.  Soon I must go &amp; see Mrs. Mauldin &amp; some others.  A Chinese ornament for 25 cts, or a little basket, or any little present, you can bring Mary Mauldin. Aunt Mary McCall today I heard from saying she had received the Check.  I hope she will receive safely 2 dollars I have since sent her.  Some pretty Calico get me for aprons for Fanny.  I would send you a 5 dollar bill at least in this letter, if it had not the key &amp; paper in it, for I know you would be glad of it.  If I write tomorrow I will send it.  I hear from you regularly each day except Monday, when no Mail comes.  I am surprised you do not receive one letter each day from me, instead of so many at one time.  Your Papa says I write too often.  I suppose that you have heard that Genl Pierce’s only child has been killed on the R[ail] Road, how sad.  I am glad you have some shells, &amp; found it pleasant on the island.  It looks a good deal like rain again.  The roads will be worse than ever. Tell your Aunts you will work them a pincushion. &amp; also Eliza &amp; Susan.  I will help you.  I did wish you to buy some books, some of Miss Milfords &amp; Mrs. Howitts works, but will have to put off for another time.  At the end of the year there are so many bills to pay, or I would have sent more money.  Another visit I will supply you better &amp; not tell you to buy so many things for me.  I wrote to Eliza yesterday.  I do not know what our Eliza will name her baby.  Aunt Eliza has no name to…of her.  She is one of the worst servants I know of.  She has no principle, &amp; I am afraid with such a Mother, her children will not have any.  They are corrupted from their infancy, &amp; if it were not for Missy, who has been a faithful servant to Mamma, I would not feel it my duty to keep such a servant.  Do not forget Becky’s comb.  She is not near as good a cook as Minerva, but she is a better servant, &amp; makes all happier.  Minerva wishes to leave the Mansion House, says she is worked too hard, but she is always dissatisfied. Give my love to Aunt Eliza &amp; your cousins, &amp; my other Aunts.  I am sorry Aunt Emily is sick.  Let me know when to expect you.  Emily Earle &amp; her sister go to the Academy.  It is the only female school now. Your Papa is quite well now.  It is no consequence when you see Augustus Hoke, &amp; Mr. Smith must be wanting in steadiness to leave his business for such a trifling reason.  Hext is well; the other children at school.  Clara as soon as the new kitchen is finished is going to have a party or Fair.  I do not like to have such things in the yard, but disliked refusing, &amp; if it is in the kitchen &amp; not in the cellar, it will not distract us.  I hope to hear tomorrow, as soon as you have taken a list of the things you are to buy, that I have written in this letter, burn it. do not show it to anyone.  It is written so badly. </t>
+  </si>
+  <si>
+    <t>EMP285_01_01_1853</t>
+  </si>
+  <si>
+    <t> I send you my chain to wear with your Medallion,  I do not like little girls to dress too fine, but I think when you spend an evening out, the chain put round your neck twice, &amp; the Medallion suspended to it, will look more suitable than the seven pence chain you bought in Columbia.  I do not think for such occasions it will look too fine.  The Chain your Papa gave to me before we were married, so I never expect to part with it.  Some time you can have a Daguerreotype likeness of your Papa &amp; myself &amp; a lock of our hair put in your Medallion. I send a gold pencil case which if your cousin William Edward has none, you may give to him, as a present from yourself, as a proof that you feel grateful for the kindness he has shown you, since you have been under his Mother’s roof.  I bought it for myself, but it was too large for a lady, &amp; I have never made use of it.  If he has a gold pencil case, this would be of no use to him, &amp; I will think of something else for you to get, but if he has none, this he will find useful. The work box or writing desk for Aunt Eliza, &amp; some present of value for your cousin[s] Eliza &amp; Susan I will write you about before long, as soon as I hear from you about the one you are to get.  I hope to send this letter by Butler Thompson, but if I hear of any other safe opportunity sooner, I will not wait for him.  If you get homesick, or anything occurs to make it inconvenient for you to be at your Aunts, write me word. &amp; by that time I dare say your Papa will be well, &amp; able to go down for you.  But your friends are so kind &amp; you seem to be passing your time so pleasantly, I suppose you are not afraid of being homesick.  I hope this visit to town will improve your manners, &amp; your character in every respect, &amp; you will learn more than at school, even if you commenced the first day, as I had expected.   I have written a long letter to you today, so will now stop.  Your affectionate Mother, [E.F.P.] Jany 1st.  I wish you many happy returns of this day and that each New Year may find you more improved in everything, that will increase your happiness here, &amp; make you happy hereafter.</t>
+  </si>
+  <si>
+    <t>EMP286_02_05_1853</t>
+  </si>
+  <si>
+    <t>Monday afternoon, 4 oclock</t>
+  </si>
+  <si>
+    <t> We arrived here a short time ago &amp; have a comfortable room at Mrs. Davis’ up in the 4th story.  Mr. Arthur, Mr. Cox &amp; Mr. Lec… took good care of us, &amp; Mr. Pinckney who got in the Cars from Aiken at Branchville was also very kind.  Mr. Arthur hired a carri[a]ge &amp; brought us to this house.  He is at the Charleston Hotel.  Our dinner was sent us upstairs.  I am undressed, &amp; am very tired.  My hand is unsteady, from the motion of the Cars, &amp; I only write to prevent your being uneasy.  I have borrowed pen ink &amp; this half sheet of paper from Mrs. Davis.  An irish woman waits on us.  I will be glad to see you any time [page torn] come, but I do not think it worth [while] [page torn] to come down twice, unless you can remain several days each time.  I would rather you come for me &amp; stay some time here.  Mr. Arthur says he &amp; Mr. Cox can vote for the delegates who are absent (from Greenville) that is he…is entitled to vote for the other, so if you come here you will vote as a delegate, but if you are away. the others will vote for you, so it makes no difference of course.  I have seen none of my friends yet.  Tomorrow morning I will go &amp; see them….to me every day, &amp; I will write Wednesday, if I have time, but if you do not hear, you must not be uneasy.  I missed you today.  No one can make up to me for you, but the gentlemen…very hard.  Mr. Pinckney said he would come &amp; see me.  I paid 1 dollar for the hire of the carri[a]ge, &amp; 50 cts to Mr. Arthur for ice creams.  He did not wish to take it, so I told him to give it to the children.  A boy has come for the…&amp;c.  I must stop. </t>
+  </si>
+  <si>
+    <t>EMP287_04_05_1853</t>
+  </si>
+  <si>
+    <t>Wednesday morning, quarter of 7</t>
+  </si>
+  <si>
+    <t> It is an hour before breakfast, &amp; as I have nothing to do, I will write to you.  Last night I took tea at Aunt Haynes.  Mr. Martin came there to see me, &amp; to ask us to stay with them.  He entertains persons constantly &amp; Aunt Mary says it is no inconvenience to him.  If you think I had better stay, I am willing to go there, as it will save the board I am paying at this house, but if you think I had better remain where I am, I will remain.  Except the expense of boarding I would rather be here, because I feel independent, but as they are so urgent &amp; say it will give them no trouble, if you think best I will remove to their house. Tomorrow I am to dine at Aunt Elizas.  I like Aunt Haynes, Uncle Arthur, &amp; Aunt Elizabeth, Aunt Brewton, &amp; Aunt Mary McCall the best.  Of the relations I have seen, I like Eloisa Martin, but Aunt Eliza &amp; her family I like least &amp; Aunt Anna Turnbull &amp; those at her house the next least. I have bought nothing yet.  Charleston is not to be compared in looks to Columbia.  The Convention sits today.  It is thought no Bishop will be elected.  Mr. Martin says he has in his pocket a letter from Dr. Atkinson acknowledging his abolition principles, that Mr. Trapier &amp; the high church ministers here, have given him up.  It looks cloudy, we need rain, but I will be sorry if it does, as I wish to shop.  Tomorrow as I am to dine out, I may not have time to write. I will now stop.  Your affectionate wife, E.F.P.  After the fact. P.S. Since writing the above Aunt Anna Turnbull has sent to ask us to dine today with her.  We are going. But first I am to shop with Aunt Mary McCall.  Aunt Mary Haynes says any evening I have no engagement I must spend with them.  Mrs. Julia Pringle is here.  I have been in the drawing room talking to her, &amp; Mrs. Martin, &amp; Col. Irvine who stays at Fort Moultrie is here, but goes back to the island today.  His wife stays here altogether.  She knows Uncle Arthur &amp; Aunt Elizabeth well.  Mrs. Pringle goes to Newport in June.  Mrs. Poinsett is in Charleston at the Miss Pinckneys. Her place was sold including furniture for 5000 500 dollars.  Mrs. Pringle says it was given away.  Mr. Pringle is not here.  </t>
+  </si>
+  <si>
+    <t>EMP288_06_05_1853</t>
+  </si>
+  <si>
+    <t>Friday morning, 1 oclock</t>
+  </si>
+  <si>
+    <t> I have just returned from shopping &amp; will write to you.  The few lines you wrote enclosing Susan’s letter, is all I have heard from you since I left Columbia.  A servant goes to the Post Office every day.  I hope today after the Cars arrive I may hear.  I have had to buy things for Susan Hoke, Mamma, Susan &amp; myself, &amp; the shopping is dreadfully fatiguing.  Yesterday &amp; the day before after shopping, I had to dine out, so at night I was very tired.  I have almost finished shopping now, so I will not be so fatigued.  Things are higher than I expected, so I have spent much more than I had any idea of, &amp; more than at the time I am aware of until the bills are made out, but after this, I will be economical.  I long to see you.  It is not worth the expense for you to come down to see me, &amp; go back &amp; come down for me, so one trip seems sufficient, but as soon as your business is done, come for me, &amp; write me word when you think you will come.  I would like to know. I was truly sorry to hear of Eliza’s death.  I could not realize she was going to die, &amp; had a faint hope she would recover.  She will be such a loss to me, having for 11 years done my work, that I do not know how I can do without her.  Clara I wish to stay with Margaret until Jany to finish her trade, as this year is the most important.  She is to learn to cut &amp; fit, but she must sleep at home every night, to attend to the baby, &amp; I hope when I have pressing work to do, Margaret will let me have her.  I am sorry for Eliza’s children &amp; Missy, &amp; will do a good part by them &amp; never part with them.  Susan’s account was quite affecting &amp; I hope Eliza is happy now.  I dined yesterday at Aunt Eliza’s, spent a pleasant time, &amp; in the afternoon walked on the Battery.  Today I am at the boarding house, &amp; am glad of a rest.  No Bishop has been elected yet.  Mr. Leary called today while I was out, &amp; Mrs. H… Simons, &amp; Mrs. Bay &amp; Mrs. Crawford yesterday, &amp; Mrs. Henry Pinckney &amp; family, Mrs. O’Driscoll, Mrs. Ramsay.  Persons have not yet found out I am in town.  Yesterday Uncle Arthur intended asking me to dine but I was engaged to Aunt Eliza’s.  I saw Aunt Emily at Aunt Eliza’s.  I will keep my letter open until the afternoon when I hope I will hear from you.  You must write of[ten] or I will get homesick.   As I do not know when the letters will come, I will close this.</t>
+  </si>
+  <si>
+    <t>EMP289_06_05_1853</t>
+  </si>
+  <si>
+    <t>Aunt Anna Turnbull came here this afternoon &amp; she says I must stay with her.  So I write at once to ask you.  I hope this letter can go by tomorrows Mail, &amp; you answer it Sunday, for I expect I had better stay my week out here, &amp; go to Aunt Anna’s Monday morning.  If you stay some time longer in Columbia, I expect as Aunt Anna seems so sincere in her invitation that I had better move there, but if you expect in a few days to come for me, I might as well remain where I am.  Write the instant you get this letter &amp; tell me how long you think you will be, before you come down &amp; my movements will depend on that.  Eloisa Martin has just been here, &amp; repeated her invitation to stay with her.  You write me what I had better do.  Mr. Arthur came to see me this afternoon.  Mr. Davis of Camden has been elected Bishop, high church Mr. Arthur says.  Write me immediately how long it will be before your business is over.  I will close so as to send this letter to the office.</t>
+  </si>
+  <si>
+    <t>EMP290_07_05_1853</t>
+  </si>
+  <si>
+    <t>Saturday, 1 oclock</t>
+  </si>
+  <si>
+    <t>Day after day passes, &amp; I do not hear from you.  I begin to think you must be sick, for as you are only one days journey from me, I cannot imagine why you do not write. I received a long letter from Susan toda, &amp; one from Frank.  Lindy’s baby had been unwell but was better.  The rest of the family were well.  May day she says was the poorest display she ever saw, but they had plenty to eat, &amp; the children enjoyed themselves.  Aunt Turnbull sent today to say she would send for me at 2 oclock to stay with her, but I wrote word I would let her know Monday, after I heard from you, how long it was probable you would be in Columbia.  If you expect to come down soon, it would not be worth moving there.  If you were not coming for me, I would perhaps go there now, but I expect you would yourself much prefer being at a boarding house, than staying at Aunt Anna’s.  You prefer being independent, &amp; I am afraid Aunt Anna for the short time I stay there, would expect me if she comes to Greenville to invite her to pass the summer.  This makes me reluctant to stay with her, but you write me what to do.  I hope to hear from you this afternoon.  Mrs. Martin is in this house, &amp; is very polite.  Mrs. Julius Pringle is here, &amp; is polite, but she is not a pleasant person.  The weather is not hot; the noise I am getting accustomed to.  Direct your letters to the care of Mr. Wm E. Martin, or Wm Ed. Hayne.  I will then be sure to get them.  I think now there must be some mistake that you have written, &amp; the letters have miscarried.  Mrs. Pringle’s servant this morning, brought me the two from Susan &amp; Frank, &amp; I am surprised none from you. Uncle Arthur last night sent to say, he had called repeatedly to see me, but I was out.  The servants do not tell me who calls. After dinner This morning when I returned from King St. I found Uncle Arthur had called again.  Aunt Anna Turnbull sent to ask me to ride with her this afternoon to Magnolia Cemetery, &amp; I am going with her.  I have just received a letter from you.  I am glad you are well.  I rather think as you think you will come down next week that I will remain where I am.  If you were not coming, I would go to Aunt Anna’s or Eloisa’s, but as you are coming, I do not think you would find it pleasant at either of those places, &amp; I expect you would not be willing to stay at a Hotel, &amp; I at a private house.  I do not think at Aunt Anna’s you would find it pleasant.  Perhaps Monday I could go to Aunt Anna’s &amp; stay until you write word you are coming, &amp; then I would move back to Mrs. Davis, &amp; be in time to meet you here.  So hat do you think; write me by return Mail.  Anna yesterday was unwell.  The water I expect has disagreed with her, &amp; she was just loose in her bowels, &amp; then bound, &amp; in great pain, &amp; Mrs. Pringle advised me to send for a Doctor, &amp; I sent for Dr. Geddings, &amp; he gave her some pills which have done her great good, &amp; by tomorrow he said she will be well.  He paid her two visits so I will have to pay his bill, &amp; if I were to move from here, I would have to pay the bill here, so I would be very glad if you would send me some more money to prevent my feeling embarrassed.  From 20 to 50 dollars according to your liberality, the letter in which you enclose it, you can direct to the care of Wm Ed Hayne, if you think it safer.  I have received two letters from you.  If these are all you have written, then there is no risk, but I think perhaps you have written some I have not received.  I was to get money from Alston for Mama, bit I dislike asking, so if I had enough I would prefer lending her mine.  Send the money by return Mail.  Mrs. Pringles servant goes for my letters, &amp; brings them safely.  I will get him to bring me some Stamps, so you will not have to pay postage.  I will not determine about Aunt Anna’s until I hear from you, whether you will like to stay there, or like me to return to Mrs. Davis &amp; meet you here, or you stay at a Hotel when you come, &amp; I at Aunt Anna’s.  She may expect me to ask her to stay with me in Greenville, &amp; this I cannot do.  Eliza dead, my work will be unusual, &amp; I expect to devote every moment to sewing.  I see ready made clothes for children, &amp; that is one thing I would like to get for Willie &amp; Frank &amp; why I wish more money, for I will not have time to do all, &amp; do not understand making boys clothes.  Eliza’s loss is irreparable.  I deeply deplore it.  For 11 years she has worked for me &amp; made my dresses better than a Mantua maker.  In consequence of her death, I am having a dress made here, which I will have to pay 3.25 for, &amp; that is thought cheap, for 5 is the price.  I am glad I have heard.  If you could get business in Charleston, I would like you to move here.  I like a City.  Your affectionate wife, E.F.P.Anna is well, but having taken medicine cannot go out this week.</t>
+  </si>
+  <si>
+    <t>EMP291_08_05_1853</t>
+  </si>
+  <si>
+    <t> I went to St. Michael’s church this morning.  Aunt Elizabeth called for me.  I did not see Uncle Arthur.  He went to Grace church, Mr. Pinckney’s church to hear the new Bishop.  Mr. Arthur preached at St. Phillips.  It was an old sermon but Aunt Elizabeth liked him.  The Bishop preaches this afternoon at St. Phillips.  Perhaps I may go there. Yesterday afternoon Aunt Brewton called to see me.  She said I must take tea with her Monday.  Aunt Anna Turnbull then called for me &amp; took me up to the Magnolia Cemetery 3 miles out of the City.  It is a beautiful spot on Cooper river.  The river winds along through the grounds.  A bridge is across it.  In one spot, there is a Gothic chapel in the midst, &amp; some beautiful monuments, one recently erected to a Mr. Jones a stranger who died here, by his widow cost 6000 dollars. After tea last night, Aunt Mary McCall called to see me, &amp; before she left Mr. Isaac Hayne &amp; his wife called.  I was surprised.  I thought after my conduct to him, they would both have passed me without notice.  They were very affable, &amp; from this time we must bury the hatchet, for really I feel sorry for him.  He has the same abstracted look Mr. Treville has, except more worried, so I have come to the conclusion, that the Attorney general’s…is never out of their minds, that as the Contest is always such a close one Mr. Treville is looking forward to getting it, but afraid he may not.  Isaac Hayne is looking forward to losing it, but hoping he may not.  His manners are not playful &amp; lively as they once were, so I make allowances for his apparent coldness to you, &amp; believe now, it is unintentional.  He asked about you.  He looks like his father.  Aunt Brewton said I must take tea with her Monday.  Aunt Elizabeth said I must dine with her Tuesday, that she was sorry she had seen so little of me.  She is the kindest of my Aunts in law.  She seems to have such a kind heart.  Uncle Arthur &amp; herself have been repeatedly to see me, but I have been out.  Aunt Brewton said her daughter in law, Alstons wife had been, &amp; left her card, but I never received it.  I do not know who has been.  Mr. Arthur this morning called before church.  I was very anxious to see him to know if he had received a box a Milliner was to pack &amp; send to him, but the servant never asked him in.  This is a pleasant house on account of the situation &amp; privacy, but they have but two boys &amp; one woman to attend to the whole house, &amp; one little boy, so I miss not having a servant.  The board for a servant I see on the rules is 4 dollars a week.  If I had brought Clara, she would have saved me 3.25 already.  I have to pay for making a dress &amp; would have gone on messages &amp; shopped for me, so another time I will bring her. Write me word what time you think you will be down.  I wrote a note to Aunt Anna yesterday, &amp; said if you were not coming down soon, perhaps I might go to her house, but if you were coming down, it would not be worthwhile to move, &amp; I would give her an answer Monday.  She seemed really sincere in asking me, but I know her disposition, &amp; she dislikes so having trouble &amp; expense, that I am certain she would like me better if I do not stay with her, so I have no idea of leaving this house.  She has been kinder than I expected. Mr. Isaac Hayne says Columbia is not as hospitable a place as it used to be.  I expect as Cities increase in population &amp; wealth, they become more fashionable &amp; less hospitable.  Aunt Susan Hayne is the only Aunt I have not seen.  She lives very high up &amp; keeps no equipage.  Anna is better, but today I thought she had better not go to church.  I expect this afternoon to go to St. Michaels again with Aunt Elizabeth, &amp; tonight to St. Peters with Aunt Martha McCall to hear the new Bishop.  Dinner is nearly ready so I will close &amp; hope to hear soon from you.  Your affectionate wife, E.F.P. I have not seen a paper since I came here.</t>
+  </si>
+  <si>
+    <t>EMP292_08_05_1853</t>
+  </si>
+  <si>
+    <t>William H. Perry</t>
+  </si>
+  <si>
+    <t>My Dear Mamma</t>
+  </si>
+  <si>
+    <t>Your affectionate son,</t>
+  </si>
+  <si>
+    <t>This is Sunday morning and we had intended going to church, but the rain prevented us.  It also rained last Wednesday, and I expect you do not have as much rain in Charleston as we have here.  I do not expect the Smallpox could have been bad or you would have went on.  Reuben said that you were not certain that you would go on if it was ther[e], but I never heard you say anything about it.  Mayday is past and Aunt Susan read me her letter…to you in which she told you about it.  She did not like the way Mrs. Earle did about the wreaths.  We had enough to eat upon a table in the yard, and we had enough of dancing also.  I danced some.  The dancing continued until late at night and it was twelve oclock when I got home.  Hudson stayed with me that night, and as we had holiday the next day he stayed  with me also until after dinner and then went home.  Aunt Susan likes very much.  I wrote a letter to Papa last Wednesday for one he wrote me before.  I wish you would write to me some, or as I expect you will be very busy in shopping and visiting.  You must tell Anna to write me, and tell her that if she will write to me I will write to her.  I am now writing upon that Aunt Brewton gave to me and you must tell her that I thank her very much, and give my love to all my relations.  I am writing in the Library and Aunt Susan has just come in and says that as I am writing she does not think she will as there is no use in both of us writing.  She says that I must tell you that we are getting on well considering there are so many together.  She says that Mrs. Caroline Reardon who was Miss Rinehart is coming to live in Greenville , and this is another reason that she is glad she has got out of the McBee family as Mrs. Reardon has such a tongue and temper.  And she says that Luther [McBee] contualy been sending notes and messages.  I must now stop writing.  You must excuse me for all the mistakes in this letter.  Frank has written to you but he would not let me read his letter.  Give my love to Anna.  You must bring me a pretty present.  Your affectionate son, William H, Perry</t>
+  </si>
+  <si>
+    <t>EMP293_09_05_1853</t>
+  </si>
+  <si>
+    <t> I have just returned from Aunt Brewtons, &amp; have only time to say, that if possible I prefer you coming down for me.  By next Wednesday I would like to leave here.  I think two weeks is as long as I ought to stay.  I do not intend going to Aunt Anna Turnbulls today.  If you cannot come, I will go up without you, but I have no time for more.  I received the money today. </t>
+  </si>
+  <si>
+    <t>EMP294_10_05_1853</t>
+  </si>
+  <si>
+    <t>I wrote you a few hurried lines last night on my return from Aunt Brewtons.  The 10 oclock bell was ringing, &amp; the servant was waiting to put the letter in the Office. I received two letters from you yesterday, one enclosing Willie’s letter, the other 40 dollars which I thank you for.  I think the expense of boarding is too great for me to stay here longer than two weeks, so next…day I ought to leave, or at least Tuesday, will make it two weeks.  If your cases will not be called for before then, suppose you come down now, &amp; when you return to Columbia, attend to your business, or cannot you beg the Court, in consideration of your wife’s waiting in town for you, to take up your cases at once, &amp; then come for me.  I will be very glad for you to come, but if it is entirely inconvenient, then I must get Wm Ed Hayne to carry me to the R[ail] Road, pay my passage, &amp; have my trunks marked, &amp; in Columbia you will be ready at the Depot, to receive me. Uncle Arthur will be very glad to see you.  Alston Hayne also expressed a wish to see you, &amp; all my relations I know would like to see you. so therefore there is not much to interest you here.  If you can with convenience come I would like it.  I am to dine at Uncle Arthur’s today. He is to send his carri[a]ge for me.  Last night at Aunt Brewton’s I saw Mr. Pinckney Alston who asked after you.  Mrs. Julius Pringle is still in this house.  Mrs. Richmond Lowndes is expected today.  Her husband &amp; family….  She was a Miss Parker.  The company is constantly changing.  It is very private, &amp; I feel quite at ease.  It is not so pleasant for you as the Charleston  Hotel.  You do not see so much company, &amp; it is not known that you are in town, so you had better go there first &amp; register your name. I told Aunt Anna Monday, I would let her know whether I would stay with her.  If she says nothing further on the subject, of course I wont think of going, &amp; I dare say she will not, for as she has given the invitation, she feels she has done her duty, &amp; I know it would give her trouble.  If she presses me as she did at first, &amp; you are not coming for a long time, I may go, but I will let you know. Aunt Eliza invited me to take tea with her last night &amp; Aunt Emily tonight, but I was engaged elsewhere.  I wish you would write every day.  I like to hear better, than when I am at home.  I long to see the children.  I suppose Hext has almost forgotten me.  I was pleased to see Willie’s letter.  I am glad Eliza’s children do not give way to grief, as it would distress me very much.  I am sure Missy feels it greatly.  Her loss is great to me.  I have not paid one cent for making my dresses for years, &amp; now I have to pay 3.25 for one.  Washing the least peice here is 6 ¼ a peice.  It will be a saving another time to bring Clara to sew &amp; wash for me.  My washing will amount to a good deal.  If you do not come, you must write me word whether I shall get Groceries, &amp; the Dinner Set.  I had to buy things to make me look genteel, &amp; those who have shopped with me, think I have at least 500 to spend, &amp; make me go beyond my means.  Hereafter I will shop alone.  Aunt Mary McCall said I must buy what would look well at the North , where they dress very fine.  I have not bought a great deal, but money in a City is soon spent, &amp; yet very little to show for it. Mrs. Wilkes &amp; Mrs. Perroneau called to see me yesterday, &amp; Miss Drayton &amp; her niece.  The servants are very careless, &amp; even cards left, they do not show me, so I do not know who has called. As I wish you to look your very best when you appear in Charleston among a people who once abused you, you must provide yourself with a dress Sack Coat suitable for the season.  I wish them to see that you are a striking looking man, &amp; as I am taken for a girl of sixteen, wish you to look of a suitable age for me.  If you can get a nice…Sack in Columbia get it there, if not here.   I will…write by return Mail, whether you will come or not, &amp; when.</t>
+  </si>
+  <si>
+    <t>EMP295_10_05_1853</t>
+  </si>
+  <si>
+    <t> I wrote you already today, &amp; will now write to send by tomorrows Mail.  I went up King st. this morning before breakfast, to shop a little.  It is the best time as from after breakfast until night, the streets are crowded.  Today I am to dine at Uncle Arthurs.  Aunt Anna Turnbull also sent to invite me, but as I was engaged to Uncle Arthur, I had to decline.  Tomorrow Aunt Mary McCall has invited me to dine at her house just opposite here, at 3 oclock.  It would take a month at least to see all my relations &amp; to return the visits paid me.  I have not seen Aunt Susan Hayne yet.  She lives very high up, &amp; keeps no equipage.  Anna is now quite well, only bit by muskutoes, which as yet though are not very bad.  You must write me, whether you can come for me or I must go up without you.  I have not much to write now, as I have written already to you today, &amp; I wish to write to Susan. Sunday afternoon.  Aunt Elizabeth carried me to St. Phillips to hear the new Bishop.  He was a Lawyer from North Carolina, 52 years old, seems in feeble health, not animated, but a very good plain preacher.  Mr. Arthur reaches Greenville tonight 8 oclock, left here yesterday afternoon, &amp; had a letter from Dr. Croft for you, which he was to have put in the Post Office at Columbia.  You must write me, whether you prefer my remaining here, or wish me to go to Columbia &amp; meet you there &amp; stay until your business is over, with you or go on to Greenville before you.  Either way I am willing to do, if it were not so expensive, I would be willing to stay here a longer time.  It is thought perfectly safe this month &amp; the next.  I pass my time pleasantly, but I will be glad to see the children particularly Hext; &amp; shopping takes so much money, that it is very unpleasant to go to shop, unless I had a good deal to spend, &amp; I buy the things perhaps I could do without, &amp; have to go without what I need.  It is dreadfully confusing, &amp; dreadfully fatiguing, &amp; I believe I would rather before I come again, write for what I wish, &amp; when I do come not enter King st., where there is so much to tempt.  Straw Mating, China, towels &amp;c I have not even looked at.  I would like very much to buy a new carri[a]ge, to put our new horses to.  If you come, you must price some.  I will now conclude &amp; write to Susan, &amp; before long I must dress &amp; go to Uncle Arthurs.</t>
+  </si>
+  <si>
+    <t>EMP296_11_05_1853</t>
+  </si>
+  <si>
+    <t> I dined at Uncle Arthurs yesterday in company with Mr. Pinckney Alston &amp; his daughter who we saw at Greenville.  He is so pleasant; he prevents a dinner party being stiff.  In the afternoon Aunt Elizabeth took us to ride round the Battery, which is a delightful place, very much extended &amp; improved.  That &amp; the Magnolia Cemetery are beautiful rides.  I have to dine at Aunt Mary McCall’s today, at 3 oclock.  She has just sent to repeat the invitation.  Tonight we are to take tea at Aunt Emily’s.  As I was out yesterday, I expect no one asked for letters at the Post Office for me, so I will send this morning.  After breakfast I am going to see Aunt Anna Turnbull, &amp; tomorrow I hope she will carry me to return some visits.  Augustus Hoke came to see us last night, just as I got home from Uncle Arthurs.  He looks &amp; seems quite well &amp; offered to escort us to the island, but I do not think we will have time to go.  Several persons called yesterday while I was out.  The weather today is very pleasant.  I have not found it hot yet.  There is generally a breeze.  Today is quite warm.  I am afraid Greenville even after the road is finished will not be patronized by the lower country.  They say it is too hot,…that when they leave Charleston, they wish for a greater change so go to Buncombe or the mountains of Georgia.   I have written you I believe every Mail, which is more than you have done me.  I must now prepare to go down to breakfast 12 oclock.  I have just received a letter from you, &amp; the boy says, there are two more, but he has to pay postage, so I sent him back with 10 cts.  I am glad you are passing your time pleasantly.  I dare say more pleasantly than you would in Charleston, for the gentlemen in Columbia are congregated together; here if you stay at this house, you would be with no gentlemen you know, &amp; may leave before your friends know you are here.  At the Charleston Hotel, you would find it pleasanter, but at this house I find it pleasant.  This morning I went to see Aunt Anna Turnbull, Aunt Haynes, &amp; Aunt Eliza.  Aunt Anna is expecting Mrs. Bull Friday, &amp; that day we are to dine with her, &amp; after Mrs. Bull leaves, she is to stay only a day or two, but I know she thinks so of trouble &amp; expense, that I do not think I will go, particularly as I do not wish to be obligated to anyone, &amp; for a few days stay, expect to ask them to stay with me a summer. If you prefer not coming down, you must write me, for I wish you to consult your pleasure, &amp; not come against your inclination.  I will today speak to Mrs. Davis &amp; ask her terms.  Aunt Mary said 18 a week, 12 for me &amp; 6 for Anna.  I hope if it is not more than that, I would rather be at a boarding house on account of the independent feeling that I have.  I have just received a letter from Susan &amp; Willie.  They are all well.  Anna is quite well now &amp; is to dine with me today at Aunt Mary McCall’s.  Tomorrow night we take tea at Aunt Haynes.  Perhaps tomorrow morning we go to the island. I would like very much to buy some Matting for our drawing room, &amp; the large chamber.  You can get it 25 cts a yd. 10 dollars for each room.  I wish you would be so good as to send me 20 dollars, if you are wil[l]ing for me to get it.  I also would like to get some Shades for our Drawing room, 3 of them.  I suppose 6 dollars would buy them &amp; I wish some towels &amp; a few large Table cloths.  If you are willing for me to get these things, send me the money, but if you would rather not, you need not.  The 40 dollars you sent me will pay two weeks board, so if you are not coming down, I am afraid to spend it, therefore have nothing now to make purchases with.  The Matting looks so cool &amp; sweet &amp; saves scouring. Mama wished me to get some money from Alston which will be due in a few days, to make some purchases for her.  I spoke to Aunt Brewton about it, but Alston has not sent me any.  If I could I would lend it to her, but I have it not.  My relations have been quite kind to me, &amp; it is a pleasant change to come to the City for a while.  All I regret is, I have not more money to spend.  Uncle Arthur told me he was surprised to find you were willing to accept a Judgeship, as he supposed you made a great deal more.  I told him you had never been a Candidate.  He says if you had removed to Charleston before this, Mr. King who has a great regard for you would have helped you greatly.  I wish you would move &amp; bring the paper here.  I have not seen a paper since I left home.  I wish you would send the Patriot.  I hear nothing of it.  I suppose Mr. Elford has not been to Columbia, as you do [not] mention him.  I think there is no risk in sending money.  If you think there is, you can direct your letters to the care of Wm Ed, but when I send my name written on paper, the letters are always brought me.  Write to me every day, that I may know your movements, &amp; buy a nice setting Sack Coat, either in Columbia or in Charleston if you come.  I will return whenever you write me. I am very glad you took a pleasant ride with Gov. Manning.  Persons here are more…of their horses than anything else, &amp; keep them for show, not for comfort.  I have walked more than I do a year in Greenville.  Dinner company seems not as common as it was.  Eloisa Martin asked me to stay with her, but has not asked me to dinner, but I suppose she will.</t>
+  </si>
+  <si>
+    <t>EMP297_12_05_1853</t>
+  </si>
+  <si>
+    <t>Thursday, 12 oclock</t>
+  </si>
+  <si>
+    <t>I have just received your letter in which you say we must go to Columbia Monday.  I hope you will be able to come down Saturday, &amp; stay here Sunday &amp; Monday, &amp; then we will all go back Tuesday,  My two weeks will then be up, but if it is impossible for you to come down, Tuesday I will go back.  Alston today is to send me some money at least bring it at 2 oclock, &amp; with that I will make Mamma’s purchases.  He will bring me more than 100, the interest due her in a few days.  I will spend out of it for myself what I need &amp; you can return it to her, so that will be better than you sending me any more money.  My dear husband you are very good in supplying your wife with money.  You know it is so pleasant for one to be able to buy things when they are in a City, &amp; see so many things they wish.  It makes me love you more &amp; more.  Mr. Leary is very much mistaken in saying it is unsafe to be here.  There is no danger until July.  I am up in the 4th story above all impure atmosphere .  The weather I have not found at all hot.  The muskutoes  are not very bad, persons laugh at the idea of there being any danger.  Many have not even come down from the country.  Uncle Arthur comes to see me almost every day, &amp; will be very glad to see you.  Alston said he would be very glad to see you, &amp; I would like very much for you to see my relations, so you must come Saturday &amp; stay a few days, &amp; beg them not to call your cases until you return.  I will not be able to go up before Tuesday.  My dress is at a Mantua maker &amp; I do not know how to get it from her.  I have to return visits &amp; shop.   I have not been able to shop for fear the money I had, I would have to pay board.  I asked Mrs. Davis today her terms.  She says 12 for me 6 for Anna a week.  This is a very pleasant house for a lady to be at.  Mr. Julius Pringle came yesterday, &amp; Mr. &amp; Mrs. Richard Lowndes.  I dined yesterday at Aunt Mary McCall’s &amp; drank tea at Aunt Emilys.  Tonight [I] am to take tea at Aunt Haynes &amp; tomorrow dine at Aunt Anna Turnbulls. Franks is a very good letter.  He does not need a gun.  You have one at home will do for him.  Write me by return Mail whether you can come.  You will get this letter Friday afternoon.  You had better come down Sunday; if you cannot leave Saturday, stay here Monday &amp; Tuesday &amp; go back Wednesday &amp; make arrangements for your cases to be called Thursday &amp; we return to Greenville Saturday.  I am glad you have bought clothes for yourself &amp; take great pride in seeing you look well.  I am taken for a Miss in King st. by the Store keepers.  I am thought to be sixteen, so I wish you to look as if you were 30, &amp; not be taken for my father any more. A change does great good.  I will enjoy my home &amp; have enjoyed myself here, &amp; long to see Hext.  If you would get business I would like you to live in Charleston, but you seem wedded to Greenville.  Susan’s troubles have made me dislike Greenville.  I would be glad to go to some other place.  I will price Clara here, &amp; look at groceries, but hope you will be here with me to purchase them.  I am very near Klin…s.  This morning Anna &amp; myself walked up to see Aunt Susan Hayne.  She invited us to dine Friday, but I am engaged to Aunt Anna Turnbull.  Uncle Arthur lives handsomely.  So does Aunt Mary McCall. &amp; Aunt Emily, &amp; all my relations live comfortably.  Aunt Anna Turnbull could live handsomely, but she is too economical.  Mrs. Bull comes down tomorrow[,] stays a day &amp; then goes to Columbia.  After that Aunt Anna says I must stay with her, but I will be gone. After dinner.  I have just sent to the office &amp; received no letter.  Perhaps the Cars have not come.  While at dinner I received an invitation from Miss Drayton to take tea there tomorrow to meet Mrs. Ford her sister.  She invited you also, if you were here.  I have accepted it.  Will dine at Aunt Anna’s &amp; take tea there this afternoon.  I am going to visit tomorrow.  I am going to shop before I dine out, so you see I have my hands full.  For S…day as yet I have no engagement, but dare say I will have.  Eloisa Martin invited me to stay with her, but has not invited me to tea or dinner.  Her health is bad perhaps is the reason.  Mrs. John Cunningham has been to see me but I was out.  I do not feel at all fatigued, never felt better, so you must not be uneasy.  Just suit yourself about coming down, perhaps by the beginning of next week you will get through your business &amp; can come I will now close &amp; write to Susan.  All I say is I would rather stay here than in Columbia, &amp; hope you can come for me.  Come down Sunday, stay a few days, &amp; return about Wednesday or Thursday.  You had better go to the Charleston Hotel as soon as you arrive, record your name, so your friends may know you are here &amp; then leave word you are coming to Mrs. D… M… home. </t>
+  </si>
+  <si>
+    <t>EMP298_14_05_1853</t>
+  </si>
+  <si>
+    <t> I have only time to say we are well, &amp; the weather today so cool that you need not be uneasy at thinking we will find it hot.  I did not hear from you yesterday, so do not know whether you are coming today or not.  I hope it will suit you to come down a little later.  Write me.  I have not got through my business yet.  This morning will do some of it, but cant get through all.  I paid visits yesterday, am engaged Monday to take tea with my old friend Maud Heyward.  Last night I took tea at Miss Draytons.  It was quite a party.  Tonight I take tea at Eloisa Martins.  I am not fatiguing myself.  Yesterday I got a letter from Susan.  They were well.  I have now to stop for breakfast.</t>
+  </si>
+  <si>
+    <t>EMP299_16_05_1853</t>
+  </si>
+  <si>
+    <t> I saw Uncle Arthur last night.  He says I must tell you, you must come for me.  That it will be very ungallant if you do not, &amp; he is very anxious to see you, so are all of our friends, &amp; as it will delay you only a few days longer.  After you have finished your business you must come for me.  If there is no danger you might take the night train.  I wish to go back only with you.  I don’t care to go with anyone else.  I will telegraph you today to know if you cannot after you have finished, come after you receive this letter as I will not have time to hear by the Mail.  Immediately telegraph me &amp; tell me you are coming, so I may not pack tonight.  You will get back in time for Dr. Croft, Saturday evening at…we can reach Greenville, or Sunday.  I dare say you can leave Columbia Wednesday.  Your affectionate wife, E.F.P. Uncle Arthur says he calls you a brave gentlemen has a very high opinion of you.</t>
+  </si>
+  <si>
+    <t>EMP300_00_05_1853</t>
+  </si>
+  <si>
+    <t> I received at dinner your letter by Mr. Vandiver.  I am too sorry I did not see you yourself.  I cannot consent that you should not come down.  Instead of my going up Tuesday, I wish you to come down here Tuesday, stay Wednesday, &amp; reach home Friday, &amp; that will be exactly the 3 weeks I expected to be away.  I am very anxious to see the children, but I am equally anxious that my relations may see my noble husband so you must come if only for the day.  You will get this letter Sunday.  Write by return Mail so I may hear Monday 2 oclock that you are coming for me.  My visit will end so much more delightfully, if you come down &amp; carry me up, &amp; you will be delayed only a little….  An old gentleman in this house Mr. Colbrun, is a good Union man, subscribes…your paper from the…Mr. Pettigru went to him, &amp; he would be so glad to see you, so will Uncle Arthur, Aunt Hayne &amp; all.  My friends have been very kind.  Mrs. Tom Lowndes sent to ask me to take tea tonight, but I was engaged to Eloisa..  Mrs. James Heyward asked me Monday.  Persons are just beginning to find out I am here, but I do not mind all this, except I want you to come, that my friends may see you.  If you cannot possibly come, I will go up Tuesday…is that I wish my friends to see you.  You are so near, &amp; you will be delayed only two days longer from Greenville, so write me by Mondays Mail that you will come, that you will have the pleasure of coming here, &amp; carrying me up which I prefer to Mr. Vandiver.  Your affectionate Wife, E.F.P.You will be only two days longer from home.</t>
+  </si>
+  <si>
+    <t>EMP301_00_05_1853</t>
+  </si>
+  <si>
+    <t>Sunday morning, 1/2 past 7 oclock</t>
+  </si>
+  <si>
+    <t>I took tea last night at Eloisa’s.  Mr. Martin says on Monday he will through the Telegraph learn from you whether you can come down Tuesday to escort me up to Columbia, or whether I must leave here Tuesday, to meet you in Columbia.  I hope you can come for me.  It will be only two days longer from home. We will get there Friday night instead of Wednesday night.  If possible you must come down, but if you say it is entirely impossible, I will of course go to you Tuesday, but my visit will end so much pleasanter if you come for me, that I feel convinced if you can, you will come.  I will keep this letter open until the Cars arrive; perhaps I may hear from you, though I think I heard the Post office was not open on Sunday.  At any rate I will send &amp; see. Anna &amp; myself are quite well.  Last night Mr. Lowndes invited us to tea.   Monday night Mr. James Heyward.  My friends have been very kind.  Mrs. Poinsett went up to Columbia Friday &amp; Mrs. Bull yesterday.  Mr. Martin says Mr. Bellinger &amp; W. DeSaussure gained the Felder Case, &amp; get a fee of 15000 between them.  Mama Susan &amp; Ann have given me such a long list of things to buy for them, that I am afraid Mama’s money &amp; mine together wont be enough to pay for what I have got, &amp; the China &amp; my board &amp; passage up, &amp; buy all Mamma wants.  If it is not, I will leave the China unpaid for.  I will pay for it as far as the money goes.  I have bought some Table cloths, Towels, Matting one peice, Servants clothes childrens clothes, Cloth for pillow cases, foot…&amp;c.  The China I suppose will be 50 dollars, &amp; my board about 40 &amp; the passage up so I believe, making 100 at once.  You promised me the interest of the Bank Stocks to provide for children servants &amp;c.  As I have spent your money in that way. You shall have the interest this time. Tomorrow as soon as I hear through the Telegraph whether you can come or not, I will arrange my plans.  I will be glad to correspond in so novel a way.  I am going to church this morning to St. Michaels with Aunt Anna Turnbull.  Before church Mr. Vandiver is to call, but I hope I am to go up with you instead of him. 9 oclock.  Mr. Vandiver has just been here, &amp; says he thinks on Tuesday you will be engaged in Court in Columbia &amp; cannot come down that day.  If this is so, let me know.  Address your communication to Mr. Martin, as I might not be at the Hotel when it is sent.  Mr. Martin will be sure to receive it &amp; bring it to me.  If you cannot come Tuesday &amp; prefer my going to Columbia that day, of course I will go, but I hope you will finish your business &amp; then come.  It will delay you only a few days longer.  You will have plenty of time to attend to Dr. Crofts business before Equity Court sits. </t>
+  </si>
+  <si>
+    <t>EMP302_00_05_1853</t>
+  </si>
+  <si>
+    <t>Thursday morning before breakfast</t>
+  </si>
+  <si>
+    <t> I write on the only paper I have to say that I dined at Aunt Anna Turnbull’s yesterday, &amp; she was very affectionate, &amp; said I might stay with her before I left, that she was expecting Mrs. Bull now, but when she left I must go, or at any rate, she must find room for me, so if you do not come as soon as you expected, I dare say I will stay with Aunt Anna next week.  I did her injustice, so wish to correct my error in saying, I liked her less than any other relations.  I took a long ride with her yesterday.  Today I am to dine with Aunt Eloisa.  I am quite comfortable, &amp; except the fatigue, I feel at [page torn] might from the walking up King st.  I am quite sure today I will buy paper.  The Biship is to be voted for today. When your business is all finished, come for me.  I am going now to breakfast.  I will get also some stamps today from Wm Ed. I hope you are well &amp; happy.  As I am so near you, you ought to feel happier than usual, when from home.  My next letter shall be longer.  Your affectionate wife, E.F.P. 2 oclock.  I have just received your letter enclosing Susans.  I am now going to Aunt Eliza’s, &amp; have just returned from shopping &amp; bought paper &amp; envelopes.</t>
+  </si>
+  <si>
+    <t>EMP303_00_05_1853</t>
+  </si>
+  <si>
+    <t>If you think your business will not come on for some time yet, &amp; that I will be detained in Columbia several days suppose you let me stay here a few days longer, as I prefer being here to Columbia, &amp; I will be very much hurried  to get through by Tuesday.  Cannot you come down Monday  stay Tuesday &amp; Wednesday &amp; go back Thursday.  Tell them not to call your cases until you return.  [I] would like to be here until the middle of next week, so as to be able to finish my business &amp; return my visits, but still I wish you to come for me.  It is perfectly safe here.  Everybody laughs at your thinking there is any danger.  Mr. Leary is very foolish.  I dare say you can ascertain by looking at the docket when your cases will be called, &amp; make your arrangements accordingly.   Today I dine at Aunt Turnbulls, tonight take tea at Miss Draytons, tomorrow at Mrs. Martins.  I have to return visits &amp; shop, &amp; would be glad if it suited you to come down the middle of next week.  I wish you to stay a few days.  I never felt better.  I wish your cases would be called the first of the week &amp; afterwards you come down.  If I am to stay either place, it had better be here, but I am not one to stay here longer than the middle of the week.  By that time I can get through but I wish you to come for me.  So now you know my wishes.  If possible you must make your movements correspond if possible. </t>
   </si>
 </sst>
 </file>
@@ -2481,11 +2895,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E196D05-2733-7A46-9004-C8C628B37F09}">
-  <dimension ref="A1:N241"/>
+  <dimension ref="A1:N296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M241" sqref="M241"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11840,6 +12254,2078 @@
         <v>685</v>
       </c>
     </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>686</v>
+      </c>
+      <c r="B242" t="s">
+        <v>9</v>
+      </c>
+      <c r="C242" t="s">
+        <v>10</v>
+      </c>
+      <c r="D242" t="s">
+        <v>22</v>
+      </c>
+      <c r="F242">
+        <v>1852</v>
+      </c>
+      <c r="G242">
+        <v>12</v>
+      </c>
+      <c r="H242">
+        <v>11</v>
+      </c>
+      <c r="I242" t="s">
+        <v>272</v>
+      </c>
+      <c r="J242" t="s">
+        <v>24</v>
+      </c>
+      <c r="M242" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>688</v>
+      </c>
+      <c r="B243" t="s">
+        <v>9</v>
+      </c>
+      <c r="C243" t="s">
+        <v>10</v>
+      </c>
+      <c r="F243">
+        <v>1852</v>
+      </c>
+      <c r="G243">
+        <v>12</v>
+      </c>
+      <c r="H243">
+        <v>11</v>
+      </c>
+      <c r="I243" t="s">
+        <v>689</v>
+      </c>
+      <c r="J243" t="s">
+        <v>690</v>
+      </c>
+      <c r="K243" t="s">
+        <v>95</v>
+      </c>
+      <c r="L243" t="s">
+        <v>57</v>
+      </c>
+      <c r="M243" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>692</v>
+      </c>
+      <c r="B244" t="s">
+        <v>9</v>
+      </c>
+      <c r="C244" t="s">
+        <v>10</v>
+      </c>
+      <c r="D244" t="s">
+        <v>22</v>
+      </c>
+      <c r="F244">
+        <v>1852</v>
+      </c>
+      <c r="G244">
+        <v>12</v>
+      </c>
+      <c r="H244">
+        <v>11</v>
+      </c>
+      <c r="I244" t="s">
+        <v>629</v>
+      </c>
+      <c r="J244" t="s">
+        <v>24</v>
+      </c>
+      <c r="K244" t="s">
+        <v>78</v>
+      </c>
+      <c r="L244" t="s">
+        <v>57</v>
+      </c>
+      <c r="M244" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>694</v>
+      </c>
+      <c r="B245" t="s">
+        <v>9</v>
+      </c>
+      <c r="C245" t="s">
+        <v>10</v>
+      </c>
+      <c r="D245" t="s">
+        <v>22</v>
+      </c>
+      <c r="E245" t="s">
+        <v>12</v>
+      </c>
+      <c r="F245">
+        <v>1852</v>
+      </c>
+      <c r="G245">
+        <v>12</v>
+      </c>
+      <c r="H245">
+        <v>12</v>
+      </c>
+      <c r="I245" t="s">
+        <v>552</v>
+      </c>
+      <c r="J245" t="s">
+        <v>24</v>
+      </c>
+      <c r="K245" t="s">
+        <v>289</v>
+      </c>
+      <c r="L245" t="s">
+        <v>57</v>
+      </c>
+      <c r="M245" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>696</v>
+      </c>
+      <c r="B246" t="s">
+        <v>9</v>
+      </c>
+      <c r="C246" t="s">
+        <v>621</v>
+      </c>
+      <c r="D246" t="s">
+        <v>22</v>
+      </c>
+      <c r="E246" t="s">
+        <v>11</v>
+      </c>
+      <c r="F246">
+        <v>1852</v>
+      </c>
+      <c r="G246">
+        <v>12</v>
+      </c>
+      <c r="H246">
+        <v>14</v>
+      </c>
+      <c r="I246" t="s">
+        <v>617</v>
+      </c>
+      <c r="J246" t="s">
+        <v>657</v>
+      </c>
+      <c r="L246" t="s">
+        <v>57</v>
+      </c>
+      <c r="M246" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>698</v>
+      </c>
+      <c r="B247" t="s">
+        <v>9</v>
+      </c>
+      <c r="C247" t="s">
+        <v>10</v>
+      </c>
+      <c r="E247" t="s">
+        <v>12</v>
+      </c>
+      <c r="F247">
+        <v>1852</v>
+      </c>
+      <c r="G247">
+        <v>12</v>
+      </c>
+      <c r="H247">
+        <v>14</v>
+      </c>
+      <c r="I247" t="s">
+        <v>699</v>
+      </c>
+      <c r="J247" t="s">
+        <v>24</v>
+      </c>
+      <c r="K247" t="s">
+        <v>95</v>
+      </c>
+      <c r="L247" t="s">
+        <v>57</v>
+      </c>
+      <c r="M247" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>701</v>
+      </c>
+      <c r="B248" t="s">
+        <v>9</v>
+      </c>
+      <c r="C248" t="s">
+        <v>10</v>
+      </c>
+      <c r="D248" t="s">
+        <v>22</v>
+      </c>
+      <c r="E248" t="s">
+        <v>12</v>
+      </c>
+      <c r="F248">
+        <v>1852</v>
+      </c>
+      <c r="G248">
+        <v>12</v>
+      </c>
+      <c r="H248">
+        <v>15</v>
+      </c>
+      <c r="I248" t="s">
+        <v>702</v>
+      </c>
+      <c r="J248" t="s">
+        <v>24</v>
+      </c>
+      <c r="K248" t="s">
+        <v>95</v>
+      </c>
+      <c r="L248" t="s">
+        <v>57</v>
+      </c>
+      <c r="M248" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>704</v>
+      </c>
+      <c r="B249" t="s">
+        <v>9</v>
+      </c>
+      <c r="C249" t="s">
+        <v>621</v>
+      </c>
+      <c r="D249" t="s">
+        <v>22</v>
+      </c>
+      <c r="E249" t="s">
+        <v>11</v>
+      </c>
+      <c r="F249">
+        <v>1852</v>
+      </c>
+      <c r="G249">
+        <v>12</v>
+      </c>
+      <c r="H249">
+        <v>16</v>
+      </c>
+      <c r="I249" t="s">
+        <v>705</v>
+      </c>
+      <c r="J249" t="s">
+        <v>657</v>
+      </c>
+      <c r="K249" t="s">
+        <v>658</v>
+      </c>
+      <c r="L249" t="s">
+        <v>57</v>
+      </c>
+      <c r="M249" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>707</v>
+      </c>
+      <c r="B250" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250" t="s">
+        <v>621</v>
+      </c>
+      <c r="D250" t="s">
+        <v>22</v>
+      </c>
+      <c r="E250" t="s">
+        <v>11</v>
+      </c>
+      <c r="F250">
+        <v>1852</v>
+      </c>
+      <c r="G250">
+        <v>12</v>
+      </c>
+      <c r="H250">
+        <v>17</v>
+      </c>
+      <c r="I250" t="s">
+        <v>708</v>
+      </c>
+      <c r="J250" t="s">
+        <v>657</v>
+      </c>
+      <c r="K250" t="s">
+        <v>447</v>
+      </c>
+      <c r="L250" t="s">
+        <v>57</v>
+      </c>
+      <c r="M250" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>710</v>
+      </c>
+      <c r="B251" t="s">
+        <v>9</v>
+      </c>
+      <c r="C251" t="s">
+        <v>621</v>
+      </c>
+      <c r="D251" t="s">
+        <v>22</v>
+      </c>
+      <c r="E251" t="s">
+        <v>11</v>
+      </c>
+      <c r="F251">
+        <v>1852</v>
+      </c>
+      <c r="G251">
+        <v>12</v>
+      </c>
+      <c r="H251">
+        <v>18</v>
+      </c>
+      <c r="I251" t="s">
+        <v>62</v>
+      </c>
+      <c r="J251" t="s">
+        <v>657</v>
+      </c>
+      <c r="L251" t="s">
+        <v>57</v>
+      </c>
+      <c r="M251" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>712</v>
+      </c>
+      <c r="B252" t="s">
+        <v>651</v>
+      </c>
+      <c r="C252" t="s">
+        <v>652</v>
+      </c>
+      <c r="D252" t="s">
+        <v>11</v>
+      </c>
+      <c r="E252" t="s">
+        <v>22</v>
+      </c>
+      <c r="F252">
+        <v>1852</v>
+      </c>
+      <c r="G252">
+        <v>12</v>
+      </c>
+      <c r="H252">
+        <v>21</v>
+      </c>
+      <c r="I252" t="s">
+        <v>713</v>
+      </c>
+      <c r="J252" t="s">
+        <v>653</v>
+      </c>
+      <c r="K252" t="s">
+        <v>714</v>
+      </c>
+      <c r="L252" t="s">
+        <v>651</v>
+      </c>
+      <c r="M252" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>716</v>
+      </c>
+      <c r="B253" t="s">
+        <v>9</v>
+      </c>
+      <c r="C253" t="s">
+        <v>621</v>
+      </c>
+      <c r="D253" t="s">
+        <v>22</v>
+      </c>
+      <c r="E253" t="s">
+        <v>11</v>
+      </c>
+      <c r="F253">
+        <v>1852</v>
+      </c>
+      <c r="G253">
+        <v>12</v>
+      </c>
+      <c r="H253">
+        <v>21</v>
+      </c>
+      <c r="J253" t="s">
+        <v>717</v>
+      </c>
+      <c r="K253" t="s">
+        <v>718</v>
+      </c>
+      <c r="L253" t="s">
+        <v>57</v>
+      </c>
+      <c r="M253" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>720</v>
+      </c>
+      <c r="B254" t="s">
+        <v>9</v>
+      </c>
+      <c r="C254" t="s">
+        <v>621</v>
+      </c>
+      <c r="D254" t="s">
+        <v>22</v>
+      </c>
+      <c r="E254" t="s">
+        <v>11</v>
+      </c>
+      <c r="F254">
+        <v>1852</v>
+      </c>
+      <c r="G254">
+        <v>12</v>
+      </c>
+      <c r="H254">
+        <v>24</v>
+      </c>
+      <c r="I254" t="s">
+        <v>23</v>
+      </c>
+      <c r="J254" t="s">
+        <v>657</v>
+      </c>
+      <c r="K254" t="s">
+        <v>721</v>
+      </c>
+      <c r="M254" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>723</v>
+      </c>
+      <c r="B255" t="s">
+        <v>9</v>
+      </c>
+      <c r="C255" t="s">
+        <v>621</v>
+      </c>
+      <c r="D255" t="s">
+        <v>22</v>
+      </c>
+      <c r="E255" t="s">
+        <v>11</v>
+      </c>
+      <c r="F255">
+        <v>1852</v>
+      </c>
+      <c r="G255">
+        <v>12</v>
+      </c>
+      <c r="H255">
+        <v>25</v>
+      </c>
+      <c r="I255" t="s">
+        <v>724</v>
+      </c>
+      <c r="J255" t="s">
+        <v>657</v>
+      </c>
+      <c r="K255" t="s">
+        <v>447</v>
+      </c>
+      <c r="L255" t="s">
+        <v>57</v>
+      </c>
+      <c r="M255" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>726</v>
+      </c>
+      <c r="B256" t="s">
+        <v>9</v>
+      </c>
+      <c r="C256" t="s">
+        <v>621</v>
+      </c>
+      <c r="D256" t="s">
+        <v>22</v>
+      </c>
+      <c r="E256" t="s">
+        <v>11</v>
+      </c>
+      <c r="F256">
+        <v>1852</v>
+      </c>
+      <c r="G256">
+        <v>12</v>
+      </c>
+      <c r="H256">
+        <v>28</v>
+      </c>
+      <c r="I256" t="s">
+        <v>727</v>
+      </c>
+      <c r="J256" t="s">
+        <v>657</v>
+      </c>
+      <c r="K256" t="s">
+        <v>447</v>
+      </c>
+      <c r="L256" t="s">
+        <v>57</v>
+      </c>
+      <c r="M256" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>729</v>
+      </c>
+      <c r="B257" t="s">
+        <v>9</v>
+      </c>
+      <c r="C257" t="s">
+        <v>621</v>
+      </c>
+      <c r="D257" t="s">
+        <v>22</v>
+      </c>
+      <c r="E257" t="s">
+        <v>11</v>
+      </c>
+      <c r="F257">
+        <v>1852</v>
+      </c>
+      <c r="G257">
+        <v>12</v>
+      </c>
+      <c r="H257">
+        <v>29</v>
+      </c>
+      <c r="J257" t="s">
+        <v>657</v>
+      </c>
+      <c r="K257" t="s">
+        <v>447</v>
+      </c>
+      <c r="L257" t="s">
+        <v>57</v>
+      </c>
+      <c r="M257" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>732</v>
+      </c>
+      <c r="B258" t="s">
+        <v>9</v>
+      </c>
+      <c r="C258" t="s">
+        <v>621</v>
+      </c>
+      <c r="D258" t="s">
+        <v>22</v>
+      </c>
+      <c r="E258" t="s">
+        <v>11</v>
+      </c>
+      <c r="F258">
+        <v>1852</v>
+      </c>
+      <c r="G258">
+        <v>12</v>
+      </c>
+      <c r="H258">
+        <v>31</v>
+      </c>
+      <c r="I258" t="s">
+        <v>684</v>
+      </c>
+      <c r="J258" t="s">
+        <v>657</v>
+      </c>
+      <c r="K258" t="s">
+        <v>447</v>
+      </c>
+      <c r="L258" t="s">
+        <v>57</v>
+      </c>
+      <c r="M258" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>733</v>
+      </c>
+      <c r="B259" t="s">
+        <v>9</v>
+      </c>
+      <c r="C259" t="s">
+        <v>621</v>
+      </c>
+      <c r="D259" t="s">
+        <v>22</v>
+      </c>
+      <c r="E259" t="s">
+        <v>11</v>
+      </c>
+      <c r="F259">
+        <v>1852</v>
+      </c>
+      <c r="G259">
+        <v>12</v>
+      </c>
+      <c r="J259" t="s">
+        <v>657</v>
+      </c>
+      <c r="K259" t="s">
+        <v>658</v>
+      </c>
+      <c r="L259" t="s">
+        <v>57</v>
+      </c>
+      <c r="M259" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>735</v>
+      </c>
+      <c r="B260" t="s">
+        <v>9</v>
+      </c>
+      <c r="C260" t="s">
+        <v>621</v>
+      </c>
+      <c r="E260" t="s">
+        <v>11</v>
+      </c>
+      <c r="F260">
+        <v>1852</v>
+      </c>
+      <c r="G260">
+        <v>12</v>
+      </c>
+      <c r="M260" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>737</v>
+      </c>
+      <c r="B261" t="s">
+        <v>9</v>
+      </c>
+      <c r="C261" t="s">
+        <v>10</v>
+      </c>
+      <c r="F261">
+        <v>1852</v>
+      </c>
+      <c r="J261" t="s">
+        <v>24</v>
+      </c>
+      <c r="K261" t="s">
+        <v>55</v>
+      </c>
+      <c r="L261" t="s">
+        <v>57</v>
+      </c>
+      <c r="M261" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>739</v>
+      </c>
+      <c r="B262" t="s">
+        <v>9</v>
+      </c>
+      <c r="C262" t="s">
+        <v>10</v>
+      </c>
+      <c r="F262">
+        <v>1852</v>
+      </c>
+      <c r="I262" t="s">
+        <v>74</v>
+      </c>
+      <c r="J262" t="s">
+        <v>24</v>
+      </c>
+      <c r="K262" t="s">
+        <v>740</v>
+      </c>
+      <c r="L262" t="s">
+        <v>57</v>
+      </c>
+      <c r="M262" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>742</v>
+      </c>
+      <c r="B263" t="s">
+        <v>9</v>
+      </c>
+      <c r="C263" t="s">
+        <v>10</v>
+      </c>
+      <c r="E263" t="s">
+        <v>376</v>
+      </c>
+      <c r="F263">
+        <v>1852</v>
+      </c>
+      <c r="I263" t="s">
+        <v>743</v>
+      </c>
+      <c r="J263" t="s">
+        <v>24</v>
+      </c>
+      <c r="K263" t="s">
+        <v>744</v>
+      </c>
+      <c r="L263" t="s">
+        <v>57</v>
+      </c>
+      <c r="M263" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>746</v>
+      </c>
+      <c r="B264" t="s">
+        <v>9</v>
+      </c>
+      <c r="C264" t="s">
+        <v>10</v>
+      </c>
+      <c r="E264" t="s">
+        <v>53</v>
+      </c>
+      <c r="F264">
+        <v>1852</v>
+      </c>
+      <c r="I264" t="s">
+        <v>263</v>
+      </c>
+      <c r="J264" t="s">
+        <v>24</v>
+      </c>
+      <c r="K264" t="s">
+        <v>553</v>
+      </c>
+      <c r="L264" t="s">
+        <v>57</v>
+      </c>
+      <c r="M264" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>748</v>
+      </c>
+      <c r="B265" t="s">
+        <v>9</v>
+      </c>
+      <c r="C265" t="s">
+        <v>621</v>
+      </c>
+      <c r="E265" t="s">
+        <v>12</v>
+      </c>
+      <c r="F265">
+        <v>1852</v>
+      </c>
+      <c r="J265" t="s">
+        <v>717</v>
+      </c>
+      <c r="K265" t="s">
+        <v>447</v>
+      </c>
+      <c r="L265" t="s">
+        <v>57</v>
+      </c>
+      <c r="M265" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>750</v>
+      </c>
+      <c r="B266" t="s">
+        <v>9</v>
+      </c>
+      <c r="C266" t="s">
+        <v>621</v>
+      </c>
+      <c r="D266" t="s">
+        <v>22</v>
+      </c>
+      <c r="E266" t="s">
+        <v>11</v>
+      </c>
+      <c r="F266">
+        <v>1853</v>
+      </c>
+      <c r="G266">
+        <v>1</v>
+      </c>
+      <c r="H266">
+        <v>1</v>
+      </c>
+      <c r="I266" t="s">
+        <v>62</v>
+      </c>
+      <c r="J266" t="s">
+        <v>657</v>
+      </c>
+      <c r="K266" t="s">
+        <v>447</v>
+      </c>
+      <c r="L266" t="s">
+        <v>57</v>
+      </c>
+      <c r="M266" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>752</v>
+      </c>
+      <c r="B267" t="s">
+        <v>9</v>
+      </c>
+      <c r="C267" t="s">
+        <v>621</v>
+      </c>
+      <c r="D267" t="s">
+        <v>22</v>
+      </c>
+      <c r="E267" t="s">
+        <v>11</v>
+      </c>
+      <c r="F267">
+        <v>1853</v>
+      </c>
+      <c r="G267">
+        <v>1</v>
+      </c>
+      <c r="H267">
+        <v>3</v>
+      </c>
+      <c r="I267" t="s">
+        <v>110</v>
+      </c>
+      <c r="J267" t="s">
+        <v>657</v>
+      </c>
+      <c r="K267" t="s">
+        <v>447</v>
+      </c>
+      <c r="L267" t="s">
+        <v>57</v>
+      </c>
+      <c r="M267" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>754</v>
+      </c>
+      <c r="B268" t="s">
+        <v>9</v>
+      </c>
+      <c r="C268" t="s">
+        <v>621</v>
+      </c>
+      <c r="D268" t="s">
+        <v>22</v>
+      </c>
+      <c r="E268" t="s">
+        <v>11</v>
+      </c>
+      <c r="F268">
+        <v>1853</v>
+      </c>
+      <c r="G268">
+        <v>1</v>
+      </c>
+      <c r="H268">
+        <v>5</v>
+      </c>
+      <c r="I268" t="s">
+        <v>755</v>
+      </c>
+      <c r="J268" t="s">
+        <v>657</v>
+      </c>
+      <c r="K268" t="s">
+        <v>447</v>
+      </c>
+      <c r="L268" t="s">
+        <v>57</v>
+      </c>
+      <c r="M268" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>757</v>
+      </c>
+      <c r="B269" t="s">
+        <v>9</v>
+      </c>
+      <c r="C269" t="s">
+        <v>621</v>
+      </c>
+      <c r="D269" t="s">
+        <v>22</v>
+      </c>
+      <c r="E269" t="s">
+        <v>11</v>
+      </c>
+      <c r="F269">
+        <v>1853</v>
+      </c>
+      <c r="G269">
+        <v>1</v>
+      </c>
+      <c r="H269">
+        <v>6</v>
+      </c>
+      <c r="I269" t="s">
+        <v>644</v>
+      </c>
+      <c r="J269" t="s">
+        <v>657</v>
+      </c>
+      <c r="K269" t="s">
+        <v>447</v>
+      </c>
+      <c r="L269" t="s">
+        <v>58</v>
+      </c>
+      <c r="M269" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>759</v>
+      </c>
+      <c r="B270" t="s">
+        <v>9</v>
+      </c>
+      <c r="C270" t="s">
+        <v>621</v>
+      </c>
+      <c r="D270" t="s">
+        <v>22</v>
+      </c>
+      <c r="E270" t="s">
+        <v>11</v>
+      </c>
+      <c r="F270">
+        <v>1853</v>
+      </c>
+      <c r="G270">
+        <v>1</v>
+      </c>
+      <c r="H270">
+        <v>7</v>
+      </c>
+      <c r="I270" t="s">
+        <v>559</v>
+      </c>
+      <c r="J270" t="s">
+        <v>657</v>
+      </c>
+      <c r="K270" t="s">
+        <v>447</v>
+      </c>
+      <c r="L270" t="s">
+        <v>58</v>
+      </c>
+      <c r="M270" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>761</v>
+      </c>
+      <c r="B271" t="s">
+        <v>9</v>
+      </c>
+      <c r="C271" t="s">
+        <v>621</v>
+      </c>
+      <c r="D271" t="s">
+        <v>22</v>
+      </c>
+      <c r="E271" t="s">
+        <v>11</v>
+      </c>
+      <c r="F271">
+        <v>1853</v>
+      </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
+      <c r="H271">
+        <v>8</v>
+      </c>
+      <c r="I271" t="s">
+        <v>272</v>
+      </c>
+      <c r="J271" t="s">
+        <v>657</v>
+      </c>
+      <c r="K271" t="s">
+        <v>447</v>
+      </c>
+      <c r="L271" t="s">
+        <v>58</v>
+      </c>
+      <c r="M271" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>763</v>
+      </c>
+      <c r="B272" t="s">
+        <v>9</v>
+      </c>
+      <c r="C272" t="s">
+        <v>621</v>
+      </c>
+      <c r="D272" t="s">
+        <v>22</v>
+      </c>
+      <c r="E272" t="s">
+        <v>11</v>
+      </c>
+      <c r="F272">
+        <v>1853</v>
+      </c>
+      <c r="G272">
+        <v>1</v>
+      </c>
+      <c r="H272">
+        <v>10</v>
+      </c>
+      <c r="I272" t="s">
+        <v>110</v>
+      </c>
+      <c r="J272" t="s">
+        <v>657</v>
+      </c>
+      <c r="K272" t="s">
+        <v>447</v>
+      </c>
+      <c r="L272" t="s">
+        <v>58</v>
+      </c>
+      <c r="M272" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>765</v>
+      </c>
+      <c r="B273" t="s">
+        <v>9</v>
+      </c>
+      <c r="C273" t="s">
+        <v>621</v>
+      </c>
+      <c r="D273" t="s">
+        <v>22</v>
+      </c>
+      <c r="E273" t="s">
+        <v>11</v>
+      </c>
+      <c r="F273">
+        <v>1853</v>
+      </c>
+      <c r="G273">
+        <v>1</v>
+      </c>
+      <c r="H273">
+        <v>11</v>
+      </c>
+      <c r="I273" t="s">
+        <v>285</v>
+      </c>
+      <c r="J273" t="s">
+        <v>657</v>
+      </c>
+      <c r="K273" t="s">
+        <v>447</v>
+      </c>
+      <c r="L273" t="s">
+        <v>58</v>
+      </c>
+      <c r="M273" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>767</v>
+      </c>
+      <c r="B274" t="s">
+        <v>9</v>
+      </c>
+      <c r="C274" t="s">
+        <v>621</v>
+      </c>
+      <c r="D274" t="s">
+        <v>22</v>
+      </c>
+      <c r="F274">
+        <v>1853</v>
+      </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
+      <c r="H274">
+        <v>11</v>
+      </c>
+      <c r="I274" t="s">
+        <v>768</v>
+      </c>
+      <c r="J274" t="s">
+        <v>657</v>
+      </c>
+      <c r="K274" t="s">
+        <v>447</v>
+      </c>
+      <c r="L274" t="s">
+        <v>58</v>
+      </c>
+      <c r="M274" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>770</v>
+      </c>
+      <c r="B275" t="s">
+        <v>9</v>
+      </c>
+      <c r="C275" t="s">
+        <v>621</v>
+      </c>
+      <c r="F275">
+        <v>1853</v>
+      </c>
+      <c r="G275">
+        <v>1</v>
+      </c>
+      <c r="M275" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>772</v>
+      </c>
+      <c r="B276" t="s">
+        <v>9</v>
+      </c>
+      <c r="C276" t="s">
+        <v>621</v>
+      </c>
+      <c r="E276" t="s">
+        <v>11</v>
+      </c>
+      <c r="F276">
+        <v>1853</v>
+      </c>
+      <c r="J276" t="s">
+        <v>657</v>
+      </c>
+      <c r="K276" t="s">
+        <v>198</v>
+      </c>
+      <c r="L276" t="s">
+        <v>57</v>
+      </c>
+      <c r="M276" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>774</v>
+      </c>
+      <c r="B277" t="s">
+        <v>9</v>
+      </c>
+      <c r="C277" t="s">
+        <v>621</v>
+      </c>
+      <c r="D277" t="s">
+        <v>22</v>
+      </c>
+      <c r="E277" t="s">
+        <v>11</v>
+      </c>
+      <c r="F277">
+        <v>1853</v>
+      </c>
+      <c r="G277">
+        <v>1</v>
+      </c>
+      <c r="H277">
+        <v>13</v>
+      </c>
+      <c r="I277" t="s">
+        <v>40</v>
+      </c>
+      <c r="J277" t="s">
+        <v>657</v>
+      </c>
+      <c r="K277" t="s">
+        <v>447</v>
+      </c>
+      <c r="L277" t="s">
+        <v>57</v>
+      </c>
+      <c r="M277" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>776</v>
+      </c>
+      <c r="B278" t="s">
+        <v>9</v>
+      </c>
+      <c r="C278" t="s">
+        <v>621</v>
+      </c>
+      <c r="D278" t="s">
+        <v>22</v>
+      </c>
+      <c r="E278" t="s">
+        <v>11</v>
+      </c>
+      <c r="F278">
+        <v>1853</v>
+      </c>
+      <c r="G278">
+        <v>1</v>
+      </c>
+      <c r="H278">
+        <v>1</v>
+      </c>
+      <c r="J278" t="s">
+        <v>657</v>
+      </c>
+      <c r="K278" t="s">
+        <v>447</v>
+      </c>
+      <c r="L278" t="s">
+        <v>57</v>
+      </c>
+      <c r="M278" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>778</v>
+      </c>
+      <c r="B279" t="s">
+        <v>9</v>
+      </c>
+      <c r="C279" t="s">
+        <v>10</v>
+      </c>
+      <c r="D279" t="s">
+        <v>11</v>
+      </c>
+      <c r="E279" t="s">
+        <v>12</v>
+      </c>
+      <c r="F279">
+        <v>1853</v>
+      </c>
+      <c r="G279">
+        <v>5</v>
+      </c>
+      <c r="H279">
+        <v>2</v>
+      </c>
+      <c r="I279" t="s">
+        <v>779</v>
+      </c>
+      <c r="J279" t="s">
+        <v>24</v>
+      </c>
+      <c r="K279" t="s">
+        <v>95</v>
+      </c>
+      <c r="L279" t="s">
+        <v>57</v>
+      </c>
+      <c r="M279" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>781</v>
+      </c>
+      <c r="B280" t="s">
+        <v>9</v>
+      </c>
+      <c r="C280" t="s">
+        <v>10</v>
+      </c>
+      <c r="D280" t="s">
+        <v>11</v>
+      </c>
+      <c r="E280" t="s">
+        <v>12</v>
+      </c>
+      <c r="F280">
+        <v>1853</v>
+      </c>
+      <c r="G280">
+        <v>5</v>
+      </c>
+      <c r="H280">
+        <v>4</v>
+      </c>
+      <c r="I280" t="s">
+        <v>782</v>
+      </c>
+      <c r="J280" t="s">
+        <v>24</v>
+      </c>
+      <c r="K280" t="s">
+        <v>48</v>
+      </c>
+      <c r="L280" t="s">
+        <v>57</v>
+      </c>
+      <c r="M280" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>784</v>
+      </c>
+      <c r="B281" t="s">
+        <v>9</v>
+      </c>
+      <c r="C281" t="s">
+        <v>10</v>
+      </c>
+      <c r="D281" t="s">
+        <v>11</v>
+      </c>
+      <c r="E281" t="s">
+        <v>12</v>
+      </c>
+      <c r="F281">
+        <v>1853</v>
+      </c>
+      <c r="G281">
+        <v>5</v>
+      </c>
+      <c r="H281">
+        <v>6</v>
+      </c>
+      <c r="I281" t="s">
+        <v>785</v>
+      </c>
+      <c r="J281" t="s">
+        <v>24</v>
+      </c>
+      <c r="K281" t="s">
+        <v>48</v>
+      </c>
+      <c r="L281" t="s">
+        <v>57</v>
+      </c>
+      <c r="M281" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>787</v>
+      </c>
+      <c r="B282" t="s">
+        <v>9</v>
+      </c>
+      <c r="C282" t="s">
+        <v>10</v>
+      </c>
+      <c r="D282" t="s">
+        <v>11</v>
+      </c>
+      <c r="E282" t="s">
+        <v>12</v>
+      </c>
+      <c r="F282">
+        <v>1853</v>
+      </c>
+      <c r="G282">
+        <v>5</v>
+      </c>
+      <c r="H282">
+        <v>6</v>
+      </c>
+      <c r="I282" t="s">
+        <v>403</v>
+      </c>
+      <c r="J282" t="s">
+        <v>24</v>
+      </c>
+      <c r="K282" t="s">
+        <v>95</v>
+      </c>
+      <c r="L282" t="s">
+        <v>57</v>
+      </c>
+      <c r="M282" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>789</v>
+      </c>
+      <c r="B283" t="s">
+        <v>9</v>
+      </c>
+      <c r="C283" t="s">
+        <v>10</v>
+      </c>
+      <c r="D283" t="s">
+        <v>11</v>
+      </c>
+      <c r="E283" t="s">
+        <v>12</v>
+      </c>
+      <c r="F283">
+        <v>1853</v>
+      </c>
+      <c r="G283">
+        <v>5</v>
+      </c>
+      <c r="H283">
+        <v>7</v>
+      </c>
+      <c r="I283" t="s">
+        <v>790</v>
+      </c>
+      <c r="J283" t="s">
+        <v>24</v>
+      </c>
+      <c r="K283" t="s">
+        <v>48</v>
+      </c>
+      <c r="L283" t="s">
+        <v>57</v>
+      </c>
+      <c r="M283" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>792</v>
+      </c>
+      <c r="B284" t="s">
+        <v>9</v>
+      </c>
+      <c r="C284" t="s">
+        <v>10</v>
+      </c>
+      <c r="D284" t="s">
+        <v>11</v>
+      </c>
+      <c r="E284" t="s">
+        <v>12</v>
+      </c>
+      <c r="F284">
+        <v>1853</v>
+      </c>
+      <c r="G284">
+        <v>5</v>
+      </c>
+      <c r="H284">
+        <v>8</v>
+      </c>
+      <c r="I284" t="s">
+        <v>546</v>
+      </c>
+      <c r="J284" t="s">
+        <v>24</v>
+      </c>
+      <c r="K284" t="s">
+        <v>48</v>
+      </c>
+      <c r="L284" t="s">
+        <v>57</v>
+      </c>
+      <c r="M284" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>794</v>
+      </c>
+      <c r="B285" t="s">
+        <v>795</v>
+      </c>
+      <c r="C285" t="s">
+        <v>652</v>
+      </c>
+      <c r="E285" t="s">
+        <v>11</v>
+      </c>
+      <c r="F285">
+        <v>1853</v>
+      </c>
+      <c r="G285">
+        <v>5</v>
+      </c>
+      <c r="H285">
+        <v>8</v>
+      </c>
+      <c r="I285" t="s">
+        <v>488</v>
+      </c>
+      <c r="J285" t="s">
+        <v>796</v>
+      </c>
+      <c r="K285" t="s">
+        <v>797</v>
+      </c>
+      <c r="L285" t="s">
+        <v>795</v>
+      </c>
+      <c r="M285" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>799</v>
+      </c>
+      <c r="B286" t="s">
+        <v>9</v>
+      </c>
+      <c r="C286" t="s">
+        <v>10</v>
+      </c>
+      <c r="D286" t="s">
+        <v>11</v>
+      </c>
+      <c r="E286" t="s">
+        <v>12</v>
+      </c>
+      <c r="F286">
+        <v>1853</v>
+      </c>
+      <c r="G286">
+        <v>5</v>
+      </c>
+      <c r="H286">
+        <v>9</v>
+      </c>
+      <c r="I286" t="s">
+        <v>135</v>
+      </c>
+      <c r="J286" t="s">
+        <v>24</v>
+      </c>
+      <c r="K286" t="s">
+        <v>48</v>
+      </c>
+      <c r="L286" t="s">
+        <v>57</v>
+      </c>
+      <c r="M286" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>801</v>
+      </c>
+      <c r="B287" t="s">
+        <v>9</v>
+      </c>
+      <c r="C287" t="s">
+        <v>10</v>
+      </c>
+      <c r="D287" t="s">
+        <v>11</v>
+      </c>
+      <c r="E287" t="s">
+        <v>12</v>
+      </c>
+      <c r="F287">
+        <v>1853</v>
+      </c>
+      <c r="G287">
+        <v>5</v>
+      </c>
+      <c r="H287">
+        <v>10</v>
+      </c>
+      <c r="J287" t="s">
+        <v>24</v>
+      </c>
+      <c r="K287" t="s">
+        <v>95</v>
+      </c>
+      <c r="L287" t="s">
+        <v>57</v>
+      </c>
+      <c r="M287" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>803</v>
+      </c>
+      <c r="B288" t="s">
+        <v>9</v>
+      </c>
+      <c r="C288" t="s">
+        <v>10</v>
+      </c>
+      <c r="D288" t="s">
+        <v>11</v>
+      </c>
+      <c r="E288" t="s">
+        <v>12</v>
+      </c>
+      <c r="F288">
+        <v>1853</v>
+      </c>
+      <c r="G288">
+        <v>5</v>
+      </c>
+      <c r="H288">
+        <v>10</v>
+      </c>
+      <c r="J288" t="s">
+        <v>24</v>
+      </c>
+      <c r="K288" t="s">
+        <v>48</v>
+      </c>
+      <c r="L288" t="s">
+        <v>57</v>
+      </c>
+      <c r="M288" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>805</v>
+      </c>
+      <c r="B289" t="s">
+        <v>9</v>
+      </c>
+      <c r="C289" t="s">
+        <v>10</v>
+      </c>
+      <c r="D289" t="s">
+        <v>11</v>
+      </c>
+      <c r="E289" t="s">
+        <v>12</v>
+      </c>
+      <c r="F289">
+        <v>1853</v>
+      </c>
+      <c r="G289">
+        <v>5</v>
+      </c>
+      <c r="H289">
+        <v>11</v>
+      </c>
+      <c r="J289" t="s">
+        <v>24</v>
+      </c>
+      <c r="K289" t="s">
+        <v>95</v>
+      </c>
+      <c r="L289" t="s">
+        <v>57</v>
+      </c>
+      <c r="M289" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>807</v>
+      </c>
+      <c r="B290" t="s">
+        <v>9</v>
+      </c>
+      <c r="C290" t="s">
+        <v>10</v>
+      </c>
+      <c r="D290" t="s">
+        <v>11</v>
+      </c>
+      <c r="E290" t="s">
+        <v>12</v>
+      </c>
+      <c r="F290">
+        <v>1853</v>
+      </c>
+      <c r="G290">
+        <v>5</v>
+      </c>
+      <c r="H290">
+        <v>12</v>
+      </c>
+      <c r="I290" t="s">
+        <v>808</v>
+      </c>
+      <c r="J290" t="s">
+        <v>24</v>
+      </c>
+      <c r="K290" t="s">
+        <v>48</v>
+      </c>
+      <c r="L290" t="s">
+        <v>57</v>
+      </c>
+      <c r="M290" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>810</v>
+      </c>
+      <c r="B291" t="s">
+        <v>9</v>
+      </c>
+      <c r="C291" t="s">
+        <v>10</v>
+      </c>
+      <c r="D291" t="s">
+        <v>11</v>
+      </c>
+      <c r="F291">
+        <v>1853</v>
+      </c>
+      <c r="G291">
+        <v>5</v>
+      </c>
+      <c r="H291">
+        <v>14</v>
+      </c>
+      <c r="I291" t="s">
+        <v>62</v>
+      </c>
+      <c r="J291" t="s">
+        <v>24</v>
+      </c>
+      <c r="K291" t="s">
+        <v>48</v>
+      </c>
+      <c r="L291" t="s">
+        <v>57</v>
+      </c>
+      <c r="M291" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>812</v>
+      </c>
+      <c r="B292" t="s">
+        <v>9</v>
+      </c>
+      <c r="C292" t="s">
+        <v>10</v>
+      </c>
+      <c r="D292" t="s">
+        <v>11</v>
+      </c>
+      <c r="E292" t="s">
+        <v>12</v>
+      </c>
+      <c r="F292">
+        <v>1853</v>
+      </c>
+      <c r="G292">
+        <v>5</v>
+      </c>
+      <c r="H292">
+        <v>16</v>
+      </c>
+      <c r="I292" t="s">
+        <v>110</v>
+      </c>
+      <c r="J292" t="s">
+        <v>24</v>
+      </c>
+      <c r="K292" t="s">
+        <v>48</v>
+      </c>
+      <c r="L292" t="s">
+        <v>57</v>
+      </c>
+      <c r="M292" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>814</v>
+      </c>
+      <c r="B293" t="s">
+        <v>9</v>
+      </c>
+      <c r="C293" t="s">
+        <v>10</v>
+      </c>
+      <c r="D293" t="s">
+        <v>11</v>
+      </c>
+      <c r="E293" t="s">
+        <v>12</v>
+      </c>
+      <c r="F293">
+        <v>1853</v>
+      </c>
+      <c r="G293">
+        <v>5</v>
+      </c>
+      <c r="I293" t="s">
+        <v>724</v>
+      </c>
+      <c r="J293" t="s">
+        <v>24</v>
+      </c>
+      <c r="K293" t="s">
+        <v>95</v>
+      </c>
+      <c r="L293" t="s">
+        <v>57</v>
+      </c>
+      <c r="M293" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>816</v>
+      </c>
+      <c r="B294" t="s">
+        <v>9</v>
+      </c>
+      <c r="C294" t="s">
+        <v>10</v>
+      </c>
+      <c r="D294" t="s">
+        <v>11</v>
+      </c>
+      <c r="E294" t="s">
+        <v>12</v>
+      </c>
+      <c r="F294">
+        <v>1853</v>
+      </c>
+      <c r="G294">
+        <v>5</v>
+      </c>
+      <c r="I294" t="s">
+        <v>817</v>
+      </c>
+      <c r="J294" t="s">
+        <v>24</v>
+      </c>
+      <c r="K294" t="s">
+        <v>48</v>
+      </c>
+      <c r="L294" t="s">
+        <v>57</v>
+      </c>
+      <c r="M294" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>819</v>
+      </c>
+      <c r="B295" t="s">
+        <v>9</v>
+      </c>
+      <c r="C295" t="s">
+        <v>10</v>
+      </c>
+      <c r="D295" t="s">
+        <v>11</v>
+      </c>
+      <c r="E295" t="s">
+        <v>12</v>
+      </c>
+      <c r="F295">
+        <v>1853</v>
+      </c>
+      <c r="G295">
+        <v>5</v>
+      </c>
+      <c r="I295" t="s">
+        <v>820</v>
+      </c>
+      <c r="J295" t="s">
+        <v>24</v>
+      </c>
+      <c r="K295" t="s">
+        <v>48</v>
+      </c>
+      <c r="L295" t="s">
+        <v>57</v>
+      </c>
+      <c r="M295" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>822</v>
+      </c>
+      <c r="B296" t="s">
+        <v>9</v>
+      </c>
+      <c r="C296" t="s">
+        <v>10</v>
+      </c>
+      <c r="D296" t="s">
+        <v>11</v>
+      </c>
+      <c r="E296" t="s">
+        <v>12</v>
+      </c>
+      <c r="F296">
+        <v>1853</v>
+      </c>
+      <c r="G296">
+        <v>5</v>
+      </c>
+      <c r="I296" t="s">
+        <v>23</v>
+      </c>
+      <c r="J296" t="s">
+        <v>24</v>
+      </c>
+      <c r="K296" t="s">
+        <v>48</v>
+      </c>
+      <c r="L296" t="s">
+        <v>57</v>
+      </c>
+      <c r="M296" t="s">
+        <v>823</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>